<commit_message>
added 270 packet run
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4A59DA-118B-436F-BF71-47D1A7B1EF86}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F14929F-0351-414D-8E39-169A699618CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
   <si>
     <t>Acc</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>270 Packets</t>
+  </si>
+  <si>
+    <t>250 Packets</t>
   </si>
 </sst>
 </file>
@@ -879,15 +882,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -897,8 +900,11 @@
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,8 +932,17 @@
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.166885614395099</v>
       </c>
@@ -946,8 +961,17 @@
       <c r="G3">
         <v>84.701129913330007</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>89.674389362335205</v>
+      </c>
+      <c r="J3">
+        <v>0.244528188925136</v>
+      </c>
+      <c r="K3">
+        <v>82.455614089965806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>88.785070180892902</v>
       </c>
@@ -966,8 +990,17 @@
       <c r="G4">
         <v>78.1411936283111</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>89.342379570007296</v>
+      </c>
+      <c r="J4">
+        <v>0.25267978321172402</v>
+      </c>
+      <c r="K4">
+        <v>75.036825656890798</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>89.546328783035193</v>
       </c>
@@ -986,8 +1019,17 @@
       <c r="G5">
         <v>77.345816135406494</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>88.751870393752995</v>
+      </c>
+      <c r="J5">
+        <v>0.25918662667721099</v>
+      </c>
+      <c r="K5">
+        <v>75.991146802902193</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90.113121271133394</v>
       </c>
@@ -1006,8 +1048,17 @@
       <c r="G6">
         <v>77.874296903610201</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>89.909172058105398</v>
+      </c>
+      <c r="J6">
+        <v>0.25369177561717199</v>
+      </c>
+      <c r="K6">
+        <v>76.640452146530095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>89.394551515579195</v>
       </c>
@@ -1026,8 +1077,17 @@
       <c r="G7">
         <v>77.542165040969806</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>89.185857772827106</v>
+      </c>
+      <c r="J7">
+        <v>0.24768675051806699</v>
+      </c>
+      <c r="K7">
+        <v>76.136749982833805</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>88.839614391326904</v>
       </c>
@@ -1046,8 +1106,17 @@
       <c r="G8">
         <v>78.732240915298405</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>88.241988420486393</v>
+      </c>
+      <c r="J8">
+        <v>0.26343331673686798</v>
+      </c>
+      <c r="K8">
+        <v>75.151413202285696</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.389806985855103</v>
       </c>
@@ -1066,8 +1135,17 @@
       <c r="G9">
         <v>78.457118749618502</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>88.903647661209106</v>
+      </c>
+      <c r="J9">
+        <v>0.25511473001401602</v>
+      </c>
+      <c r="K9">
+        <v>74.383100032806396</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.460951089858995</v>
       </c>
@@ -1086,8 +1164,17 @@
       <c r="G10">
         <v>77.395019054412799</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>88.804042339324894</v>
+      </c>
+      <c r="J10">
+        <v>0.25308474167839601</v>
+      </c>
+      <c r="K10">
+        <v>74.369613409042302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.043563604354802</v>
       </c>
@@ -1106,8 +1193,17 @@
       <c r="G11">
         <v>77.431273937225299</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>88.585859537124605</v>
+      </c>
+      <c r="J11">
+        <v>0.25379235884448298</v>
+      </c>
+      <c r="K11">
+        <v>74.491253614425602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>89.247518777847205</v>
       </c>
@@ -1126,8 +1222,17 @@
       <c r="G12">
         <v>76.575281381606999</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>89.795339107513399</v>
+      </c>
+      <c r="J12">
+        <v>0.23951616773269299</v>
+      </c>
+      <c r="K12">
+        <v>75.908175230026202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>89.961344003677297</v>
       </c>
@@ -1146,8 +1251,17 @@
       <c r="G13">
         <v>77.414097309112506</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>89.937627315521198</v>
+      </c>
+      <c r="J13">
+        <v>0.24038724478290899</v>
+      </c>
+      <c r="K13">
+        <v>75.984380960464406</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>89.385062456130896</v>
       </c>
@@ -1166,8 +1280,17 @@
       <c r="G14">
         <v>76.740263700485201</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>88.585859537124605</v>
+      </c>
+      <c r="J14">
+        <v>0.25078049290404097</v>
+      </c>
+      <c r="K14">
+        <v>75.073441743850694</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.280718564987097</v>
       </c>
@@ -1186,8 +1309,17 @@
       <c r="G15">
         <v>76.593142747879</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>90.295726060867295</v>
+      </c>
+      <c r="J15">
+        <v>0.23855006397332301</v>
+      </c>
+      <c r="K15">
+        <v>75.772522926330495</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>89.197713136672903</v>
       </c>
@@ -1206,8 +1338,17 @@
       <c r="G16">
         <v>77.570351839065495</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>89.254629611968994</v>
+      </c>
+      <c r="J16">
+        <v>0.261448279177599</v>
+      </c>
+      <c r="K16">
+        <v>75.891891717910696</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.546328783035193</v>
       </c>
@@ -1226,8 +1367,17 @@
       <c r="G17">
         <v>77.369984149932804</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>88.747125864028902</v>
+      </c>
+      <c r="J17">
+        <v>0.25448242167212898</v>
+      </c>
+      <c r="K17">
+        <v>74.464914083480807</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.657789468765202</v>
       </c>
@@ -1246,8 +1396,17 @@
       <c r="G18">
         <v>76.568186759948702</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>89.418268203735295</v>
+      </c>
+      <c r="J18">
+        <v>0.24392899600639401</v>
+      </c>
+      <c r="K18">
+        <v>74.943201541900606</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>89.0909969806671</v>
       </c>
@@ -1266,8 +1425,17 @@
       <c r="G19">
         <v>78.089726209640503</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>89.304435253143296</v>
+      </c>
+      <c r="J19">
+        <v>0.24944798000179599</v>
+      </c>
+      <c r="K19">
+        <v>76.312826156616197</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>89.420634508132906</v>
       </c>
@@ -1286,8 +1454,17 @@
       <c r="G20">
         <v>77.533040285110403</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>89.444351196289006</v>
+      </c>
+      <c r="J20">
+        <v>0.24763306652123901</v>
+      </c>
+      <c r="K20">
+        <v>76.144528627395601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90.049088001251206</v>
       </c>
@@ -1306,8 +1483,17 @@
       <c r="G21">
         <v>76.407927513122502</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>88.832497596740694</v>
+      </c>
+      <c r="J21">
+        <v>0.25881855143789601</v>
+      </c>
+      <c r="K21">
+        <v>75.318665742874103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>89.548701047897296</v>
       </c>
@@ -1326,8 +1512,17 @@
       <c r="G22">
         <v>76.4855859279632</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>89.577156305313096</v>
+      </c>
+      <c r="J22">
+        <v>0.242277082595513</v>
+      </c>
+      <c r="K22">
+        <v>75.418741703033405</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>89.072024822235093</v>
       </c>
@@ -1346,8 +1541,17 @@
       <c r="G23">
         <v>76.903504371642995</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>88.9131307601928</v>
+      </c>
+      <c r="J23">
+        <v>0.25252829890109002</v>
+      </c>
+      <c r="K23">
+        <v>75.688076972961397</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.920247554778996</v>
       </c>
@@ -1366,8 +1570,17 @@
       <c r="G24">
         <v>76.386791467666598</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>89.311546087265</v>
+      </c>
+      <c r="J24">
+        <v>0.25169569942632403</v>
+      </c>
+      <c r="K24">
+        <v>76.163012027740393</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88.8989031314849</v>
       </c>
@@ -1386,8 +1599,17 @@
       <c r="G25">
         <v>76.663475751876803</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>88.972419500350895</v>
+      </c>
+      <c r="J25">
+        <v>0.25440847281804102</v>
+      </c>
+      <c r="K25">
+        <v>75.628634691238403</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90.087032318115206</v>
       </c>
@@ -1406,8 +1628,17 @@
       <c r="G26">
         <v>76.341283798217702</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>88.889414072036701</v>
+      </c>
+      <c r="J26">
+        <v>0.25551032082455299</v>
+      </c>
+      <c r="K26">
+        <v>75.975719213485704</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.9273583889007</v>
       </c>
@@ -1426,8 +1657,17 @@
       <c r="G27">
         <v>77.214232921600299</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>89.192968606948796</v>
+      </c>
+      <c r="J27">
+        <v>0.25626749786626601</v>
+      </c>
+      <c r="K27">
+        <v>76.8635346889495</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.425379037856999</v>
       </c>
@@ -1446,8 +1686,17 @@
       <c r="G28">
         <v>76.506627082824707</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>88.972419500350895</v>
+      </c>
+      <c r="J28">
+        <v>0.25850718530676298</v>
+      </c>
+      <c r="K28">
+        <v>76.635301589965806</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.382690191268907</v>
       </c>
@@ -1466,8 +1715,17 @@
       <c r="G29">
         <v>77.495549201965304</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>89.294946193694997</v>
+      </c>
+      <c r="J29">
+        <v>0.25150514153655101</v>
+      </c>
+      <c r="K29">
+        <v>75.884287595748901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>89.188230037689195</v>
       </c>
@@ -1486,8 +1744,17 @@
       <c r="G30">
         <v>76.9297127723693</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>89.1716241836547</v>
+      </c>
+      <c r="J30">
+        <v>0.25054168452265502</v>
+      </c>
+      <c r="K30">
+        <v>74.442911386489797</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>89.064908027648897</v>
       </c>
@@ -1506,8 +1773,17 @@
       <c r="G31">
         <v>76.664077281951904</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>88.863331079483004</v>
+      </c>
+      <c r="J31">
+        <v>0.27117592397217899</v>
+      </c>
+      <c r="K31">
+        <v>75.919968605041504</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.559776544570894</v>
       </c>
@@ -1526,8 +1802,17 @@
       <c r="G32">
         <v>78.127259016036902</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>89.577156305313096</v>
+      </c>
+      <c r="J32">
+        <v>0.244464064881007</v>
+      </c>
+      <c r="K32">
+        <v>76.845924854278493</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.588231801986694</v>
       </c>
@@ -1546,8 +1831,17 @@
       <c r="G33">
         <v>76.402573823928805</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>89.197713136672903</v>
+      </c>
+      <c r="J33">
+        <v>0.26747144625227998</v>
+      </c>
+      <c r="K33">
+        <v>76.167885541915894</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -1566,8 +1860,17 @@
       <c r="G34">
         <v>76.664586544036794</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>88.732898235321002</v>
+      </c>
+      <c r="J34">
+        <v>0.264799719276476</v>
+      </c>
+      <c r="K34">
+        <v>76.130175828933702</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.955819606781006</v>
       </c>
@@ -1586,8 +1889,17 @@
       <c r="G35">
         <v>76.837721586227403</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>88.699692487716604</v>
+      </c>
+      <c r="J35">
+        <v>0.258527421027829</v>
+      </c>
+      <c r="K35">
+        <v>76.171753644943195</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>89.2973184585571</v>
       </c>
@@ -1606,8 +1918,17 @@
       <c r="G36">
         <v>77.528557300567599</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>89.534467458724905</v>
+      </c>
+      <c r="J36">
+        <v>0.25453679464543799</v>
+      </c>
+      <c r="K36">
+        <v>76.952017784118596</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.391393423080402</v>
       </c>
@@ -1626,8 +1947,17 @@
       <c r="G37">
         <v>76.864413976669297</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>89.257001876830998</v>
+      </c>
+      <c r="J37">
+        <v>0.24804810150953499</v>
+      </c>
+      <c r="K37">
+        <v>76.221291780471802</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>89.380323886871295</v>
       </c>
@@ -1646,8 +1976,17 @@
       <c r="G38">
         <v>76.483597040176306</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>89.577156305313096</v>
+      </c>
+      <c r="J38">
+        <v>0.25602399755423799</v>
+      </c>
+      <c r="K38">
+        <v>75.4796013832092</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.7858500480651</v>
       </c>
@@ -1666,8 +2005,17 @@
       <c r="G39">
         <v>76.901098251342702</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>89.005619287490802</v>
+      </c>
+      <c r="J39">
+        <v>0.258948004286644</v>
+      </c>
+      <c r="K39">
+        <v>75.752249002456594</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>88.863331079483004</v>
       </c>
@@ -1686,8 +2034,17 @@
       <c r="G40">
         <v>77.099527597427297</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>89.226174354553194</v>
+      </c>
+      <c r="J40">
+        <v>0.25585194801063998</v>
+      </c>
+      <c r="K40">
+        <v>76.804516315460205</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>89.311546087265</v>
       </c>
@@ -1706,8 +2063,17 @@
       <c r="G41">
         <v>77.154038429260197</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>89.3637180328369</v>
+      </c>
+      <c r="J41">
+        <v>0.23998273261691599</v>
+      </c>
+      <c r="K41">
+        <v>76.135252714157104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>89.413523674011202</v>
       </c>
@@ -1726,8 +2092,17 @@
       <c r="G42">
         <v>77.3783762454986</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>89.570045471191406</v>
+      </c>
+      <c r="J42">
+        <v>0.244280452884269</v>
+      </c>
+      <c r="K42">
+        <v>76.395229101181002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89.311546087265</v>
       </c>
@@ -1746,8 +2121,17 @@
       <c r="G43">
         <v>75.699454069137502</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>88.929730653762803</v>
+      </c>
+      <c r="J43">
+        <v>0.25502020090282601</v>
+      </c>
+      <c r="K43">
+        <v>75.890778541564899</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.290201663970905</v>
       </c>
@@ -1766,8 +2150,17 @@
       <c r="G44">
         <v>77.577924013137803</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>89.067280292510901</v>
+      </c>
+      <c r="J44">
+        <v>0.25527764901182698</v>
+      </c>
+      <c r="K44">
+        <v>75.688072443008394</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90.013515949249197</v>
       </c>
@@ -1786,8 +2179,17 @@
       <c r="G45">
         <v>76.912440299987793</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>88.955819606781006</v>
+      </c>
+      <c r="J45">
+        <v>0.25693635091425499</v>
+      </c>
+      <c r="K45">
+        <v>76.632386922836304</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90.068060159683199</v>
       </c>
@@ -1806,8 +2208,17 @@
       <c r="G46">
         <v>76.762998104095402</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>89.669644832610999</v>
+      </c>
+      <c r="J46">
+        <v>0.242593294158473</v>
+      </c>
+      <c r="K46">
+        <v>75.193731069564805</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>89.351862668991004</v>
       </c>
@@ -1826,8 +2237,17 @@
       <c r="G47">
         <v>76.690966844558702</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>89.396923780441199</v>
+      </c>
+      <c r="J47">
+        <v>0.24983933237144601</v>
+      </c>
+      <c r="K47">
+        <v>76.821705341339097</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>89.238029718399005</v>
       </c>
@@ -1846,8 +2266,17 @@
       <c r="G48">
         <v>77.556117057800293</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>88.8846755027771</v>
+      </c>
+      <c r="J48">
+        <v>0.25353088884362601</v>
+      </c>
+      <c r="K48">
+        <v>76.058594942092896</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.445943593978797</v>
       </c>
@@ -1866,8 +2295,17 @@
       <c r="G49">
         <v>78.085031032562199</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>88.955819606781006</v>
+      </c>
+      <c r="J49">
+        <v>0.25039767996927298</v>
+      </c>
+      <c r="K49">
+        <v>76.064940690994206</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>89.337635040283203</v>
       </c>
@@ -1886,8 +2324,17 @@
       <c r="G50">
         <v>76.572036981582599</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>89.396923780441199</v>
+      </c>
+      <c r="J50">
+        <v>0.25604076211240601</v>
+      </c>
+      <c r="K50">
+        <v>75.976545572280799</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>89.157396554946899</v>
       </c>
@@ -1905,6 +2352,15 @@
       </c>
       <c r="G51">
         <v>77.243500709533606</v>
+      </c>
+      <c r="I51">
+        <v>89.439606666564899</v>
+      </c>
+      <c r="J51">
+        <v>0.25780443963407501</v>
+      </c>
+      <c r="K51">
+        <v>75.536620140075598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 250 packet run
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F14929F-0351-414D-8E39-169A699618CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3D36C2-9544-4808-812A-C27E6D32D491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN 1D" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
   <si>
     <t>Acc</t>
   </si>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>250 Packets</t>
+  </si>
+  <si>
+    <t>230 Packets</t>
   </si>
 </sst>
 </file>
@@ -882,15 +885,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="R10" sqref="R10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -903,8 +906,11 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -941,8 +947,17 @@
       <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.166885614395099</v>
       </c>
@@ -970,8 +985,17 @@
       <c r="K3">
         <v>82.455614089965806</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>89.178740978240896</v>
+      </c>
+      <c r="N3">
+        <v>0.252545211645541</v>
+      </c>
+      <c r="O3">
+        <v>57.434668302535997</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>88.785070180892902</v>
       </c>
@@ -999,8 +1023,17 @@
       <c r="K4">
         <v>75.036825656890798</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>89.069652557373004</v>
+      </c>
+      <c r="N4">
+        <v>0.252583463879403</v>
+      </c>
+      <c r="O4">
+        <v>50.736342430114703</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>89.546328783035193</v>
       </c>
@@ -1028,8 +1061,17 @@
       <c r="K5">
         <v>75.991146802902193</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>89.366090297698904</v>
+      </c>
+      <c r="N5">
+        <v>0.25359862651281401</v>
+      </c>
+      <c r="O5">
+        <v>52.417280435562098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90.113121271133394</v>
       </c>
@@ -1057,8 +1099,17 @@
       <c r="K6">
         <v>76.640452146530095</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>89.311546087265</v>
+      </c>
+      <c r="N6">
+        <v>0.25728204508864599</v>
+      </c>
+      <c r="O6">
+        <v>70.234991788864093</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>89.394551515579195</v>
       </c>
@@ -1086,8 +1137,17 @@
       <c r="K7">
         <v>76.136749982833805</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>88.614320755004798</v>
+      </c>
+      <c r="N7">
+        <v>0.25985459607330103</v>
+      </c>
+      <c r="O7">
+        <v>72.422914505004798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>88.839614391326904</v>
       </c>
@@ -1115,8 +1175,17 @@
       <c r="K8">
         <v>75.151413202285696</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>89.252257347106905</v>
+      </c>
+      <c r="N8">
+        <v>0.25010520547531501</v>
+      </c>
+      <c r="O8">
+        <v>73.780971765518103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.389806985855103</v>
       </c>
@@ -1144,8 +1213,17 @@
       <c r="K9">
         <v>74.383100032806396</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>89.444351196289006</v>
+      </c>
+      <c r="N9">
+        <v>0.25206261013849601</v>
+      </c>
+      <c r="O9">
+        <v>73.470363855361896</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.460951089858995</v>
       </c>
@@ -1173,8 +1251,17 @@
       <c r="K10">
         <v>74.369613409042302</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>89.176368713378906</v>
+      </c>
+      <c r="N10">
+        <v>0.25984460084723598</v>
+      </c>
+      <c r="O10">
+        <v>73.888139009475694</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.043563604354802</v>
       </c>
@@ -1202,8 +1289,17 @@
       <c r="K11">
         <v>74.491253614425602</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>88.713926076888995</v>
+      </c>
+      <c r="N11">
+        <v>0.26225827017307601</v>
+      </c>
+      <c r="O11">
+        <v>73.667391538619995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>89.247518777847205</v>
       </c>
@@ -1231,8 +1327,17 @@
       <c r="K12">
         <v>75.908175230026202</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>89.207202196121202</v>
+      </c>
+      <c r="N12">
+        <v>0.26163952592211198</v>
+      </c>
+      <c r="O12">
+        <v>73.167571067810002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>89.961344003677297</v>
       </c>
@@ -1260,8 +1365,17 @@
       <c r="K13">
         <v>75.984380960464406</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>88.547915220260606</v>
+      </c>
+      <c r="N13">
+        <v>0.25785235024443198</v>
+      </c>
+      <c r="O13">
+        <v>73.064140081405597</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>89.385062456130896</v>
       </c>
@@ -1289,8 +1403,17 @@
       <c r="K14">
         <v>75.073441743850694</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>89.095735549926701</v>
+      </c>
+      <c r="N14">
+        <v>0.25773916314572298</v>
+      </c>
+      <c r="O14">
+        <v>73.371634960174504</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.280718564987097</v>
       </c>
@@ -1318,8 +1441,17 @@
       <c r="K15">
         <v>75.772522926330495</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>88.837242126464801</v>
+      </c>
+      <c r="N15">
+        <v>0.25607624672087997</v>
+      </c>
+      <c r="O15">
+        <v>73.299146175384493</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>89.197713136672903</v>
       </c>
@@ -1347,8 +1479,17 @@
       <c r="K16">
         <v>75.891891717910696</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>88.339221477508502</v>
+      </c>
+      <c r="N16">
+        <v>0.25407364842019797</v>
+      </c>
+      <c r="O16">
+        <v>72.054840087890597</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.546328783035193</v>
       </c>
@@ -1376,8 +1517,17 @@
       <c r="K17">
         <v>74.464914083480807</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>89.240401983261094</v>
+      </c>
+      <c r="N17">
+        <v>0.25561310755237299</v>
+      </c>
+      <c r="O17">
+        <v>66.818587303161607</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.657789468765202</v>
       </c>
@@ -1405,8 +1555,17 @@
       <c r="K18">
         <v>74.943201541900606</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>88.431710004806504</v>
+      </c>
+      <c r="N18">
+        <v>0.25459275126052899</v>
+      </c>
+      <c r="O18">
+        <v>65.315620660781804</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>89.0909969806671</v>
       </c>
@@ -1434,8 +1593,17 @@
       <c r="K19">
         <v>76.312826156616197</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>89.484667778015094</v>
+      </c>
+      <c r="N19">
+        <v>0.24229520157583401</v>
+      </c>
+      <c r="O19">
+        <v>65.325640916824298</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>89.420634508132906</v>
       </c>
@@ -1463,8 +1631,17 @@
       <c r="K20">
         <v>76.144528627395601</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>89.107596874237004</v>
+      </c>
+      <c r="N20">
+        <v>0.25341787500523899</v>
+      </c>
+      <c r="O20">
+        <v>64.942824602127004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90.049088001251206</v>
       </c>
@@ -1492,8 +1669,17 @@
       <c r="K21">
         <v>75.318665742874103</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>89.638817310333195</v>
+      </c>
+      <c r="N21">
+        <v>0.24233236525013399</v>
+      </c>
+      <c r="O21">
+        <v>71.640696287155095</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>89.548701047897296</v>
       </c>
@@ -1521,8 +1707,17 @@
       <c r="K22">
         <v>75.418741703033405</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>88.730525970458899</v>
+      </c>
+      <c r="N22">
+        <v>0.25192946128653698</v>
+      </c>
+      <c r="O22">
+        <v>72.8096537590026</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>89.072024822235093</v>
       </c>
@@ -1550,8 +1745,17 @@
       <c r="K23">
         <v>75.688076972961397</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>88.604831695556598</v>
+      </c>
+      <c r="N23">
+        <v>0.26436049926094901</v>
+      </c>
+      <c r="O23">
+        <v>73.1050026416778</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.920247554778996</v>
       </c>
@@ -1579,8 +1783,17 @@
       <c r="K24">
         <v>76.163012027740393</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>89.747905731201101</v>
+      </c>
+      <c r="N24">
+        <v>0.24085296937197001</v>
+      </c>
+      <c r="O24">
+        <v>72.422594308853107</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88.8989031314849</v>
       </c>
@@ -1608,8 +1821,17 @@
       <c r="K25">
         <v>75.628634691238403</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>89.524984359741197</v>
+      </c>
+      <c r="N25">
+        <v>0.24993859493842199</v>
+      </c>
+      <c r="O25">
+        <v>73.375932931899996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90.087032318115206</v>
       </c>
@@ -1637,8 +1859,17 @@
       <c r="K26">
         <v>75.975719213485704</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>88.728153705596895</v>
+      </c>
+      <c r="N26">
+        <v>0.26853464283145401</v>
+      </c>
+      <c r="O26">
+        <v>72.435604810714693</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.9273583889007</v>
       </c>
@@ -1666,8 +1897,17 @@
       <c r="K27">
         <v>76.8635346889495</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>89.373207092285099</v>
+      </c>
+      <c r="N27">
+        <v>0.245401347847126</v>
+      </c>
+      <c r="O27">
+        <v>71.9085404872894</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.425379037856999</v>
       </c>
@@ -1695,8 +1935,17 @@
       <c r="K28">
         <v>76.635301589965806</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>88.6546373367309</v>
+      </c>
+      <c r="N28">
+        <v>0.25298739580282997</v>
+      </c>
+      <c r="O28">
+        <v>72.832605600356999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.382690191268907</v>
       </c>
@@ -1724,8 +1973,17 @@
       <c r="K29">
         <v>75.884287595748901</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>88.889414072036701</v>
+      </c>
+      <c r="N29">
+        <v>0.24597882526853401</v>
+      </c>
+      <c r="O29">
+        <v>73.371208667755099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>89.188230037689195</v>
       </c>
@@ -1753,8 +2011,17 @@
       <c r="K30">
         <v>74.442911386489797</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>89.766877889633093</v>
+      </c>
+      <c r="N30">
+        <v>0.25262072788501999</v>
+      </c>
+      <c r="O30">
+        <v>73.339866638183594</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>89.064908027648897</v>
       </c>
@@ -1782,8 +2049,17 @@
       <c r="K31">
         <v>75.919968605041504</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>90.167665481567298</v>
+      </c>
+      <c r="N31">
+        <v>0.24315573055814199</v>
+      </c>
+      <c r="O31">
+        <v>72.988338470458899</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.559776544570894</v>
       </c>
@@ -1811,8 +2087,17 @@
       <c r="K32">
         <v>76.845924854278493</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>89.147913455963106</v>
+      </c>
+      <c r="N32">
+        <v>0.260568303093277</v>
+      </c>
+      <c r="O32">
+        <v>73.194815874099703</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.588231801986694</v>
       </c>
@@ -1840,8 +2125,17 @@
       <c r="K33">
         <v>76.167885541915894</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>88.498115539550696</v>
+      </c>
+      <c r="N33">
+        <v>0.26244507051402999</v>
+      </c>
+      <c r="O33">
+        <v>72.461916446685706</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -1869,8 +2163,17 @@
       <c r="K34">
         <v>76.130175828933702</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>88.906013965606604</v>
+      </c>
+      <c r="N34">
+        <v>0.25796546142202897</v>
+      </c>
+      <c r="O34">
+        <v>72.133360624313298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.955819606781006</v>
       </c>
@@ -1898,8 +2201,17 @@
       <c r="K35">
         <v>76.171753644943195</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>89.249885082244802</v>
+      </c>
+      <c r="N35">
+        <v>0.246497458720698</v>
+      </c>
+      <c r="O35">
+        <v>72.210428237914996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>89.2973184585571</v>
       </c>
@@ -1927,8 +2239,17 @@
       <c r="K36">
         <v>76.952017784118596</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>89.226174354553194</v>
+      </c>
+      <c r="N36">
+        <v>0.24958485578640799</v>
+      </c>
+      <c r="O36">
+        <v>73.164016008377004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.391393423080402</v>
       </c>
@@ -1956,8 +2277,17 @@
       <c r="K37">
         <v>76.221291780471802</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>89.373207092285099</v>
+      </c>
+      <c r="N37">
+        <v>0.249828237407385</v>
+      </c>
+      <c r="O37">
+        <v>72.7936882972717</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>89.380323886871295</v>
       </c>
@@ -1985,8 +2315,17 @@
       <c r="K38">
         <v>75.4796013832092</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>88.939219713211003</v>
+      </c>
+      <c r="N38">
+        <v>0.25471635787702301</v>
+      </c>
+      <c r="O38">
+        <v>72.7490456104278</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.7858500480651</v>
       </c>
@@ -2014,8 +2353,17 @@
       <c r="K39">
         <v>75.752249002456594</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>88.974791765212998</v>
+      </c>
+      <c r="N39">
+        <v>0.25970559938143001</v>
+      </c>
+      <c r="O39">
+        <v>72.168561935424805</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>88.863331079483004</v>
       </c>
@@ -2043,8 +2391,17 @@
       <c r="K40">
         <v>76.804516315460205</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>89.337635040283203</v>
+      </c>
+      <c r="N40">
+        <v>0.250110044411053</v>
+      </c>
+      <c r="O40">
+        <v>73.477121829986501</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>89.311546087265</v>
       </c>
@@ -2072,8 +2429,17 @@
       <c r="K41">
         <v>76.135252714157104</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>89.370834827423096</v>
+      </c>
+      <c r="N41">
+        <v>0.25412208723213903</v>
+      </c>
+      <c r="O41">
+        <v>74.128241539001394</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>89.413523674011202</v>
       </c>
@@ -2101,8 +2467,17 @@
       <c r="K42">
         <v>76.395229101181002</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>88.896530866622896</v>
+      </c>
+      <c r="N42">
+        <v>0.258900934794837</v>
+      </c>
+      <c r="O42">
+        <v>71.630872964858995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89.311546087265</v>
       </c>
@@ -2130,8 +2505,17 @@
       <c r="K43">
         <v>75.890778541564899</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>89.041191339492798</v>
+      </c>
+      <c r="N43">
+        <v>0.25723445218750002</v>
+      </c>
+      <c r="O43">
+        <v>73.095628261566105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.290201663970905</v>
       </c>
@@ -2159,8 +2543,17 @@
       <c r="K44">
         <v>75.688072443008394</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>88.085472583770695</v>
+      </c>
+      <c r="N44">
+        <v>0.26046220264874897</v>
+      </c>
+      <c r="O44">
+        <v>73.030666589736896</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90.013515949249197</v>
       </c>
@@ -2188,8 +2581,17 @@
       <c r="K45">
         <v>76.632386922836304</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>88.929730653762803</v>
+      </c>
+      <c r="N45">
+        <v>0.25560344505453297</v>
+      </c>
+      <c r="O45">
+        <v>73.410993814468299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90.068060159683199</v>
       </c>
@@ -2217,8 +2619,17 @@
       <c r="K46">
         <v>75.193731069564805</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>89.057791233062702</v>
+      </c>
+      <c r="N46">
+        <v>0.25533980482943403</v>
+      </c>
+      <c r="O46">
+        <v>72.2200510501861</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>89.351862668991004</v>
       </c>
@@ -2246,8 +2657,17 @@
       <c r="K47">
         <v>76.821705341339097</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>89.520239830017005</v>
+      </c>
+      <c r="N47">
+        <v>0.25332533133851998</v>
+      </c>
+      <c r="O47">
+        <v>73.4147531986236</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>89.238029718399005</v>
       </c>
@@ -2275,8 +2695,17 @@
       <c r="K48">
         <v>76.058594942092896</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>88.837242126464801</v>
+      </c>
+      <c r="N48">
+        <v>0.26096192185155198</v>
+      </c>
+      <c r="O48">
+        <v>74.024282932281494</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.445943593978797</v>
       </c>
@@ -2304,8 +2733,17 @@
       <c r="K49">
         <v>76.064940690994206</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>89.109969139099107</v>
+      </c>
+      <c r="N49">
+        <v>0.24715598011463799</v>
+      </c>
+      <c r="O49">
+        <v>73.7614839076995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>89.337635040283203</v>
       </c>
@@ -2333,8 +2771,17 @@
       <c r="K50">
         <v>75.976545572280799</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>89.093369245529104</v>
+      </c>
+      <c r="N50">
+        <v>0.25077409204322998</v>
+      </c>
+      <c r="O50">
+        <v>72.682822227477999</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>89.157396554946899</v>
       </c>
@@ -2361,6 +2808,15 @@
       </c>
       <c r="K51">
         <v>75.536620140075598</v>
+      </c>
+      <c r="M51">
+        <v>89.342379570007296</v>
+      </c>
+      <c r="N51">
+        <v>0.248062007436813</v>
+      </c>
+      <c r="O51">
+        <v>73.191655397415104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 230 packet run
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E3D36C2-9544-4808-812A-C27E6D32D491}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BF6E08-9033-41AA-9396-84FC7216F08A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
   <si>
     <t>Acc</t>
   </si>
@@ -44,6 +44,9 @@
   </si>
   <si>
     <t>230 Packets</t>
+  </si>
+  <si>
+    <t>210 Packets</t>
   </si>
 </sst>
 </file>
@@ -885,15 +888,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -909,8 +912,11 @@
       <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,8 +962,17 @@
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.166885614395099</v>
       </c>
@@ -994,8 +1009,17 @@
       <c r="O3">
         <v>57.434668302535997</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>89.072024822235093</v>
+      </c>
+      <c r="R3">
+        <v>0.26912349552781201</v>
+      </c>
+      <c r="S3">
+        <v>76.8498628139495</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>88.785070180892902</v>
       </c>
@@ -1032,8 +1056,17 @@
       <c r="O4">
         <v>50.736342430114703</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>88.799297809600802</v>
+      </c>
+      <c r="R4">
+        <v>0.25287529295787198</v>
+      </c>
+      <c r="S4">
+        <v>68.147766590118394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>89.546328783035193</v>
       </c>
@@ -1070,8 +1103,17 @@
       <c r="O5">
         <v>52.417280435562098</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>89.067280292510901</v>
+      </c>
+      <c r="R5">
+        <v>0.25610320560331401</v>
+      </c>
+      <c r="S5">
+        <v>67.9189066886901</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90.113121271133394</v>
       </c>
@@ -1108,8 +1150,17 @@
       <c r="O6">
         <v>70.234991788864093</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>88.770842552185002</v>
+      </c>
+      <c r="R6">
+        <v>0.263082958474816</v>
+      </c>
+      <c r="S6">
+        <v>68.626559019088702</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>89.394551515579195</v>
       </c>
@@ -1146,8 +1197,17 @@
       <c r="O7">
         <v>72.422914505004798</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>88.4909987449646</v>
+      </c>
+      <c r="R7">
+        <v>0.25077301616098102</v>
+      </c>
+      <c r="S7">
+        <v>67.212399482726994</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>88.839614391326904</v>
       </c>
@@ -1184,8 +1244,17 @@
       <c r="O8">
         <v>73.780971765518103</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>89.019846916198702</v>
+      </c>
+      <c r="R8">
+        <v>0.25939821293550802</v>
+      </c>
+      <c r="S8">
+        <v>68.903663635253906</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.389806985855103</v>
       </c>
@@ -1222,8 +1291,17 @@
       <c r="O9">
         <v>73.470363855361896</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>88.588231801986694</v>
+      </c>
+      <c r="R9">
+        <v>0.25101132475818999</v>
+      </c>
+      <c r="S9">
+        <v>67.710575819015503</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.460951089858995</v>
       </c>
@@ -1260,8 +1338,17 @@
       <c r="O10">
         <v>73.888139009475694</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>89.026963710784898</v>
+      </c>
+      <c r="R10">
+        <v>0.25330214329852102</v>
+      </c>
+      <c r="S10">
+        <v>68.029569864273</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.043563604354802</v>
       </c>
@@ -1298,8 +1385,17 @@
       <c r="O11">
         <v>73.667391538619995</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>89.674389362335205</v>
+      </c>
+      <c r="R11">
+        <v>0.246350247479621</v>
+      </c>
+      <c r="S11">
+        <v>69.242267370223999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>89.247518777847205</v>
       </c>
@@ -1336,8 +1432,17 @@
       <c r="O12">
         <v>73.167571067810002</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>89.349490404129</v>
+      </c>
+      <c r="R12">
+        <v>0.25696080555966999</v>
+      </c>
+      <c r="S12">
+        <v>68.885797739028902</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>89.961344003677297</v>
       </c>
@@ -1374,8 +1479,17 @@
       <c r="O13">
         <v>73.064140081405597</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>89.223802089691105</v>
+      </c>
+      <c r="R13">
+        <v>0.25985198954120797</v>
+      </c>
+      <c r="S13">
+        <v>68.990481376647907</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>89.385062456130896</v>
       </c>
@@ -1412,8 +1526,17 @@
       <c r="O14">
         <v>73.371634960174504</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>89.278346300125094</v>
+      </c>
+      <c r="R14">
+        <v>0.25125204967355402</v>
+      </c>
+      <c r="S14">
+        <v>69.237408876418996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.280718564987097</v>
       </c>
@@ -1450,8 +1573,17 @@
       <c r="O15">
         <v>73.299146175384493</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>89.294946193694997</v>
+      </c>
+      <c r="R15">
+        <v>0.25244044060549198</v>
+      </c>
+      <c r="S15">
+        <v>67.954193115234304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>89.197713136672903</v>
       </c>
@@ -1488,8 +1620,17 @@
       <c r="O16">
         <v>72.054840087890597</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>89.913916587829505</v>
+      </c>
+      <c r="R16">
+        <v>0.240826629251888</v>
+      </c>
+      <c r="S16">
+        <v>68.948252916336003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.546328783035193</v>
       </c>
@@ -1526,8 +1667,17 @@
       <c r="O17">
         <v>66.818587303161607</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>89.098107814788804</v>
+      </c>
+      <c r="R17">
+        <v>0.255289133261347</v>
+      </c>
+      <c r="S17">
+        <v>68.126592636108398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.657789468765202</v>
       </c>
@@ -1564,8 +1714,17 @@
       <c r="O18">
         <v>65.315620660781804</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>89.522612094879094</v>
+      </c>
+      <c r="R18">
+        <v>0.246590712003668</v>
+      </c>
+      <c r="S18">
+        <v>68.684085369110093</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>89.0909969806671</v>
       </c>
@@ -1602,8 +1761,17 @@
       <c r="O19">
         <v>65.325640916824298</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>88.875186443328801</v>
+      </c>
+      <c r="R19">
+        <v>0.26004882433884602</v>
+      </c>
+      <c r="S19">
+        <v>68.964230775833101</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>89.420634508132906</v>
       </c>
@@ -1640,8 +1808,17 @@
       <c r="O20">
         <v>64.942824602127004</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>89.219057559966998</v>
+      </c>
+      <c r="R20">
+        <v>0.25694732281784199</v>
+      </c>
+      <c r="S20">
+        <v>68.421115875244098</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90.049088001251206</v>
       </c>
@@ -1678,8 +1855,17 @@
       <c r="O21">
         <v>71.640696287155095</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>89.534467458724905</v>
+      </c>
+      <c r="R21">
+        <v>0.25473587350469601</v>
+      </c>
+      <c r="S21">
+        <v>69.155242919921804</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>89.548701047897296</v>
       </c>
@@ -1716,8 +1902,17 @@
       <c r="O22">
         <v>72.8096537590026</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>89.394551515579195</v>
+      </c>
+      <c r="R22">
+        <v>0.25280641418191602</v>
+      </c>
+      <c r="S22">
+        <v>68.854432821273804</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>89.072024822235093</v>
       </c>
@@ -1754,8 +1949,17 @@
       <c r="O23">
         <v>73.1050026416778</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>88.851469755172701</v>
+      </c>
+      <c r="R23">
+        <v>0.26166377226755</v>
+      </c>
+      <c r="S23">
+        <v>68.335008144378605</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.920247554778996</v>
       </c>
@@ -1792,8 +1996,17 @@
       <c r="O24">
         <v>72.422594308853107</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>89.278346300125094</v>
+      </c>
+      <c r="R24">
+        <v>0.25392871053295302</v>
+      </c>
+      <c r="S24">
+        <v>68.157465219497595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88.8989031314849</v>
       </c>
@@ -1830,8 +2043,17 @@
       <c r="O25">
         <v>73.375932931899996</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>88.450682163238497</v>
+      </c>
+      <c r="R25">
+        <v>0.26895801092282801</v>
+      </c>
+      <c r="S25">
+        <v>67.761798143386798</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90.087032318115206</v>
       </c>
@@ -1868,8 +2090,17 @@
       <c r="O26">
         <v>72.435604810714693</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>89.733678102493201</v>
+      </c>
+      <c r="R26">
+        <v>0.248675107689834</v>
+      </c>
+      <c r="S26">
+        <v>68.530229330062795</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.9273583889007</v>
       </c>
@@ -1906,8 +2137,17 @@
       <c r="O27">
         <v>71.9085404872894</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>89.368462562561007</v>
+      </c>
+      <c r="R27">
+        <v>0.25674521599223599</v>
+      </c>
+      <c r="S27">
+        <v>68.778434991836505</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.425379037856999</v>
       </c>
@@ -1944,8 +2184,17 @@
       <c r="O28">
         <v>72.832605600356999</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>89.038819074630695</v>
+      </c>
+      <c r="R28">
+        <v>0.25517505047163902</v>
+      </c>
+      <c r="S28">
+        <v>67.442076683044405</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.382690191268907</v>
       </c>
@@ -1982,8 +2231,17 @@
       <c r="O29">
         <v>73.371208667755099</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>89.510756731033297</v>
+      </c>
+      <c r="R29">
+        <v>0.24333109311892101</v>
+      </c>
+      <c r="S29">
+        <v>68.255703687667804</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>89.188230037689195</v>
       </c>
@@ -2020,8 +2278,17 @@
       <c r="O30">
         <v>73.339866638183594</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>89.543956518173204</v>
+      </c>
+      <c r="R30">
+        <v>0.245791154289593</v>
+      </c>
+      <c r="S30">
+        <v>69.228202104568396</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>89.064908027648897</v>
       </c>
@@ -2058,8 +2325,17 @@
       <c r="O31">
         <v>72.988338470458899</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>88.965302705764699</v>
+      </c>
+      <c r="R31">
+        <v>0.26215698969425799</v>
+      </c>
+      <c r="S31">
+        <v>68.481005430221501</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.559776544570894</v>
       </c>
@@ -2096,8 +2372,17 @@
       <c r="O32">
         <v>73.194815874099703</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>89.152652025222693</v>
+      </c>
+      <c r="R32">
+        <v>0.251220728692363</v>
+      </c>
+      <c r="S32">
+        <v>67.891291379928504</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.588231801986694</v>
       </c>
@@ -2134,8 +2419,17 @@
       <c r="O33">
         <v>72.461916446685706</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>89.098107814788804</v>
+      </c>
+      <c r="R33">
+        <v>0.24443516779753599</v>
+      </c>
+      <c r="S33">
+        <v>68.9181227684021</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -2172,8 +2466,17 @@
       <c r="O34">
         <v>72.133360624313298</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>88.851469755172701</v>
+      </c>
+      <c r="R34">
+        <v>0.26175096853258201</v>
+      </c>
+      <c r="S34">
+        <v>68.831122875213595</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.955819606781006</v>
       </c>
@@ -2210,8 +2513,17 @@
       <c r="O35">
         <v>72.210428237914996</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>89.143168926238999</v>
+      </c>
+      <c r="R35">
+        <v>0.250213219927652</v>
+      </c>
+      <c r="S35">
+        <v>69.915167093276906</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>89.2973184585571</v>
       </c>
@@ -2248,8 +2560,17 @@
       <c r="O36">
         <v>73.164016008377004</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>89.747905731201101</v>
+      </c>
+      <c r="R36">
+        <v>0.251498217096777</v>
+      </c>
+      <c r="S36">
+        <v>69.450585126876803</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.391393423080402</v>
       </c>
@@ -2286,8 +2607,17 @@
       <c r="O37">
         <v>72.7936882972717</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>88.804042339324894</v>
+      </c>
+      <c r="R37">
+        <v>0.26033363638799401</v>
+      </c>
+      <c r="S37">
+        <v>69.064718723297105</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>89.380323886871295</v>
       </c>
@@ -2324,8 +2654,17 @@
       <c r="O38">
         <v>72.7490456104278</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>88.493371009826603</v>
+      </c>
+      <c r="R38">
+        <v>0.25170568995396603</v>
+      </c>
+      <c r="S38">
+        <v>68.731973648071204</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.7858500480651</v>
       </c>
@@ -2362,8 +2701,17 @@
       <c r="O39">
         <v>72.168561935424805</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>88.372421264648395</v>
+      </c>
+      <c r="R39">
+        <v>0.25919652122440601</v>
+      </c>
+      <c r="S39">
+        <v>68.462583303451495</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>88.863331079483004</v>
       </c>
@@ -2400,8 +2748,17 @@
       <c r="O40">
         <v>73.477121829986501</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>89.112341403961096</v>
+      </c>
+      <c r="R40">
+        <v>0.252560794765531</v>
+      </c>
+      <c r="S40">
+        <v>68.509573459625202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>89.311546087265</v>
       </c>
@@ -2438,8 +2795,17 @@
       <c r="O41">
         <v>74.128241539001394</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>89.067280292510901</v>
+      </c>
+      <c r="R41">
+        <v>0.25214308744849601</v>
+      </c>
+      <c r="S41">
+        <v>69.308448314666705</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>89.413523674011202</v>
       </c>
@@ -2476,8 +2842,17 @@
       <c r="O42">
         <v>71.630872964858995</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>89.944744110107393</v>
+      </c>
+      <c r="R42">
+        <v>0.24519696594476201</v>
+      </c>
+      <c r="S42">
+        <v>69.181425809860201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89.311546087265</v>
       </c>
@@ -2514,8 +2889,17 @@
       <c r="O43">
         <v>73.095628261566105</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>88.661748170852604</v>
+      </c>
+      <c r="R43">
+        <v>0.25244328693842799</v>
+      </c>
+      <c r="S43">
+        <v>67.910869598388601</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.290201663970905</v>
       </c>
@@ -2552,8 +2936,17 @@
       <c r="O44">
         <v>73.030666589736896</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>89.019846916198702</v>
+      </c>
+      <c r="R44">
+        <v>0.25686037386819499</v>
+      </c>
+      <c r="S44">
+        <v>67.286752700805593</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90.013515949249197</v>
       </c>
@@ -2590,8 +2983,17 @@
       <c r="O45">
         <v>73.410993814468299</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>88.896530866622896</v>
+      </c>
+      <c r="R45">
+        <v>0.26274500668609302</v>
+      </c>
+      <c r="S45">
+        <v>68.270944833755493</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90.068060159683199</v>
       </c>
@@ -2628,8 +3030,17 @@
       <c r="O46">
         <v>72.2200510501861</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>89.019846916198702</v>
+      </c>
+      <c r="R46">
+        <v>0.25729004903374297</v>
+      </c>
+      <c r="S46">
+        <v>69.058609247207599</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>89.351862668991004</v>
       </c>
@@ -2666,8 +3077,17 @@
       <c r="O47">
         <v>73.4147531986236</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>88.611948490142794</v>
+      </c>
+      <c r="R47">
+        <v>0.26704773569128498</v>
+      </c>
+      <c r="S47">
+        <v>67.666248798370304</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>89.238029718399005</v>
       </c>
@@ -2704,8 +3124,17 @@
       <c r="O48">
         <v>74.024282932281494</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>89.968460798263493</v>
+      </c>
+      <c r="R48">
+        <v>0.246782750153139</v>
+      </c>
+      <c r="S48">
+        <v>68.321039438247595</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.445943593978797</v>
       </c>
@@ -2742,8 +3171,17 @@
       <c r="O49">
         <v>73.7614839076995</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>89.306801557540894</v>
+      </c>
+      <c r="R49">
+        <v>0.25290859650150699</v>
+      </c>
+      <c r="S49">
+        <v>68.892151355743394</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>89.337635040283203</v>
       </c>
@@ -2780,8 +3218,17 @@
       <c r="O50">
         <v>72.682822227477999</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>88.792181015014606</v>
+      </c>
+      <c r="R50">
+        <v>0.25707833496460297</v>
+      </c>
+      <c r="S50">
+        <v>68.697601079940796</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>89.157396554946899</v>
       </c>
@@ -2817,6 +3264,15 @@
       </c>
       <c r="O51">
         <v>73.191655397415104</v>
+      </c>
+      <c r="Q51">
+        <v>89.145541191101003</v>
+      </c>
+      <c r="R51">
+        <v>0.25451644660448802</v>
+      </c>
+      <c r="S51">
+        <v>68.886629104614201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 210 packet run
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36BF6E08-9033-41AA-9396-84FC7216F08A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5C3512-BFC6-477F-BA03-1A159F25A9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
   <si>
     <t>Acc</t>
   </si>
@@ -47,6 +47,12 @@
   </si>
   <si>
     <t>210 Packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 88.99850845336914]</t>
+  </si>
+  <si>
+    <t>190 Packets</t>
   </si>
 </sst>
 </file>
@@ -888,15 +894,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W51"/>
+  <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z9" sqref="Z9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -915,8 +921,11 @@
       <c r="V1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="Z1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -971,8 +980,17 @@
       <c r="W2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.166885614395099</v>
       </c>
@@ -1018,8 +1036,17 @@
       <c r="S3">
         <v>76.8498628139495</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U3">
+        <v>88.6688649654388</v>
+      </c>
+      <c r="V3">
+        <v>0.25934758216158899</v>
+      </c>
+      <c r="W3">
+        <v>74.262355804443303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>88.785070180892902</v>
       </c>
@@ -1065,8 +1092,17 @@
       <c r="S4">
         <v>68.147766590118394</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U4">
+        <v>89.204829931259098</v>
+      </c>
+      <c r="V4">
+        <v>0.26116378010725699</v>
+      </c>
+      <c r="W4">
+        <v>67.056726217269897</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>89.546328783035193</v>
       </c>
@@ -1112,8 +1148,17 @@
       <c r="S5">
         <v>67.9189066886901</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U5">
+        <v>89.672017097473102</v>
+      </c>
+      <c r="V5">
+        <v>0.25677374567799599</v>
+      </c>
+      <c r="W5">
+        <v>66.8016037940979</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>90.113121271133394</v>
       </c>
@@ -1159,8 +1204,17 @@
       <c r="S6">
         <v>68.626559019088702</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U6">
+        <v>89.109969139099107</v>
+      </c>
+      <c r="V6">
+        <v>0.25671114812366902</v>
+      </c>
+      <c r="W6">
+        <v>67.263541698455796</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>89.394551515579195</v>
       </c>
@@ -1206,8 +1260,17 @@
       <c r="S7">
         <v>67.212399482726994</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U7">
+        <v>89.358979463577199</v>
+      </c>
+      <c r="V7">
+        <v>0.25011162909726298</v>
+      </c>
+      <c r="W7">
+        <v>66.447059392929006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>88.839614391326904</v>
       </c>
@@ -1253,8 +1316,17 @@
       <c r="S8">
         <v>68.903663635253906</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U8">
+        <v>88.410365581512394</v>
+      </c>
+      <c r="V8">
+        <v>0.25854574584609902</v>
+      </c>
+      <c r="W8">
+        <v>67.286705255508394</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.389806985855103</v>
       </c>
@@ -1300,8 +1372,17 @@
       <c r="S9">
         <v>67.710575819015503</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U9">
+        <v>89.138424396514793</v>
+      </c>
+      <c r="V9">
+        <v>0.25441960220068499</v>
+      </c>
+      <c r="W9">
+        <v>66.330063343048096</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.460951089858995</v>
       </c>
@@ -1347,8 +1428,17 @@
       <c r="S10">
         <v>68.029569864273</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U10">
+        <v>89.316290616989093</v>
+      </c>
+      <c r="V10">
+        <v>0.25215584548049202</v>
+      </c>
+      <c r="W10">
+        <v>67.074635744094806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.043563604354802</v>
       </c>
@@ -1394,8 +1484,17 @@
       <c r="S11">
         <v>69.242267370223999</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U11">
+        <v>89.034080505371094</v>
+      </c>
+      <c r="V11">
+        <v>0.25438966601274199</v>
+      </c>
+      <c r="W11">
+        <v>66.764318704605103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>89.247518777847205</v>
       </c>
@@ -1441,8 +1540,17 @@
       <c r="S12">
         <v>68.885797739028902</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U12">
+        <v>89.275974035263005</v>
+      </c>
+      <c r="V12">
+        <v>0.25434290394047299</v>
+      </c>
+      <c r="W12">
+        <v>66.868839502334595</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>89.961344003677297</v>
       </c>
@@ -1488,8 +1596,17 @@
       <c r="S13">
         <v>68.990481376647907</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U13">
+        <v>89.114707708358694</v>
+      </c>
+      <c r="V13">
+        <v>0.25018582702005299</v>
+      </c>
+      <c r="W13">
+        <v>66.011216163635197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>89.385062456130896</v>
       </c>
@@ -1535,8 +1652,17 @@
       <c r="S14">
         <v>69.237408876418996</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U14">
+        <v>89.498895406722994</v>
+      </c>
+      <c r="V14">
+        <v>0.251874246114559</v>
+      </c>
+      <c r="W14">
+        <v>67.089039325714097</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.280718564987097</v>
       </c>
@@ -1582,8 +1708,17 @@
       <c r="S15">
         <v>67.954193115234304</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="U15">
+        <v>88.455426692962604</v>
+      </c>
+      <c r="V15">
+        <v>0.26733159638007797</v>
+      </c>
+      <c r="W15">
+        <v>66.597969293594304</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>89.197713136672903</v>
       </c>
@@ -1629,8 +1764,17 @@
       <c r="S16">
         <v>68.948252916336003</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U16">
+        <v>89.287829399108801</v>
+      </c>
+      <c r="V16">
+        <v>0.25385067766290997</v>
+      </c>
+      <c r="W16">
+        <v>66.982653617858801</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.546328783035193</v>
       </c>
@@ -1676,8 +1820,17 @@
       <c r="S17">
         <v>68.126592636108398</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U17">
+        <v>89.821422100067096</v>
+      </c>
+      <c r="V17">
+        <v>0.25177153254137902</v>
+      </c>
+      <c r="W17">
+        <v>65.608634948730398</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.657789468765202</v>
       </c>
@@ -1723,8 +1876,17 @@
       <c r="S18">
         <v>68.684085369110093</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U18">
+        <v>88.841986656188894</v>
+      </c>
+      <c r="V18">
+        <v>0.25823497754035102</v>
+      </c>
+      <c r="W18">
+        <v>66.258340835571204</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>89.0909969806671</v>
       </c>
@@ -1770,8 +1932,17 @@
       <c r="S19">
         <v>68.964230775833101</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U19">
+        <v>88.0688667297363</v>
+      </c>
+      <c r="V19">
+        <v>0.25948571404496701</v>
+      </c>
+      <c r="W19">
+        <v>66.645341396331702</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>89.420634508132906</v>
       </c>
@@ -1817,8 +1988,17 @@
       <c r="S20">
         <v>68.421115875244098</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>88.581115007400498</v>
+      </c>
+      <c r="V20">
+        <v>0.25049730098220302</v>
+      </c>
+      <c r="W20">
+        <v>65.941144704818697</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90.049088001251206</v>
       </c>
@@ -1864,8 +2044,17 @@
       <c r="S21">
         <v>69.155242919921804</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U21">
+        <v>89.287829399108801</v>
+      </c>
+      <c r="V21">
+        <v>0.25933104252607098</v>
+      </c>
+      <c r="W21">
+        <v>66.492254495620699</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>89.548701047897296</v>
       </c>
@@ -1911,8 +2100,17 @@
       <c r="S22">
         <v>68.854432821273804</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U22">
+        <v>88.877558708190904</v>
+      </c>
+      <c r="V22">
+        <v>0.25306688412392397</v>
+      </c>
+      <c r="W22">
+        <v>67.353629589080796</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>89.072024822235093</v>
       </c>
@@ -1958,8 +2156,17 @@
       <c r="S23">
         <v>68.335008144378605</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U23">
+        <v>89.169257879257202</v>
+      </c>
+      <c r="V23">
+        <v>0.25597477278740999</v>
+      </c>
+      <c r="W23">
+        <v>67.097359657287598</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.920247554778996</v>
       </c>
@@ -2005,8 +2212,17 @@
       <c r="S24">
         <v>68.157465219497595</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>88.887041807174597</v>
+      </c>
+      <c r="V24">
+        <v>0.25601118781132098</v>
+      </c>
+      <c r="W24">
+        <v>67.054003000259399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88.8989031314849</v>
       </c>
@@ -2052,8 +2268,17 @@
       <c r="S25">
         <v>67.761798143386798</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>89.192968606948796</v>
+      </c>
+      <c r="V25">
+        <v>0.249479398120769</v>
+      </c>
+      <c r="W25">
+        <v>66.617006540298405</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90.087032318115206</v>
       </c>
@@ -2099,8 +2324,17 @@
       <c r="S26">
         <v>68.530229330062795</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U26">
+        <v>89.181113243102999</v>
+      </c>
+      <c r="V26">
+        <v>0.25443345032098502</v>
+      </c>
+      <c r="W26">
+        <v>66.326906204223604</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.9273583889007</v>
       </c>
@@ -2146,8 +2380,17 @@
       <c r="S27">
         <v>68.778434991836505</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U27">
+        <v>88.685464859008704</v>
+      </c>
+      <c r="V27">
+        <v>0.25832459695445797</v>
+      </c>
+      <c r="W27">
+        <v>67.195863962173405</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.425379037856999</v>
       </c>
@@ -2193,8 +2436,17 @@
       <c r="S28">
         <v>67.442076683044405</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>89.444351196289006</v>
+      </c>
+      <c r="V28">
+        <v>0.25188562783665502</v>
+      </c>
+      <c r="W28">
+        <v>67.372123956680298</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.382690191268907</v>
       </c>
@@ -2240,8 +2492,17 @@
       <c r="S29">
         <v>68.255703687667804</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>89.095735549926701</v>
+      </c>
+      <c r="V29">
+        <v>0.267513954964477</v>
+      </c>
+      <c r="W29">
+        <v>66.127695798873901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>89.188230037689195</v>
       </c>
@@ -2287,8 +2548,17 @@
       <c r="S30">
         <v>69.228202104568396</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U30">
+        <v>88.965302705764699</v>
+      </c>
+      <c r="V30">
+        <v>0.257179626512129</v>
+      </c>
+      <c r="W30">
+        <v>67.253837585449205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>89.064908027648897</v>
       </c>
@@ -2334,8 +2604,17 @@
       <c r="S31">
         <v>68.481005430221501</v>
       </c>
-    </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U31">
+        <v>88.426971435546804</v>
+      </c>
+      <c r="V31">
+        <v>0.25743814151486999</v>
+      </c>
+      <c r="W31">
+        <v>66.283339262008596</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.559776544570894</v>
       </c>
@@ -2381,8 +2660,17 @@
       <c r="S32">
         <v>67.891291379928504</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U32">
+        <v>89.266490936279297</v>
+      </c>
+      <c r="V32">
+        <v>0.245754239570736</v>
+      </c>
+      <c r="W32">
+        <v>66.198042154312105</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.588231801986694</v>
       </c>
@@ -2428,8 +2716,17 @@
       <c r="S33">
         <v>68.9181227684021</v>
       </c>
-    </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U33">
+        <v>88.384282588958698</v>
+      </c>
+      <c r="V33">
+        <v>0.25803214582539502</v>
+      </c>
+      <c r="W33">
+        <v>66.416597366332994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -2475,8 +2772,17 @@
       <c r="S34">
         <v>68.831122875213595</v>
       </c>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U34">
+        <v>89.200085401535006</v>
+      </c>
+      <c r="V34">
+        <v>0.26604930700906398</v>
+      </c>
+      <c r="W34">
+        <v>66.435062646865802</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.955819606781006</v>
       </c>
@@ -2522,8 +2828,17 @@
       <c r="S35">
         <v>69.915167093276906</v>
       </c>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U35">
+        <v>89.062535762786794</v>
+      </c>
+      <c r="V35">
+        <v>0.25426672133652301</v>
+      </c>
+      <c r="W35">
+        <v>66.350146055221501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>89.2973184585571</v>
       </c>
@@ -2569,8 +2884,17 @@
       <c r="S36">
         <v>69.450585126876803</v>
       </c>
-    </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U36">
+        <v>88.860958814620901</v>
+      </c>
+      <c r="V36">
+        <v>0.25741595921508098</v>
+      </c>
+      <c r="W36">
+        <v>66.787248611450195</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.391393423080402</v>
       </c>
@@ -2616,8 +2940,17 @@
       <c r="S37">
         <v>69.064718723297105</v>
       </c>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U37">
+        <v>88.811153173446598</v>
+      </c>
+      <c r="V37">
+        <v>0.25426651996323302</v>
+      </c>
+      <c r="W37">
+        <v>65.905633449554401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>89.380323886871295</v>
       </c>
@@ -2663,8 +2996,17 @@
       <c r="S38">
         <v>68.731973648071204</v>
       </c>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U38">
+        <v>88.7352645397186</v>
+      </c>
+      <c r="V38">
+        <v>0.26501452281481302</v>
+      </c>
+      <c r="W38">
+        <v>67.146267890930105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.7858500480651</v>
       </c>
@@ -2710,8 +3052,17 @@
       <c r="S39">
         <v>68.462583303451495</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U39">
+        <v>88.386654853820801</v>
+      </c>
+      <c r="V39">
+        <v>0.263480796469655</v>
+      </c>
+      <c r="W39">
+        <v>66.012729644775305</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>88.863331079483004</v>
       </c>
@@ -2757,8 +3108,17 @@
       <c r="S40">
         <v>68.509573459625202</v>
       </c>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U40">
+        <v>88.801670074462805</v>
+      </c>
+      <c r="V40">
+        <v>0.25527435053535402</v>
+      </c>
+      <c r="W40">
+        <v>66.728349447250295</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>89.311546087265</v>
       </c>
@@ -2804,8 +3164,17 @@
       <c r="S41">
         <v>69.308448314666705</v>
       </c>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U41">
+        <v>88.704437017440796</v>
+      </c>
+      <c r="V41">
+        <v>0.258508421178688</v>
+      </c>
+      <c r="W41">
+        <v>65.847539901733398</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>89.413523674011202</v>
       </c>
@@ -2851,8 +3220,17 @@
       <c r="S42">
         <v>69.181425809860201</v>
       </c>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U42">
+        <v>88.673609495162907</v>
+      </c>
+      <c r="V42">
+        <v>0.25643364860937801</v>
+      </c>
+      <c r="W42">
+        <v>66.383737802505493</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89.311546087265</v>
       </c>
@@ -2898,8 +3276,17 @@
       <c r="S43">
         <v>67.910869598388601</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U43">
+        <v>88.834869861602698</v>
+      </c>
+      <c r="V43">
+        <v>0.247812827585909</v>
+      </c>
+      <c r="W43">
+        <v>66.099624633789006</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.290201663970905</v>
       </c>
@@ -2945,8 +3332,17 @@
       <c r="S44">
         <v>67.286752700805593</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U44">
+        <v>88.2325053215026</v>
+      </c>
+      <c r="V44">
+        <v>0.27097763357065102</v>
+      </c>
+      <c r="W44">
+        <v>66.113665103912297</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90.013515949249197</v>
       </c>
@@ -2992,8 +3388,17 @@
       <c r="S45">
         <v>68.270944833755493</v>
       </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U45">
+        <v>88.799297809600802</v>
+      </c>
+      <c r="V45">
+        <v>0.25647250204662803</v>
+      </c>
+      <c r="W45">
+        <v>66.300842761993394</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90.068060159683199</v>
       </c>
@@ -3039,8 +3444,17 @@
       <c r="S46">
         <v>69.058609247207599</v>
       </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U46">
+        <v>88.135272264480506</v>
+      </c>
+      <c r="V46">
+        <v>0.26448322193947998</v>
+      </c>
+      <c r="W46">
+        <v>67.312455415725694</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>89.351862668991004</v>
       </c>
@@ -3086,8 +3500,17 @@
       <c r="S47">
         <v>67.666248798370304</v>
       </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U47">
+        <v>88.865703344344993</v>
+      </c>
+      <c r="V47">
+        <v>0.26319794338199598</v>
+      </c>
+      <c r="W47">
+        <v>65.750478267669607</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>89.238029718399005</v>
       </c>
@@ -3133,8 +3556,17 @@
       <c r="S48">
         <v>68.321039438247595</v>
       </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U48">
+        <v>89.152652025222693</v>
+      </c>
+      <c r="V48">
+        <v>0.25641162460143102</v>
+      </c>
+      <c r="W48">
+        <v>66.2691104412078</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.445943593978797</v>
       </c>
@@ -3180,8 +3612,17 @@
       <c r="S49">
         <v>68.892151355743394</v>
       </c>
-    </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U49">
+        <v>89.292573928832994</v>
+      </c>
+      <c r="V49">
+        <v>0.24674472755254201</v>
+      </c>
+      <c r="W49">
+        <v>66.859905719756995</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>89.337635040283203</v>
       </c>
@@ -3227,8 +3668,17 @@
       <c r="S50">
         <v>68.697601079940796</v>
       </c>
-    </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U50">
+        <v>88.972419500350895</v>
+      </c>
+      <c r="V50">
+        <v>0.26532755009217701</v>
+      </c>
+      <c r="W50">
+        <v>66.540035963058401</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>89.157396554946899</v>
       </c>
@@ -3273,6 +3723,15 @@
       </c>
       <c r="S51">
         <v>68.886629104614201</v>
+      </c>
+      <c r="U51" t="s">
+        <v>9</v>
+      </c>
+      <c r="V51">
+        <v>0.24941599555441599</v>
+      </c>
+      <c r="W51">
+        <v>66.768295764923096</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished 1d cnn packet select
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5C3512-BFC6-477F-BA03-1A159F25A9B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92AD52F-C104-423F-BE43-BEB70D67DA2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
     <t xml:space="preserve"> 88.99850845336914]</t>
   </si>
   <si>
-    <t>190 Packets</t>
+    <t>200 Packets</t>
   </si>
 </sst>
 </file>
@@ -897,7 +897,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9"/>
+      <selection activeCell="AA3" sqref="AA3:AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,6 +1045,15 @@
       <c r="W3">
         <v>74.262355804443303</v>
       </c>
+      <c r="Y3">
+        <v>89.105224609375</v>
+      </c>
+      <c r="Z3">
+        <v>0.25438294162742697</v>
+      </c>
+      <c r="AA3">
+        <v>73.582070589065495</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1101,6 +1110,15 @@
       <c r="W4">
         <v>67.056726217269897</v>
       </c>
+      <c r="Y4">
+        <v>89.036452770233097</v>
+      </c>
+      <c r="Z4">
+        <v>0.254669853235239</v>
+      </c>
+      <c r="AA4">
+        <v>67.9497230052948</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1157,6 +1175,15 @@
       <c r="W5">
         <v>66.8016037940979</v>
       </c>
+      <c r="Y5">
+        <v>89.3352627754211</v>
+      </c>
+      <c r="Z5">
+        <v>0.253604208176749</v>
+      </c>
+      <c r="AA5">
+        <v>66.092020034789996</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1213,6 +1240,15 @@
       <c r="W6">
         <v>67.263541698455796</v>
       </c>
+      <c r="Y6">
+        <v>88.517087697982703</v>
+      </c>
+      <c r="Z6">
+        <v>0.26864633259369203</v>
+      </c>
+      <c r="AA6">
+        <v>66.409309387207003</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1269,6 +1305,15 @@
       <c r="W7">
         <v>66.447059392929006</v>
       </c>
+      <c r="Y7">
+        <v>89.102852344512897</v>
+      </c>
+      <c r="Z7">
+        <v>0.26269290123330002</v>
+      </c>
+      <c r="AA7">
+        <v>66.010299682617102</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1325,6 +1370,15 @@
       <c r="W8">
         <v>67.286705255508394</v>
       </c>
+      <c r="Y8">
+        <v>88.602459430694495</v>
+      </c>
+      <c r="Z8">
+        <v>0.26003783162621602</v>
+      </c>
+      <c r="AA8">
+        <v>66.264995574951101</v>
+      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1381,6 +1435,15 @@
       <c r="W9">
         <v>66.330063343048096</v>
       </c>
+      <c r="Y9">
+        <v>89.280718564987097</v>
+      </c>
+      <c r="Z9">
+        <v>0.258972979994395</v>
+      </c>
+      <c r="AA9">
+        <v>65.976788997650104</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1437,6 +1500,15 @@
       <c r="W10">
         <v>67.074635744094806</v>
       </c>
+      <c r="Y10">
+        <v>88.770842552185002</v>
+      </c>
+      <c r="Z10">
+        <v>0.25462025246967701</v>
+      </c>
+      <c r="AA10">
+        <v>65.205659151077199</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1493,6 +1565,15 @@
       <c r="W11">
         <v>66.764318704605103</v>
       </c>
+      <c r="Y11">
+        <v>89.340007305145207</v>
+      </c>
+      <c r="Z11">
+        <v>0.253632214114274</v>
+      </c>
+      <c r="AA11">
+        <v>65.611485958099294</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1549,6 +1630,15 @@
       <c r="W12">
         <v>66.868839502334595</v>
       </c>
+      <c r="Y12">
+        <v>88.009577989578204</v>
+      </c>
+      <c r="Z12">
+        <v>0.27674202843933299</v>
+      </c>
+      <c r="AA12">
+        <v>66.539926290512</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1605,6 +1695,15 @@
       <c r="W13">
         <v>66.011216163635197</v>
       </c>
+      <c r="Y13">
+        <v>89.230912923812795</v>
+      </c>
+      <c r="Z13">
+        <v>0.269551629044956</v>
+      </c>
+      <c r="AA13">
+        <v>65.167735099792395</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1661,6 +1760,15 @@
       <c r="W14">
         <v>67.089039325714097</v>
       </c>
+      <c r="Y14">
+        <v>89.055424928665104</v>
+      </c>
+      <c r="Z14">
+        <v>0.25408717550116899</v>
+      </c>
+      <c r="AA14">
+        <v>65.925595998763995</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1717,6 +1825,15 @@
       <c r="W15">
         <v>66.597969293594304</v>
       </c>
+      <c r="Y15">
+        <v>88.8989031314849</v>
+      </c>
+      <c r="Z15">
+        <v>0.258276793598396</v>
+      </c>
+      <c r="AA15">
+        <v>67.157522201538001</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1773,8 +1890,17 @@
       <c r="W16">
         <v>66.982653617858801</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y16">
+        <v>88.965302705764699</v>
+      </c>
+      <c r="Z16">
+        <v>0.25737923893893799</v>
+      </c>
+      <c r="AA16">
+        <v>65.675297260284395</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.546328783035193</v>
       </c>
@@ -1829,8 +1955,17 @@
       <c r="W17">
         <v>65.608634948730398</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y17">
+        <v>88.922619819641099</v>
+      </c>
+      <c r="Z17">
+        <v>0.26277419243781802</v>
+      </c>
+      <c r="AA17">
+        <v>66.605241537094102</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.657789468765202</v>
       </c>
@@ -1885,8 +2020,17 @@
       <c r="W18">
         <v>66.258340835571204</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y18">
+        <v>88.275194168090806</v>
+      </c>
+      <c r="Z18">
+        <v>0.27176142808745202</v>
+      </c>
+      <c r="AA18">
+        <v>66.532241106033297</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>89.0909969806671</v>
       </c>
@@ -1941,8 +2085,17 @@
       <c r="W19">
         <v>66.645341396331702</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y19">
+        <v>89.043563604354802</v>
+      </c>
+      <c r="Z19">
+        <v>0.24872770649891701</v>
+      </c>
+      <c r="AA19">
+        <v>66.140627145767198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>89.420634508132906</v>
       </c>
@@ -1997,8 +2150,17 @@
       <c r="W20">
         <v>65.941144704818697</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y20">
+        <v>89.5795285701751</v>
+      </c>
+      <c r="Z20">
+        <v>0.25570197520383497</v>
+      </c>
+      <c r="AA20">
+        <v>65.496098279953003</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>90.049088001251206</v>
       </c>
@@ -2053,8 +2215,17 @@
       <c r="W21">
         <v>66.492254495620699</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y21">
+        <v>89.304435253143296</v>
+      </c>
+      <c r="Z21">
+        <v>0.26295139850374</v>
+      </c>
+      <c r="AA21">
+        <v>66.7325856685638</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>89.548701047897296</v>
       </c>
@@ -2109,8 +2280,17 @@
       <c r="W22">
         <v>67.353629589080796</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y22">
+        <v>89.375579357147203</v>
+      </c>
+      <c r="Z22">
+        <v>0.26155262232016901</v>
+      </c>
+      <c r="AA22">
+        <v>66.541148662567096</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>89.072024822235093</v>
       </c>
@@ -2165,8 +2345,17 @@
       <c r="W23">
         <v>67.097359657287598</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>89.1194522380828</v>
+      </c>
+      <c r="Z23">
+        <v>0.257388196507287</v>
+      </c>
+      <c r="AA23">
+        <v>66.388028383255005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.920247554778996</v>
       </c>
@@ -2221,8 +2410,17 @@
       <c r="W24">
         <v>67.054003000259399</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y24">
+        <v>88.417482376098604</v>
+      </c>
+      <c r="Z24">
+        <v>0.260061346537801</v>
+      </c>
+      <c r="AA24">
+        <v>65.9139981269836</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>88.8989031314849</v>
       </c>
@@ -2277,8 +2475,17 @@
       <c r="W25">
         <v>66.617006540298405</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y25">
+        <v>89.107596874237004</v>
+      </c>
+      <c r="Z25">
+        <v>0.25518282571728901</v>
+      </c>
+      <c r="AA25">
+        <v>66.501577854156494</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>90.087032318115206</v>
       </c>
@@ -2333,8 +2540,17 @@
       <c r="W26">
         <v>66.326906204223604</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y26">
+        <v>89.3210351467132</v>
+      </c>
+      <c r="Z26">
+        <v>0.25594247625935002</v>
+      </c>
+      <c r="AA26">
+        <v>65.911603450775104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.9273583889007</v>
       </c>
@@ -2389,8 +2605,17 @@
       <c r="W27">
         <v>67.195863962173405</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y27">
+        <v>89.418268203735295</v>
+      </c>
+      <c r="Z27">
+        <v>0.25779701111085102</v>
+      </c>
+      <c r="AA27">
+        <v>65.8059756755828</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.425379037856999</v>
       </c>
@@ -2445,8 +2670,17 @@
       <c r="W28">
         <v>67.372123956680298</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y28">
+        <v>89.444351196289006</v>
+      </c>
+      <c r="Z28">
+        <v>0.24904361947571199</v>
+      </c>
+      <c r="AA28">
+        <v>66.723790645599294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.382690191268907</v>
       </c>
@@ -2501,8 +2735,17 @@
       <c r="W29">
         <v>66.127695798873901</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y29">
+        <v>88.5052263736724</v>
+      </c>
+      <c r="Z29">
+        <v>0.26518077581271299</v>
+      </c>
+      <c r="AA29">
+        <v>65.204807519912706</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>89.188230037689195</v>
       </c>
@@ -2557,8 +2800,17 @@
       <c r="W30">
         <v>67.253837585449205</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y30">
+        <v>89.344745874404893</v>
+      </c>
+      <c r="Z30">
+        <v>0.25775008423846102</v>
+      </c>
+      <c r="AA30">
+        <v>66.849703073501502</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>89.064908027648897</v>
       </c>
@@ -2613,8 +2865,17 @@
       <c r="W31">
         <v>66.283339262008596</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y31">
+        <v>88.877558708190904</v>
+      </c>
+      <c r="Z31">
+        <v>0.25866306127234401</v>
+      </c>
+      <c r="AA31">
+        <v>65.678332090377793</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.559776544570894</v>
       </c>
@@ -2669,8 +2930,17 @@
       <c r="W32">
         <v>66.198042154312105</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y32">
+        <v>89.854627847671495</v>
+      </c>
+      <c r="Z32">
+        <v>0.24555993769185699</v>
+      </c>
+      <c r="AA32">
+        <v>66.234234571456895</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.588231801986694</v>
       </c>
@@ -2725,8 +2995,17 @@
       <c r="W33">
         <v>66.416597366332994</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y33">
+        <v>89.264118671417194</v>
+      </c>
+      <c r="Z33">
+        <v>0.25078757245077699</v>
+      </c>
+      <c r="AA33">
+        <v>65.366728305816594</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -2781,8 +3060,17 @@
       <c r="W34">
         <v>66.435062646865802</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y34">
+        <v>89.010363817214895</v>
+      </c>
+      <c r="Z34">
+        <v>0.26172375478293702</v>
+      </c>
+      <c r="AA34">
+        <v>65.6241614818573</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.955819606781006</v>
       </c>
@@ -2837,8 +3125,17 @@
       <c r="W35">
         <v>66.350146055221501</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y35">
+        <v>88.268077373504596</v>
+      </c>
+      <c r="Z35">
+        <v>0.25872530461726601</v>
+      </c>
+      <c r="AA35">
+        <v>66.216899871826101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>89.2973184585571</v>
       </c>
@@ -2893,8 +3190,17 @@
       <c r="W36">
         <v>66.787248611450195</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y36">
+        <v>88.2467329502105</v>
+      </c>
+      <c r="Z36">
+        <v>0.26951708561742199</v>
+      </c>
+      <c r="AA36">
+        <v>66.761482715606604</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.391393423080402</v>
       </c>
@@ -2949,8 +3255,17 @@
       <c r="W37">
         <v>65.905633449554401</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y37">
+        <v>88.543170690536499</v>
+      </c>
+      <c r="Z37">
+        <v>0.26200680068615201</v>
+      </c>
+      <c r="AA37">
+        <v>65.874914646148596</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>89.380323886871295</v>
       </c>
@@ -3005,8 +3320,17 @@
       <c r="W38">
         <v>67.146267890930105</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y38">
+        <v>88.939219713211003</v>
+      </c>
+      <c r="Z38">
+        <v>0.25170213104571498</v>
+      </c>
+      <c r="AA38">
+        <v>66.123952150344806</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.7858500480651</v>
       </c>
@@ -3061,8 +3385,17 @@
       <c r="W39">
         <v>66.012729644775305</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y39">
+        <v>88.4388267993927</v>
+      </c>
+      <c r="Z39">
+        <v>0.25689226990108799</v>
+      </c>
+      <c r="AA39">
+        <v>65.218166351318303</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>88.863331079483004</v>
       </c>
@@ -3117,8 +3450,17 @@
       <c r="W40">
         <v>66.728349447250295</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y40">
+        <v>88.436454534530597</v>
+      </c>
+      <c r="Z40">
+        <v>0.26715390335801198</v>
+      </c>
+      <c r="AA40">
+        <v>66.768859863281193</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>89.311546087265</v>
       </c>
@@ -3173,8 +3515,17 @@
       <c r="W41">
         <v>65.847539901733398</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y41">
+        <v>89.247518777847205</v>
+      </c>
+      <c r="Z41">
+        <v>0.25163316931152802</v>
+      </c>
+      <c r="AA41">
+        <v>65.841428995132404</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>89.413523674011202</v>
       </c>
@@ -3229,8 +3580,17 @@
       <c r="W42">
         <v>66.383737802505493</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y42">
+        <v>89.456212520599294</v>
+      </c>
+      <c r="Z42">
+        <v>0.251611393987623</v>
+      </c>
+      <c r="AA42">
+        <v>66.209949731826697</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>89.311546087265</v>
       </c>
@@ -3285,8 +3645,17 @@
       <c r="W43">
         <v>66.099624633789006</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y43">
+        <v>88.386654853820801</v>
+      </c>
+      <c r="Z43">
+        <v>0.267891941957629</v>
+      </c>
+      <c r="AA43">
+        <v>65.915704965591402</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.290201663970905</v>
       </c>
@@ -3341,8 +3710,17 @@
       <c r="W44">
         <v>66.113665103912297</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y44">
+        <v>88.557404279708805</v>
+      </c>
+      <c r="Z44">
+        <v>0.25702410885892202</v>
+      </c>
+      <c r="AA44">
+        <v>65.625644922256399</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>90.013515949249197</v>
       </c>
@@ -3397,8 +3775,17 @@
       <c r="W45">
         <v>66.300842761993394</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y45">
+        <v>88.400882482528601</v>
+      </c>
+      <c r="Z45">
+        <v>0.259289089396744</v>
+      </c>
+      <c r="AA45">
+        <v>65.7077312469482</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>90.068060159683199</v>
       </c>
@@ -3453,8 +3840,17 @@
       <c r="W46">
         <v>67.312455415725694</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y46">
+        <v>89.093369245529104</v>
+      </c>
+      <c r="Z46">
+        <v>0.25922640642127298</v>
+      </c>
+      <c r="AA46">
+        <v>66.727711915969806</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>89.351862668991004</v>
       </c>
@@ -3509,8 +3905,17 @@
       <c r="W47">
         <v>65.750478267669607</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y47">
+        <v>88.524198532104407</v>
+      </c>
+      <c r="Z47">
+        <v>0.26364589213584899</v>
+      </c>
+      <c r="AA47">
+        <v>65.662639856338501</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>89.238029718399005</v>
       </c>
@@ -3565,8 +3970,17 @@
       <c r="W48">
         <v>66.2691104412078</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y48">
+        <v>89.226174354553194</v>
+      </c>
+      <c r="Z48">
+        <v>0.25290057101533198</v>
+      </c>
+      <c r="AA48">
+        <v>65.695250272750798</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.445943593978797</v>
       </c>
@@ -3621,8 +4035,17 @@
       <c r="W49">
         <v>66.859905719756995</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y49">
+        <v>88.045156002044607</v>
+      </c>
+      <c r="Z49">
+        <v>0.26422306826310699</v>
+      </c>
+      <c r="AA49">
+        <v>65.567113876342702</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>89.337635040283203</v>
       </c>
@@ -3677,8 +4100,17 @@
       <c r="W50">
         <v>66.540035963058401</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y50">
+        <v>88.984274864196706</v>
+      </c>
+      <c r="Z50">
+        <v>0.25475019325397502</v>
+      </c>
+      <c r="AA50">
+        <v>66.367227077484102</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>89.157396554946899</v>
       </c>
@@ -3732,6 +4164,15 @@
       </c>
       <c r="W51">
         <v>66.768295764923096</v>
+      </c>
+      <c r="Y51">
+        <v>88.389027118682804</v>
+      </c>
+      <c r="Z51">
+        <v>0.25856195903409301</v>
+      </c>
+      <c r="AA51">
+        <v>65.674752950668307</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 298 packet run 2d
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92AD52F-C104-423F-BE43-BEB70D67DA2B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A9364D-88E2-432C-9571-A1FEA2F6E64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN 1D" sheetId="1" r:id="rId1"/>
+    <sheet name="CNN 2D" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t>Acc</t>
   </si>
@@ -896,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3:AA51"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4179,4 +4180,586 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D26FF1-09F9-44E0-BBA7-4C47B034FF96}">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>87.468874454498206</v>
+      </c>
+      <c r="B3">
+        <v>0.27769745134200002</v>
+      </c>
+      <c r="C3">
+        <v>89.2846999168396</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>87.563735246658297</v>
+      </c>
+      <c r="B4">
+        <v>0.29503988322422398</v>
+      </c>
+      <c r="C4">
+        <v>85.845623970031696</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>88.000094890594397</v>
+      </c>
+      <c r="B5">
+        <v>0.26785905080514</v>
+      </c>
+      <c r="C5">
+        <v>85.7653968334198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>87.767684459686194</v>
+      </c>
+      <c r="B6">
+        <v>0.26710454454858301</v>
+      </c>
+      <c r="C6">
+        <v>85.182788848876896</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>83.306849002838106</v>
+      </c>
+      <c r="B7">
+        <v>0.28680863579486499</v>
+      </c>
+      <c r="C7">
+        <v>82.337363481521606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>87.162947654724107</v>
+      </c>
+      <c r="B8">
+        <v>0.28182332678524202</v>
+      </c>
+      <c r="C8">
+        <v>81.9637322425842</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>87.698912620544405</v>
+      </c>
+      <c r="B9">
+        <v>0.28215008380884199</v>
+      </c>
+      <c r="C9">
+        <v>82.482324123382497</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>83.330565690994206</v>
+      </c>
+      <c r="B10">
+        <v>0.291507470804097</v>
+      </c>
+      <c r="C10">
+        <v>86.969259738922105</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>87.459385395050006</v>
+      </c>
+      <c r="B11">
+        <v>0.274819421176835</v>
+      </c>
+      <c r="C11">
+        <v>88.251056432723999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>87.826973199844304</v>
+      </c>
+      <c r="B12">
+        <v>0.26558895921090497</v>
+      </c>
+      <c r="C12">
+        <v>86.576238393783498</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>87.976378202438298</v>
+      </c>
+      <c r="B13">
+        <v>0.26511989357827398</v>
+      </c>
+      <c r="C13">
+        <v>87.722548484802203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>87.537646293640094</v>
+      </c>
+      <c r="B14">
+        <v>0.28136088573315199</v>
+      </c>
+      <c r="C14">
+        <v>81.793133020401001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>87.122631072998004</v>
+      </c>
+      <c r="B15">
+        <v>0.30348183921715999</v>
+      </c>
+      <c r="C15">
+        <v>86.800741195678697</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>88.555032014846802</v>
+      </c>
+      <c r="B16">
+        <v>0.26193962489184303</v>
+      </c>
+      <c r="C16">
+        <v>84.190393209457397</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>83.700525760650606</v>
+      </c>
+      <c r="B17">
+        <v>0.29319895227982401</v>
+      </c>
+      <c r="C17">
+        <v>85.059386491775498</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>87.964522838592501</v>
+      </c>
+      <c r="B18">
+        <v>0.28085267110243001</v>
+      </c>
+      <c r="C18">
+        <v>88.176538705825806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>87.774801254272404</v>
+      </c>
+      <c r="B19">
+        <v>0.28680695181275501</v>
+      </c>
+      <c r="C19">
+        <v>82.430211544036794</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>87.732112407684298</v>
+      </c>
+      <c r="B20">
+        <v>0.275884313022213</v>
+      </c>
+      <c r="C20">
+        <v>85.980497121810899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>83.211988210678101</v>
+      </c>
+      <c r="B21">
+        <v>0.29968467387745201</v>
+      </c>
+      <c r="C21">
+        <v>87.220519542694007</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>88.185071945190401</v>
+      </c>
+      <c r="B22">
+        <v>0.29059914103836698</v>
+      </c>
+      <c r="C22">
+        <v>86.060844182968097</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B23">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C23">
+        <v>82.944344520568805</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>87.746340036392198</v>
+      </c>
+      <c r="B24">
+        <v>0.26187385342304698</v>
+      </c>
+      <c r="C24">
+        <v>83.588365554809499</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B25">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C25">
+        <v>85.223354816436697</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B26">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C26">
+        <v>81.924137830734196</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B27">
+        <v>0.32914232458174197</v>
+      </c>
+      <c r="C27">
+        <v>88.039988994598303</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>87.770056724548297</v>
+      </c>
+      <c r="B28">
+        <v>0.26239407995377001</v>
+      </c>
+      <c r="C28">
+        <v>86.666295766830402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>86.963737010955796</v>
+      </c>
+      <c r="B29">
+        <v>0.28287483567024402</v>
+      </c>
+      <c r="C29">
+        <v>86.143874883651705</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>87.5661075115203</v>
+      </c>
+      <c r="B30">
+        <v>0.28233318821814501</v>
+      </c>
+      <c r="C30">
+        <v>82.168639659881507</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>86.911565065383897</v>
+      </c>
+      <c r="B31">
+        <v>0.29228865190134301</v>
+      </c>
+      <c r="C31">
+        <v>82.568189859390202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>87.355041503906193</v>
+      </c>
+      <c r="B32">
+        <v>0.297896636297244</v>
+      </c>
+      <c r="C32">
+        <v>88.141471385955796</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>88.367682695388794</v>
+      </c>
+      <c r="B33">
+        <v>0.26378162383908099</v>
+      </c>
+      <c r="C33">
+        <v>86.535898685455294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>88.713926076888995</v>
+      </c>
+      <c r="B34">
+        <v>0.26751537651942398</v>
+      </c>
+      <c r="C34">
+        <v>88.09033203125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>87.606424093246403</v>
+      </c>
+      <c r="B35">
+        <v>0.27296707574541801</v>
+      </c>
+      <c r="C35">
+        <v>87.8489665985107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>88.611948490142794</v>
+      </c>
+      <c r="B36">
+        <v>0.27581942583646002</v>
+      </c>
+      <c r="C36">
+        <v>86.214573621749807</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>87.509191036224294</v>
+      </c>
+      <c r="B37">
+        <v>0.28830567644077898</v>
+      </c>
+      <c r="C37">
+        <v>82.366712570190401</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B38">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C38">
+        <v>87.390394210815401</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>87.992978096008301</v>
+      </c>
+      <c r="B39">
+        <v>0.261784661588019</v>
+      </c>
+      <c r="C39">
+        <v>82.509093046188298</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>87.402468919754</v>
+      </c>
+      <c r="B40">
+        <v>0.27729379129241</v>
+      </c>
+      <c r="C40">
+        <v>86.764262437820406</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>88.014322519302297</v>
+      </c>
+      <c r="B41">
+        <v>0.264681776859853</v>
+      </c>
+      <c r="C41">
+        <v>85.485150337219196</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>84.355062246322603</v>
+      </c>
+      <c r="B42">
+        <v>0.31403404351810699</v>
+      </c>
+      <c r="C42">
+        <v>88.892863273620605</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>86.766904592513995</v>
+      </c>
+      <c r="B43">
+        <v>0.276541047344738</v>
+      </c>
+      <c r="C43">
+        <v>83.066589593887301</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B44">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C44">
+        <v>81.904806852340698</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B45">
+        <v>0.33979109252344702</v>
+      </c>
+      <c r="C45">
+        <v>82.287146091461096</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>87.682312726974402</v>
+      </c>
+      <c r="B46">
+        <v>0.261655265279719</v>
+      </c>
+      <c r="C46">
+        <v>82.849242687225299</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>86.973226070403996</v>
+      </c>
+      <c r="B47">
+        <v>0.30061166674435102</v>
+      </c>
+      <c r="C47">
+        <v>84.153202295303302</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>87.281525135040198</v>
+      </c>
+      <c r="B48">
+        <v>0.29289897332598203</v>
+      </c>
+      <c r="C48">
+        <v>88.161750078201294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>87.260180711746202</v>
+      </c>
+      <c r="B49">
+        <v>0.29638089413215002</v>
+      </c>
+      <c r="C49">
+        <v>86.880231142043996</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B50">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C50">
+        <v>87.098807334899902</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>87.736856937408405</v>
+      </c>
+      <c r="B51">
+        <v>0.271246363287586</v>
+      </c>
+      <c r="C51">
+        <v>82.711402893066406</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added 290 packet run 2d
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2A9364D-88E2-432C-9571-A1FEA2F6E64F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4568FC55-5B84-4B59-A9DF-C3AB2CD32B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
   <si>
     <t>Acc</t>
   </si>
@@ -4184,23 +4184,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D26FF1-09F9-44E0-BBA7-4C47B034FF96}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4219,8 +4222,17 @@
       <c r="G2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>87.468874454498206</v>
       </c>
@@ -4230,8 +4242,17 @@
       <c r="C3">
         <v>89.2846999168396</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>87.523418664932194</v>
+      </c>
+      <c r="F3">
+        <v>0.27601916275212202</v>
+      </c>
+      <c r="G3">
+        <v>86.042796850204397</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>87.563735246658297</v>
       </c>
@@ -4241,8 +4262,17 @@
       <c r="C4">
         <v>85.845623970031696</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>83.631747961044297</v>
+      </c>
+      <c r="F4">
+        <v>0.28836688755879702</v>
+      </c>
+      <c r="G4">
+        <v>82.178172588348303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>88.000094890594397</v>
       </c>
@@ -4252,8 +4282,17 @@
       <c r="C5">
         <v>85.7653968334198</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>88.061755895614596</v>
+      </c>
+      <c r="F5">
+        <v>0.25757784132007699</v>
+      </c>
+      <c r="G5">
+        <v>82.852301836013794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.767684459686194</v>
       </c>
@@ -4263,8 +4302,17 @@
       <c r="C6">
         <v>85.182788848876896</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>87.715512514114295</v>
+      </c>
+      <c r="F6">
+        <v>0.27564888606440002</v>
+      </c>
+      <c r="G6">
+        <v>78.845731258392306</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>83.306849002838106</v>
       </c>
@@ -4274,8 +4322,17 @@
       <c r="C7">
         <v>82.337363481521606</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>87.637251615524207</v>
+      </c>
+      <c r="F7">
+        <v>0.27157388276724398</v>
+      </c>
+      <c r="G7">
+        <v>84.234914541244507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87.162947654724107</v>
       </c>
@@ -4285,8 +4342,17 @@
       <c r="C8">
         <v>81.9637322425842</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>87.822228670120197</v>
+      </c>
+      <c r="F8">
+        <v>0.27510275845858601</v>
+      </c>
+      <c r="G8">
+        <v>83.965537786483694</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>87.698912620544405</v>
       </c>
@@ -4296,8 +4362,17 @@
       <c r="C9">
         <v>82.482324123382497</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>83.297365903854299</v>
+      </c>
+      <c r="F9">
+        <v>0.32062178085626702</v>
+      </c>
+      <c r="G9">
+        <v>83.761220932006793</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>83.330565690994206</v>
       </c>
@@ -4307,8 +4382,17 @@
       <c r="C10">
         <v>86.969259738922105</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>86.024618148803697</v>
+      </c>
+      <c r="F10">
+        <v>0.298445907240941</v>
+      </c>
+      <c r="G10">
+        <v>82.680081844329806</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>87.459385395050006</v>
       </c>
@@ -4318,8 +4402,17 @@
       <c r="C11">
         <v>88.251056432723999</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>88.358193635940495</v>
+      </c>
+      <c r="F11">
+        <v>0.26434668743870698</v>
+      </c>
+      <c r="G11">
+        <v>78.730302333831702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>87.826973199844304</v>
       </c>
@@ -4329,8 +4422,17 @@
       <c r="C12">
         <v>86.576238393783498</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>87.215119600296006</v>
+      </c>
+      <c r="F12">
+        <v>0.27926671390230401</v>
+      </c>
+      <c r="G12">
+        <v>82.667416334152193</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>87.976378202438298</v>
       </c>
@@ -4340,8 +4442,17 @@
       <c r="C13">
         <v>87.722548484802203</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>87.573218345642005</v>
+      </c>
+      <c r="F13">
+        <v>0.278621514167321</v>
+      </c>
+      <c r="G13">
+        <v>83.788228511810303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>87.537646293640094</v>
       </c>
@@ -4351,8 +4462,17 @@
       <c r="C14">
         <v>81.793133020401001</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>85.076010227203298</v>
+      </c>
+      <c r="F14">
+        <v>0.28687788840489897</v>
+      </c>
+      <c r="G14">
+        <v>78.902676582336397</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87.122631072998004</v>
       </c>
@@ -4362,8 +4482,17 @@
       <c r="C15">
         <v>86.800741195678697</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>87.558990716934204</v>
+      </c>
+      <c r="F15">
+        <v>0.265405901820637</v>
+      </c>
+      <c r="G15">
+        <v>82.747016906738196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.555032014846802</v>
       </c>
@@ -4373,8 +4502,17 @@
       <c r="C16">
         <v>84.190393209457397</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>83.491832017898503</v>
+      </c>
+      <c r="F16">
+        <v>0.287447618680373</v>
+      </c>
+      <c r="G16">
+        <v>83.847701549530001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>83.700525760650606</v>
       </c>
@@ -4384,8 +4522,17 @@
       <c r="C17">
         <v>85.059386491775498</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>87.990605831146198</v>
+      </c>
+      <c r="F17">
+        <v>0.28632474602824298</v>
+      </c>
+      <c r="G17">
+        <v>78.339874029159503</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>87.964522838592501</v>
       </c>
@@ -4395,8 +4542,17 @@
       <c r="C18">
         <v>88.176538705825806</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>87.060970067977905</v>
+      </c>
+      <c r="F18">
+        <v>0.27733732076754403</v>
+      </c>
+      <c r="G18">
+        <v>78.372923135757404</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>87.774801254272404</v>
       </c>
@@ -4406,8 +4562,17 @@
       <c r="C19">
         <v>82.430211544036794</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>83.261793851852403</v>
+      </c>
+      <c r="F19">
+        <v>0.30469947454019902</v>
+      </c>
+      <c r="G19">
+        <v>82.768985271453801</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>87.732112407684298</v>
       </c>
@@ -4417,8 +4582,17 @@
       <c r="C20">
         <v>85.980497121810899</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>87.312352657318101</v>
+      </c>
+      <c r="F20">
+        <v>0.31860044258782599</v>
+      </c>
+      <c r="G20">
+        <v>78.103746414184499</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>83.211988210678101</v>
       </c>
@@ -4428,8 +4602,17 @@
       <c r="C21">
         <v>87.220519542694007</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>86.420661211013794</v>
+      </c>
+      <c r="F21">
+        <v>0.29146146650996102</v>
+      </c>
+      <c r="G21">
+        <v>83.461101055145207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>88.185071945190401</v>
       </c>
@@ -4439,8 +4622,17 @@
       <c r="C22">
         <v>86.060844182968097</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>87.392985820770207</v>
+      </c>
+      <c r="F22">
+        <v>0.28529822053480702</v>
+      </c>
+      <c r="G22">
+        <v>84.087702035903902</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>82.941639423370304</v>
       </c>
@@ -4450,8 +4642,17 @@
       <c r="C23">
         <v>82.944344520568805</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>87.480729818344102</v>
+      </c>
+      <c r="F23">
+        <v>0.28788178539928799</v>
+      </c>
+      <c r="G23">
+        <v>82.849156379699707</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>87.746340036392198</v>
       </c>
@@ -4461,8 +4662,17 @@
       <c r="C24">
         <v>83.588365554809499</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>88.154244422912598</v>
+      </c>
+      <c r="F24">
+        <v>0.26996309225579901</v>
+      </c>
+      <c r="G24">
+        <v>84.929803609847994</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>82.941639423370304</v>
       </c>
@@ -4472,8 +4682,17 @@
       <c r="C25">
         <v>85.223354816436697</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>87.480729818344102</v>
+      </c>
+      <c r="F25">
+        <v>0.26997012312736401</v>
+      </c>
+      <c r="G25">
+        <v>78.031920909881507</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>82.941639423370304</v>
       </c>
@@ -4483,8 +4702,17 @@
       <c r="C26">
         <v>81.924137830734196</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>88.042783737182603</v>
+      </c>
+      <c r="F26">
+        <v>0.26982108908240598</v>
+      </c>
+      <c r="G26">
+        <v>83.901474714279104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>82.941639423370304</v>
       </c>
@@ -4494,8 +4722,17 @@
       <c r="C27">
         <v>88.039988994598303</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>87.834089994430499</v>
+      </c>
+      <c r="F27">
+        <v>0.27539024574641702</v>
+      </c>
+      <c r="G27">
+        <v>83.4094624519348</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>87.770056724548297</v>
       </c>
@@ -4505,8 +4742,17 @@
       <c r="C28">
         <v>86.666295766830402</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="F28">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="G28">
+        <v>81.862338066101003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>86.963737010955796</v>
       </c>
@@ -4516,8 +4762,17 @@
       <c r="C29">
         <v>86.143874883651705</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="F29">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="G29">
+        <v>82.8009259700775</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>87.5661075115203</v>
       </c>
@@ -4527,8 +4782,17 @@
       <c r="C30">
         <v>82.168639659881507</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="F30">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="G30">
+        <v>82.688198804855304</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>86.911565065383897</v>
       </c>
@@ -4538,8 +4802,17 @@
       <c r="C31">
         <v>82.568189859390202</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>87.843573093414307</v>
+      </c>
+      <c r="F31">
+        <v>0.268820609204653</v>
+      </c>
+      <c r="G31">
+        <v>83.282687425613403</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>87.355041503906193</v>
       </c>
@@ -4549,8 +4822,17 @@
       <c r="C32">
         <v>88.141471385955796</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="F32">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="G32">
+        <v>79.176611661910997</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.367682695388794</v>
       </c>
@@ -4560,8 +4842,17 @@
       <c r="C33">
         <v>86.535898685455294</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>87.094175815582204</v>
+      </c>
+      <c r="F33">
+        <v>0.26979230514485403</v>
+      </c>
+      <c r="G33">
+        <v>79.665502071380601</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.713926076888995</v>
       </c>
@@ -4571,8 +4862,17 @@
       <c r="C34">
         <v>88.09033203125</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>86.420661211013794</v>
+      </c>
+      <c r="F34">
+        <v>0.31910174135417702</v>
+      </c>
+      <c r="G34">
+        <v>78.725725173950195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>87.606424093246403</v>
       </c>
@@ -4582,8 +4882,17 @@
       <c r="C35">
         <v>87.8489665985107</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>87.7582013607025</v>
+      </c>
+      <c r="F35">
+        <v>0.27807993861128399</v>
+      </c>
+      <c r="G35">
+        <v>82.961811542510901</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.611948490142794</v>
       </c>
@@ -4593,8 +4902,17 @@
       <c r="C36">
         <v>86.214573621749807</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>83.302110433578406</v>
+      </c>
+      <c r="F36">
+        <v>0.29837795085629798</v>
+      </c>
+      <c r="G36">
+        <v>80.4127902984619</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>87.509191036224294</v>
       </c>
@@ -4604,8 +4922,17 @@
       <c r="C37">
         <v>82.366712570190401</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>87.570852041244507</v>
+      </c>
+      <c r="F37">
+        <v>0.28663002960216899</v>
+      </c>
+      <c r="G37">
+        <v>82.908334255218506</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>82.941639423370304</v>
       </c>
@@ -4615,8 +4942,17 @@
       <c r="C38">
         <v>87.390394210815401</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>87.103658914565997</v>
+      </c>
+      <c r="F38">
+        <v>0.29996143048544099</v>
+      </c>
+      <c r="G38">
+        <v>78.399708509445105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>87.992978096008301</v>
       </c>
@@ -4626,8 +4962,17 @@
       <c r="C39">
         <v>82.509093046188298</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>87.6182794570922</v>
+      </c>
+      <c r="F39">
+        <v>0.31409958712108998</v>
+      </c>
+      <c r="G39">
+        <v>83.599899291992102</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.402468919754</v>
       </c>
@@ -4637,8 +4982,17 @@
       <c r="C40">
         <v>86.764262437820406</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>87.134486436843801</v>
+      </c>
+      <c r="F40">
+        <v>0.29030622976850001</v>
+      </c>
+      <c r="G40">
+        <v>82.726615190505896</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.014322519302297</v>
       </c>
@@ -4648,8 +5002,17 @@
       <c r="C41">
         <v>85.485150337219196</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>87.253063917160006</v>
+      </c>
+      <c r="F41">
+        <v>0.29968842456796302</v>
+      </c>
+      <c r="G41">
+        <v>82.879879236221299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>84.355062246322603</v>
       </c>
@@ -4659,8 +5022,17 @@
       <c r="C42">
         <v>88.892863273620605</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>87.687051296234102</v>
+      </c>
+      <c r="F42">
+        <v>0.27863506997420601</v>
+      </c>
+      <c r="G42">
+        <v>78.569346189498901</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>86.766904592513995</v>
       </c>
@@ -4670,8 +5042,17 @@
       <c r="C43">
         <v>83.066589593887301</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="F43">
+        <v>0.33626153936570802</v>
+      </c>
+      <c r="G43">
+        <v>79.537481307983398</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>82.941639423370304</v>
       </c>
@@ -4681,8 +5062,17 @@
       <c r="C44">
         <v>81.904806852340698</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>88.0688667297363</v>
+      </c>
+      <c r="F44">
+        <v>0.27671523363010903</v>
+      </c>
+      <c r="G44">
+        <v>84.583001375198293</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -4692,8 +5082,17 @@
       <c r="C45">
         <v>82.287146091461096</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>87.748712301254201</v>
+      </c>
+      <c r="F45">
+        <v>0.26505278520989101</v>
+      </c>
+      <c r="G45">
+        <v>80.653891801834106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>87.682312726974402</v>
       </c>
@@ -4703,8 +5102,17 @@
       <c r="C46">
         <v>82.849242687225299</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>87.646740674972506</v>
+      </c>
+      <c r="F46">
+        <v>0.27481404390639003</v>
+      </c>
+      <c r="G46">
+        <v>83.2636559009552</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>86.973226070403996</v>
       </c>
@@ -4714,8 +5122,17 @@
       <c r="C47">
         <v>84.153202295303302</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>87.518674135208101</v>
+      </c>
+      <c r="F47">
+        <v>0.27853036461736802</v>
+      </c>
+      <c r="G47">
+        <v>83.485069274902301</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>87.281525135040198</v>
       </c>
@@ -4725,8 +5142,17 @@
       <c r="C48">
         <v>88.161750078201294</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>87.736856937408405</v>
+      </c>
+      <c r="F48">
+        <v>0.27262644007157699</v>
+      </c>
+      <c r="G48">
+        <v>83.912900447845402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>87.260180711746202</v>
       </c>
@@ -4736,8 +5162,17 @@
       <c r="C49">
         <v>86.880231142043996</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>87.094175815582204</v>
+      </c>
+      <c r="F49">
+        <v>0.29761943380857298</v>
+      </c>
+      <c r="G49">
+        <v>79.744165182113605</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>82.941639423370304</v>
       </c>
@@ -4747,8 +5182,17 @@
       <c r="C50">
         <v>87.098807334899902</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>87.900489568710299</v>
+      </c>
+      <c r="F50">
+        <v>0.28061396861286497</v>
+      </c>
+      <c r="G50">
+        <v>78.309705734252901</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>87.736856937408405</v>
       </c>
@@ -4757,6 +5201,15 @@
       </c>
       <c r="C51">
         <v>82.711402893066406</v>
+      </c>
+      <c r="E51">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="F51">
+        <v>0.46228909113169803</v>
+      </c>
+      <c r="G51">
+        <v>82.619557142257605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 270 packet run 2d
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4568FC55-5B84-4B59-A9DF-C3AB2CD32B72}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C8E351-C6C3-4EC5-A572-BC17A6F082E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="11">
   <si>
     <t>Acc</t>
   </si>
@@ -4184,15 +4184,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D26FF1-09F9-44E0-BBA7-4C47B034FF96}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:P51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4202,8 +4202,11 @@
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4231,8 +4234,17 @@
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>87.468874454498206</v>
       </c>
@@ -4251,8 +4263,18 @@
       <c r="G3">
         <v>86.042796850204397</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>87.701284885406494</v>
+      </c>
+      <c r="J3">
+        <v>0.281579822667617</v>
+      </c>
+      <c r="K3">
+        <v>80.972155332565293</v>
+      </c>
+      <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>87.563735246658297</v>
       </c>
@@ -4271,8 +4293,17 @@
       <c r="G4">
         <v>82.178172588348303</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>87.7582013607025</v>
+      </c>
+      <c r="J4">
+        <v>0.26426110206051301</v>
+      </c>
+      <c r="K4">
+        <v>78.541208028793307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>88.000094890594397</v>
       </c>
@@ -4291,8 +4322,17 @@
       <c r="G5">
         <v>82.852301836013794</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>82.946377992630005</v>
+      </c>
+      <c r="J5">
+        <v>0.32385418468048899</v>
+      </c>
+      <c r="K5">
+        <v>79.411511182785006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.767684459686194</v>
       </c>
@@ -4311,8 +4351,17 @@
       <c r="G6">
         <v>78.845731258392306</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>87.912350893020601</v>
+      </c>
+      <c r="J6">
+        <v>0.27443617149637201</v>
+      </c>
+      <c r="K6">
+        <v>74.000648260116506</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>83.306849002838106</v>
       </c>
@@ -4331,8 +4380,17 @@
       <c r="G7">
         <v>84.234914541244507</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>84.151113033294607</v>
+      </c>
+      <c r="J7">
+        <v>0.29780629344655002</v>
+      </c>
+      <c r="K7">
+        <v>75.676692724227905</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87.162947654724107</v>
       </c>
@@ -4351,8 +4409,17 @@
       <c r="G8">
         <v>83.965537786483694</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>87.848317623138399</v>
+      </c>
+      <c r="J8">
+        <v>0.27876328906797898</v>
+      </c>
+      <c r="K8">
+        <v>79.787362098693805</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>87.698912620544405</v>
       </c>
@@ -4371,8 +4438,17 @@
       <c r="G9">
         <v>83.761220932006793</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>87.291008234024005</v>
+      </c>
+      <c r="J9">
+        <v>0.27485895048335901</v>
+      </c>
+      <c r="K9">
+        <v>76.678598642349201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>83.330565690994206</v>
       </c>
@@ -4391,8 +4467,17 @@
       <c r="G10">
         <v>82.680081844329806</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>87.736856937408405</v>
+      </c>
+      <c r="J10">
+        <v>0.27890797038134202</v>
+      </c>
+      <c r="K10">
+        <v>79.052517175674396</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>87.459385395050006</v>
       </c>
@@ -4411,8 +4496,17 @@
       <c r="G11">
         <v>78.730302333831702</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>87.136858701705904</v>
+      </c>
+      <c r="J11">
+        <v>0.26925302901499998</v>
+      </c>
+      <c r="K11">
+        <v>78.737239837646399</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>87.826973199844304</v>
       </c>
@@ -4431,8 +4525,17 @@
       <c r="G12">
         <v>82.667416334152193</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>87.317097187042194</v>
+      </c>
+      <c r="J12">
+        <v>0.26928981486074</v>
+      </c>
+      <c r="K12">
+        <v>73.556599617004395</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>87.976378202438298</v>
       </c>
@@ -4451,8 +4554,17 @@
       <c r="G13">
         <v>83.788228511810303</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>86.963737010955796</v>
+      </c>
+      <c r="J13">
+        <v>0.28855843345665799</v>
+      </c>
+      <c r="K13">
+        <v>79.295894861221299</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>87.537646293640094</v>
       </c>
@@ -4471,8 +4583,17 @@
       <c r="G14">
         <v>78.902676582336397</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>87.5661075115203</v>
+      </c>
+      <c r="J14">
+        <v>0.27154288616769101</v>
+      </c>
+      <c r="K14">
+        <v>73.768463850021305</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87.122631072998004</v>
       </c>
@@ -4491,8 +4612,17 @@
       <c r="G15">
         <v>82.747016906738196</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J15">
+        <v>0.36397536017183901</v>
+      </c>
+      <c r="K15">
+        <v>73.477962732315007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.555032014846802</v>
       </c>
@@ -4511,8 +4641,17 @@
       <c r="G16">
         <v>83.847701549530001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>88.156616687774601</v>
+      </c>
+      <c r="J16">
+        <v>0.263351672608027</v>
+      </c>
+      <c r="K16">
+        <v>78.990332841873098</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>83.700525760650606</v>
       </c>
@@ -4531,8 +4670,17 @@
       <c r="G17">
         <v>78.339874029159503</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J17">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K17">
+        <v>78.900684118270803</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>87.964522838592501</v>
       </c>
@@ -4551,8 +4699,17 @@
       <c r="G18">
         <v>78.372923135757404</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>87.784284353256197</v>
+      </c>
+      <c r="J18">
+        <v>0.267221673143484</v>
+      </c>
+      <c r="K18">
+        <v>74.1186909675598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>87.774801254272404</v>
       </c>
@@ -4571,8 +4728,17 @@
       <c r="G19">
         <v>82.768985271453801</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>87.106031179428101</v>
+      </c>
+      <c r="J19">
+        <v>0.28073625322633999</v>
+      </c>
+      <c r="K19">
+        <v>79.827952384948702</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>87.732112407684298</v>
       </c>
@@ -4591,8 +4757,17 @@
       <c r="G20">
         <v>78.103746414184499</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>87.063342332839895</v>
+      </c>
+      <c r="J20">
+        <v>0.27096173594753098</v>
+      </c>
+      <c r="K20">
+        <v>80.142581701278601</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>83.211988210678101</v>
       </c>
@@ -4611,8 +4786,17 @@
       <c r="G21">
         <v>83.461101055145207</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J21">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K21">
+        <v>78.234706163406301</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>88.185071945190401</v>
       </c>
@@ -4631,8 +4815,17 @@
       <c r="G22">
         <v>84.087702035903902</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>88.832497596740694</v>
+      </c>
+      <c r="J22">
+        <v>0.25051751339032202</v>
+      </c>
+      <c r="K22">
+        <v>75.989291429519596</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>82.941639423370304</v>
       </c>
@@ -4651,8 +4844,17 @@
       <c r="G23">
         <v>82.849156379699707</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>88.007211685180593</v>
+      </c>
+      <c r="J23">
+        <v>0.26455069644328499</v>
+      </c>
+      <c r="K23">
+        <v>78.745748519897404</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>87.746340036392198</v>
       </c>
@@ -4671,8 +4873,17 @@
       <c r="G24">
         <v>84.929803609847994</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J24">
+        <v>0.36215162343127799</v>
+      </c>
+      <c r="K24">
+        <v>78.887847423553396</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>82.941639423370304</v>
       </c>
@@ -4691,8 +4902,17 @@
       <c r="G25">
         <v>78.031920909881507</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>88.486254215240393</v>
+      </c>
+      <c r="J25">
+        <v>0.27336596498878402</v>
+      </c>
+      <c r="K25">
+        <v>79.977481842041001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>82.941639423370304</v>
       </c>
@@ -4711,8 +4931,17 @@
       <c r="G26">
         <v>83.901474714279104</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>86.949509382247896</v>
+      </c>
+      <c r="J26">
+        <v>0.30994683470727402</v>
+      </c>
+      <c r="K26">
+        <v>74.751729488372803</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>82.941639423370304</v>
       </c>
@@ -4731,8 +4960,17 @@
       <c r="G27">
         <v>83.4094624519348</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>87.298125028610201</v>
+      </c>
+      <c r="J27">
+        <v>0.29157089938466801</v>
+      </c>
+      <c r="K27">
+        <v>79.983191728591905</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>87.770056724548297</v>
       </c>
@@ -4751,8 +4989,17 @@
       <c r="G28">
         <v>81.862338066101003</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>87.191402912139793</v>
+      </c>
+      <c r="J28">
+        <v>0.28714244804722799</v>
+      </c>
+      <c r="K28">
+        <v>79.043774604797306</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>86.963737010955796</v>
       </c>
@@ -4771,8 +5018,17 @@
       <c r="G29">
         <v>82.8009259700775</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>87.798517942428504</v>
+      </c>
+      <c r="J29">
+        <v>0.26780801476218402</v>
+      </c>
+      <c r="K29">
+        <v>79.591427564620901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>87.5661075115203</v>
       </c>
@@ -4791,8 +5047,17 @@
       <c r="G30">
         <v>82.688198804855304</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J30">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K30">
+        <v>76.579574584960895</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>86.911565065383897</v>
       </c>
@@ -4811,8 +5076,17 @@
       <c r="G31">
         <v>83.282687425613403</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J31">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K31">
+        <v>78.583029270172105</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>87.355041503906193</v>
       </c>
@@ -4831,8 +5105,17 @@
       <c r="G32">
         <v>79.176611661910997</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>88.128155469894395</v>
+      </c>
+      <c r="J32">
+        <v>0.262321183658207</v>
+      </c>
+      <c r="K32">
+        <v>78.656756401061998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.367682695388794</v>
       </c>
@@ -4851,8 +5134,17 @@
       <c r="G33">
         <v>79.665502071380601</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J33">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K33">
+        <v>80.617680311203003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.713926076888995</v>
       </c>
@@ -4871,8 +5163,17 @@
       <c r="G34">
         <v>78.725725173950195</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J34">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K34">
+        <v>80.356753349304199</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>87.606424093246403</v>
       </c>
@@ -4891,8 +5192,17 @@
       <c r="G35">
         <v>82.961811542510901</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>87.1297478675842</v>
+      </c>
+      <c r="J35">
+        <v>0.28395239979500098</v>
+      </c>
+      <c r="K35">
+        <v>80.6863050460815</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.611948490142794</v>
       </c>
@@ -4911,8 +5221,17 @@
       <c r="G36">
         <v>80.4127902984619</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>87.755829095840397</v>
+      </c>
+      <c r="J36">
+        <v>0.27187566282327602</v>
+      </c>
+      <c r="K36">
+        <v>76.584472179412799</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>87.509191036224294</v>
       </c>
@@ -4931,8 +5250,17 @@
       <c r="G37">
         <v>82.908334255218506</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>87.888634204864502</v>
+      </c>
+      <c r="J37">
+        <v>0.27590422758115002</v>
+      </c>
+      <c r="K37">
+        <v>79.409518241882296</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>82.941639423370304</v>
       </c>
@@ -4951,8 +5279,17 @@
       <c r="G38">
         <v>78.399708509445105</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>87.577962875366197</v>
+      </c>
+      <c r="J38">
+        <v>0.28363601776416297</v>
+      </c>
+      <c r="K38">
+        <v>74.430688619613605</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>87.992978096008301</v>
       </c>
@@ -4971,8 +5308,17 @@
       <c r="G39">
         <v>83.599899291992102</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>87.767684459686194</v>
+      </c>
+      <c r="J39">
+        <v>0.26228163083129802</v>
+      </c>
+      <c r="K39">
+        <v>78.724582195281897</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.402468919754</v>
       </c>
@@ -4991,8 +5337,17 @@
       <c r="G40">
         <v>82.726615190505896</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>84.217518568038898</v>
+      </c>
+      <c r="J40">
+        <v>0.29633449149425201</v>
+      </c>
+      <c r="K40">
+        <v>78.965286254882798</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.014322519302297</v>
       </c>
@@ -5011,8 +5366,17 @@
       <c r="G41">
         <v>82.879879236221299</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>87.743967771530095</v>
+      </c>
+      <c r="J41">
+        <v>0.26737022138150401</v>
+      </c>
+      <c r="K41">
+        <v>80.286141395568805</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>84.355062246322603</v>
       </c>
@@ -5031,8 +5395,17 @@
       <c r="G42">
         <v>78.569346189498901</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>88.306021690368596</v>
+      </c>
+      <c r="J42">
+        <v>0.27982012202458001</v>
+      </c>
+      <c r="K42">
+        <v>79.297119140625</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>86.766904592513995</v>
       </c>
@@ -5051,8 +5424,17 @@
       <c r="G43">
         <v>79.537481307983398</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>87.722629308700505</v>
+      </c>
+      <c r="J43">
+        <v>0.26376537824767798</v>
+      </c>
+      <c r="K43">
+        <v>78.875142335891695</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>82.941639423370304</v>
       </c>
@@ -5071,8 +5453,17 @@
       <c r="G44">
         <v>84.583001375198293</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J44">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K44">
+        <v>78.057503223419104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -5091,8 +5482,17 @@
       <c r="G45">
         <v>80.653891801834106</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>86.857020854949894</v>
+      </c>
+      <c r="J45">
+        <v>0.295255313200599</v>
+      </c>
+      <c r="K45">
+        <v>78.459477186203003</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>87.682312726974402</v>
       </c>
@@ -5111,8 +5511,17 @@
       <c r="G46">
         <v>83.2636559009552</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J46">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K46">
+        <v>78.317126512527395</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>86.973226070403996</v>
       </c>
@@ -5131,8 +5540,17 @@
       <c r="G47">
         <v>83.485069274902301</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>88.559776544570894</v>
+      </c>
+      <c r="J47">
+        <v>0.27634043613196901</v>
+      </c>
+      <c r="K47">
+        <v>80.199063062667804</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>87.281525135040198</v>
       </c>
@@ -5151,8 +5569,17 @@
       <c r="G48">
         <v>83.912900447845402</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J48">
+        <v>0.30398330739653601</v>
+      </c>
+      <c r="K48">
+        <v>77.574971914291297</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>87.260180711746202</v>
       </c>
@@ -5171,8 +5598,17 @@
       <c r="G49">
         <v>79.744165182113605</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>88.071238994598303</v>
+      </c>
+      <c r="J49">
+        <v>0.269248082937873</v>
+      </c>
+      <c r="K49">
+        <v>80.014773368835407</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>82.941639423370304</v>
       </c>
@@ -5191,8 +5627,17 @@
       <c r="G50">
         <v>78.309705734252901</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>87.717884778976398</v>
+      </c>
+      <c r="J50">
+        <v>0.27013809832448699</v>
+      </c>
+      <c r="K50">
+        <v>79.551973342895494</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>87.736856937408405</v>
       </c>
@@ -5210,6 +5655,15 @@
       </c>
       <c r="G51">
         <v>82.619557142257605</v>
+      </c>
+      <c r="I51">
+        <v>87.789028882980304</v>
+      </c>
+      <c r="J51">
+        <v>0.28877040364610901</v>
+      </c>
+      <c r="K51">
+        <v>79.829184055328298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 250 packet run 2d
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C8E351-C6C3-4EC5-A572-BC17A6F082E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195B6DBA-341A-4392-A3D0-85AE7899BAC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
   <si>
     <t>Acc</t>
   </si>
@@ -4184,15 +4184,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D26FF1-09F9-44E0-BBA7-4C47B034FF96}">
-  <dimension ref="A1:P51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="T14" sqref="T14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4205,8 +4205,11 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4243,8 +4246,17 @@
       <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>87.468874454498206</v>
       </c>
@@ -4272,9 +4284,18 @@
       <c r="K3">
         <v>80.972155332565293</v>
       </c>
+      <c r="M3">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N3">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="O3">
+        <v>79.981187105178805</v>
+      </c>
       <c r="P3" s="1"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>87.563735246658297</v>
       </c>
@@ -4302,8 +4323,17 @@
       <c r="K4">
         <v>78.541208028793307</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>87.829345464706407</v>
+      </c>
+      <c r="N4">
+        <v>0.264625312352887</v>
+      </c>
+      <c r="O4">
+        <v>70.9035866260528</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>88.000094890594397</v>
       </c>
@@ -4331,8 +4361,17 @@
       <c r="K5">
         <v>79.411511182785006</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>87.869662046432495</v>
+      </c>
+      <c r="N5">
+        <v>0.275874593980038</v>
+      </c>
+      <c r="O5">
+        <v>69.936318874359102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.767684459686194</v>
       </c>
@@ -4360,8 +4399,17 @@
       <c r="K6">
         <v>74.000648260116506</v>
       </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>88.379538059234605</v>
+      </c>
+      <c r="N6">
+        <v>0.25691701595578398</v>
+      </c>
+      <c r="O6">
+        <v>76.476198911666799</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>83.306849002838106</v>
       </c>
@@ -4389,8 +4437,17 @@
       <c r="K7">
         <v>75.676692724227905</v>
       </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>87.3502969741821</v>
+      </c>
+      <c r="N7">
+        <v>0.277072963475259</v>
+      </c>
+      <c r="O7">
+        <v>75.686116695403996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87.162947654724107</v>
       </c>
@@ -4418,8 +4475,17 @@
       <c r="K8">
         <v>79.787362098693805</v>
       </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N8">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="O8">
+        <v>70.673139333724905</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>87.698912620544405</v>
       </c>
@@ -4447,8 +4513,17 @@
       <c r="K9">
         <v>76.678598642349201</v>
       </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>87.876772880554199</v>
+      </c>
+      <c r="N9">
+        <v>0.273769662052744</v>
+      </c>
+      <c r="O9">
+        <v>75.790327787399207</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>83.330565690994206</v>
       </c>
@@ -4476,8 +4551,17 @@
       <c r="K10">
         <v>79.052517175674396</v>
       </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>88.498115539550696</v>
+      </c>
+      <c r="N10">
+        <v>0.27249325014062198</v>
+      </c>
+      <c r="O10">
+        <v>73.677732467651296</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>87.459385395050006</v>
       </c>
@@ -4505,8 +4589,17 @@
       <c r="K11">
         <v>78.737239837646399</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>87.025398015975895</v>
+      </c>
+      <c r="N11">
+        <v>0.28442993207168299</v>
+      </c>
+      <c r="O11">
+        <v>72.953715562820406</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>87.826973199844304</v>
       </c>
@@ -4534,8 +4627,17 @@
       <c r="K12">
         <v>73.556599617004395</v>
       </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>87.245953083038302</v>
+      </c>
+      <c r="N12">
+        <v>0.26331662705797199</v>
+      </c>
+      <c r="O12">
+        <v>77.163248062133704</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>87.976378202438298</v>
       </c>
@@ -4563,8 +4665,17 @@
       <c r="K13">
         <v>79.295894861221299</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>87.011170387267995</v>
+      </c>
+      <c r="N13">
+        <v>0.27875969776002901</v>
+      </c>
+      <c r="O13">
+        <v>74.365638732910099</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>87.537646293640094</v>
       </c>
@@ -4592,8 +4703,17 @@
       <c r="K14">
         <v>73.768463850021305</v>
       </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>88.306021690368596</v>
+      </c>
+      <c r="N14">
+        <v>0.264986227652805</v>
+      </c>
+      <c r="O14">
+        <v>75.288620233535696</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87.122631072998004</v>
       </c>
@@ -4621,8 +4741,17 @@
       <c r="K15">
         <v>73.477962732315007</v>
       </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>88.014322519302297</v>
+      </c>
+      <c r="N15">
+        <v>0.26830112650344801</v>
+      </c>
+      <c r="O15">
+        <v>72.426981210708604</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.555032014846802</v>
       </c>
@@ -4650,8 +4779,17 @@
       <c r="K16">
         <v>78.990332841873098</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>87.236464023590003</v>
+      </c>
+      <c r="N16">
+        <v>0.27969539775049601</v>
+      </c>
+      <c r="O16">
+        <v>72.276866912841797</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>83.700525760650606</v>
       </c>
@@ -4679,8 +4817,17 @@
       <c r="K17">
         <v>78.900684118270803</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>87.995350360870304</v>
+      </c>
+      <c r="N17">
+        <v>0.259511783328573</v>
+      </c>
+      <c r="O17">
+        <v>70.518104314804006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>87.964522838592501</v>
       </c>
@@ -4708,8 +4855,17 @@
       <c r="K18">
         <v>74.1186909675598</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>87.542390823364201</v>
+      </c>
+      <c r="N18">
+        <v>0.28381115740686402</v>
+      </c>
+      <c r="O18">
+        <v>74.608963251113806</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>87.774801254272404</v>
       </c>
@@ -4737,8 +4893,17 @@
       <c r="K19">
         <v>79.827952384948702</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N19">
+        <v>0.30356287893547301</v>
+      </c>
+      <c r="O19">
+        <v>71.804437398910494</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>87.732112407684298</v>
       </c>
@@ -4766,8 +4931,17 @@
       <c r="K20">
         <v>80.142581701278601</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>86.833304166793795</v>
+      </c>
+      <c r="N20">
+        <v>0.28241683919118099</v>
+      </c>
+      <c r="O20">
+        <v>70.653208732604895</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>83.211988210678101</v>
       </c>
@@ -4795,8 +4969,17 @@
       <c r="K21">
         <v>78.234706163406301</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N21">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="O21">
+        <v>74.5605340003967</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>88.185071945190401</v>
       </c>
@@ -4824,8 +5007,17 @@
       <c r="K22">
         <v>75.989291429519596</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>88.595348596572805</v>
+      </c>
+      <c r="N22">
+        <v>0.256593548464145</v>
+      </c>
+      <c r="O22">
+        <v>72.6554660797119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>82.941639423370304</v>
       </c>
@@ -4853,8 +5045,17 @@
       <c r="K23">
         <v>78.745748519897404</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>88.308393955230699</v>
+      </c>
+      <c r="N23">
+        <v>0.264681673419637</v>
+      </c>
+      <c r="O23">
+        <v>72.875539779663001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>87.746340036392198</v>
       </c>
@@ -4882,8 +5083,17 @@
       <c r="K24">
         <v>78.887847423553396</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>83.292621374130206</v>
+      </c>
+      <c r="N24">
+        <v>0.283929232093865</v>
+      </c>
+      <c r="O24">
+        <v>71.4219002723693</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>82.941639423370304</v>
       </c>
@@ -4911,8 +5121,17 @@
       <c r="K25">
         <v>79.977481842041001</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>87.990605831146198</v>
+      </c>
+      <c r="N25">
+        <v>0.25927294716534</v>
+      </c>
+      <c r="O25">
+        <v>74.556910276412907</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>82.941639423370304</v>
       </c>
@@ -4940,8 +5159,17 @@
       <c r="K26">
         <v>74.751729488372803</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>88.512343168258596</v>
+      </c>
+      <c r="N26">
+        <v>0.26462417335476501</v>
+      </c>
+      <c r="O26">
+        <v>70.297173976898193</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>82.941639423370304</v>
       </c>
@@ -4969,8 +5197,17 @@
       <c r="K27">
         <v>79.983191728591905</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>87.808001041412297</v>
+      </c>
+      <c r="N27">
+        <v>0.26087337634886898</v>
+      </c>
+      <c r="O27">
+        <v>77.233538150787297</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>87.770056724548297</v>
       </c>
@@ -4998,8 +5235,17 @@
       <c r="K28">
         <v>79.043774604797306</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N28">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="O28">
+        <v>77.932897090911794</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>86.963737010955796</v>
       </c>
@@ -5027,8 +5273,17 @@
       <c r="K29">
         <v>79.591427564620901</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>87.786656618118201</v>
+      </c>
+      <c r="N29">
+        <v>0.27476585600764097</v>
+      </c>
+      <c r="O29">
+        <v>70.965582609176593</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>87.5661075115203</v>
       </c>
@@ -5056,8 +5311,17 @@
       <c r="K30">
         <v>76.579574584960895</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>88.469654321670504</v>
+      </c>
+      <c r="N30">
+        <v>0.26097718422941002</v>
+      </c>
+      <c r="O30">
+        <v>75.934179544448796</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>86.911565065383897</v>
       </c>
@@ -5085,8 +5349,17 @@
       <c r="K31">
         <v>78.583029270172105</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>87.357413768768296</v>
+      </c>
+      <c r="N31">
+        <v>0.28638225017276198</v>
+      </c>
+      <c r="O31">
+        <v>70.873831272125202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>87.355041503906193</v>
       </c>
@@ -5114,8 +5387,17 @@
       <c r="K32">
         <v>78.656756401061998</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>87.400096654891897</v>
+      </c>
+      <c r="N32">
+        <v>0.26282273293082797</v>
+      </c>
+      <c r="O32">
+        <v>70.536624431610093</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.367682695388794</v>
       </c>
@@ -5143,8 +5425,17 @@
       <c r="K33">
         <v>80.617680311203003</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>87.990605831146198</v>
+      </c>
+      <c r="N33">
+        <v>0.25526879585726803</v>
+      </c>
+      <c r="O33">
+        <v>70.537974357604895</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.713926076888995</v>
       </c>
@@ -5172,8 +5463,17 @@
       <c r="K34">
         <v>80.356753349304199</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>88.187444210052405</v>
+      </c>
+      <c r="N34">
+        <v>0.26598735865391299</v>
+      </c>
+      <c r="O34">
+        <v>74.6077942848205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>87.606424093246403</v>
       </c>
@@ -5201,8 +5501,17 @@
       <c r="K35">
         <v>80.6863050460815</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>87.928950786590505</v>
+      </c>
+      <c r="N35">
+        <v>0.258728507533112</v>
+      </c>
+      <c r="O35">
+        <v>71.2465531826019</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.611948490142794</v>
       </c>
@@ -5230,8 +5539,17 @@
       <c r="K36">
         <v>76.584472179412799</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N36">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="O36">
+        <v>70.495869398116994</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>87.509191036224294</v>
       </c>
@@ -5259,8 +5577,17 @@
       <c r="K37">
         <v>79.409518241882296</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>87.191402912139793</v>
+      </c>
+      <c r="N37">
+        <v>0.284947408038772</v>
+      </c>
+      <c r="O37">
+        <v>73.691384077072101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>82.941639423370304</v>
       </c>
@@ -5288,8 +5615,17 @@
       <c r="K38">
         <v>74.430688619613605</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>87.615907192230196</v>
+      </c>
+      <c r="N38">
+        <v>0.30869558429299998</v>
+      </c>
+      <c r="O38">
+        <v>72.077340126037598</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>87.992978096008301</v>
       </c>
@@ -5317,8 +5653,17 @@
       <c r="K39">
         <v>78.724582195281897</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>88.085472583770695</v>
+      </c>
+      <c r="N39">
+        <v>0.25281027914581999</v>
+      </c>
+      <c r="O39">
+        <v>76.662908792495699</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.402468919754</v>
       </c>
@@ -5346,8 +5691,17 @@
       <c r="K40">
         <v>78.965286254882798</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>87.236464023590003</v>
+      </c>
+      <c r="N40">
+        <v>0.29592066387937099</v>
+      </c>
+      <c r="O40">
+        <v>78.373812913894596</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.014322519302297</v>
       </c>
@@ -5375,8 +5729,17 @@
       <c r="K41">
         <v>80.286141395568805</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>87.395358085632296</v>
+      </c>
+      <c r="N41">
+        <v>0.27818662244915299</v>
+      </c>
+      <c r="O41">
+        <v>72.380852460861206</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>84.355062246322603</v>
       </c>
@@ -5404,8 +5767,17 @@
       <c r="K42">
         <v>79.297119140625</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>87.924206256866398</v>
+      </c>
+      <c r="N42">
+        <v>0.27434361932050999</v>
+      </c>
+      <c r="O42">
+        <v>72.045834302902193</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>86.766904592513995</v>
       </c>
@@ -5433,8 +5805,17 @@
       <c r="K43">
         <v>78.875142335891695</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>83.204877376556396</v>
+      </c>
+      <c r="N43">
+        <v>0.30220035082075303</v>
+      </c>
+      <c r="O43">
+        <v>75.1889808177948</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>82.941639423370304</v>
       </c>
@@ -5462,8 +5843,17 @@
       <c r="K44">
         <v>78.057503223419104</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>87.974005937576294</v>
+      </c>
+      <c r="N44">
+        <v>0.26029498222245701</v>
+      </c>
+      <c r="O44">
+        <v>71.436408996582003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -5491,8 +5881,17 @@
       <c r="K45">
         <v>78.459477186203003</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>87.767684459686194</v>
+      </c>
+      <c r="N45">
+        <v>0.27104607281253201</v>
+      </c>
+      <c r="O45">
+        <v>74.170302152633596</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>87.682312726974402</v>
       </c>
@@ -5520,8 +5919,17 @@
       <c r="K46">
         <v>78.317126512527395</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>87.800884246826101</v>
+      </c>
+      <c r="N46">
+        <v>0.26542148996487003</v>
+      </c>
+      <c r="O46">
+        <v>75.208889961242605</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>86.973226070403996</v>
       </c>
@@ -5549,8 +5957,17 @@
       <c r="K47">
         <v>80.199063062667804</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>88.147127628326402</v>
+      </c>
+      <c r="N47">
+        <v>0.28181546851739903</v>
+      </c>
+      <c r="O47">
+        <v>74.689979314804006</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>87.281525135040198</v>
       </c>
@@ -5578,8 +5995,17 @@
       <c r="K48">
         <v>77.574971914291297</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>87.587451934814396</v>
+      </c>
+      <c r="N48">
+        <v>0.27010709252139098</v>
+      </c>
+      <c r="O48">
+        <v>75.620335817336994</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>87.260180711746202</v>
       </c>
@@ -5607,8 +6033,17 @@
       <c r="K49">
         <v>80.014773368835407</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>87.653851509094196</v>
+      </c>
+      <c r="N49">
+        <v>0.268638267395235</v>
+      </c>
+      <c r="O49">
+        <v>74.735875129699707</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>82.941639423370304</v>
       </c>
@@ -5636,8 +6071,17 @@
       <c r="K50">
         <v>79.551973342895494</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>88.782697916030799</v>
+      </c>
+      <c r="N50">
+        <v>0.25336455599020902</v>
+      </c>
+      <c r="O50">
+        <v>72.200090408325195</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>87.736856937408405</v>
       </c>
@@ -5664,6 +6108,15 @@
       </c>
       <c r="K51">
         <v>79.829184055328298</v>
+      </c>
+      <c r="M51">
+        <v>87.291008234024005</v>
+      </c>
+      <c r="N51">
+        <v>0.279400984002945</v>
+      </c>
+      <c r="O51">
+        <v>74.092184543609605</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 230 packet run 2d
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195B6DBA-341A-4392-A3D0-85AE7899BAC9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50DAFE39-A86E-4790-85EF-DECE6D436316}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="11">
   <si>
     <t>Acc</t>
   </si>
@@ -4184,15 +4184,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D26FF1-09F9-44E0-BBA7-4C47B034FF96}">
-  <dimension ref="A1:S51"/>
+  <dimension ref="A1:W51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -4208,8 +4208,11 @@
       <c r="R1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -4255,8 +4258,17 @@
       <c r="S2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="U2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>87.468874454498206</v>
       </c>
@@ -4294,8 +4306,17 @@
         <v>79.981187105178805</v>
       </c>
       <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q3">
+        <v>88.412737846374498</v>
+      </c>
+      <c r="R3">
+        <v>0.264765702028815</v>
+      </c>
+      <c r="S3">
+        <v>80.053917646407996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>87.563735246658297</v>
       </c>
@@ -4332,8 +4353,17 @@
       <c r="O4">
         <v>70.9035866260528</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q4">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="R4">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="S4">
+        <v>72.853944778442298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>88.000094890594397</v>
       </c>
@@ -4370,8 +4400,17 @@
       <c r="O5">
         <v>69.936318874359102</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q5">
+        <v>84.075224399566594</v>
+      </c>
+      <c r="R5">
+        <v>0.29043662896042799</v>
+      </c>
+      <c r="S5">
+        <v>73.184900760650606</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.767684459686194</v>
       </c>
@@ -4408,8 +4447,17 @@
       <c r="O6">
         <v>76.476198911666799</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q6">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="R6">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="S6">
+        <v>72.305456638336096</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>83.306849002838106</v>
       </c>
@@ -4446,8 +4494,17 @@
       <c r="O7">
         <v>75.686116695403996</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q7">
+        <v>83.226221799850407</v>
+      </c>
+      <c r="R7">
+        <v>0.30168453050423799</v>
+      </c>
+      <c r="S7">
+        <v>73.291011810302706</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>87.162947654724107</v>
       </c>
@@ -4484,8 +4541,17 @@
       <c r="O8">
         <v>70.673139333724905</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q8">
+        <v>86.332917213439899</v>
+      </c>
+      <c r="R8">
+        <v>0.29237627452062398</v>
+      </c>
+      <c r="S8">
+        <v>73.248565196990896</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>87.698912620544405</v>
       </c>
@@ -4522,8 +4588,17 @@
       <c r="O9">
         <v>75.790327787399207</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q9">
+        <v>88.690209388732896</v>
+      </c>
+      <c r="R9">
+        <v>0.27188473447171702</v>
+      </c>
+      <c r="S9">
+        <v>73.021291494369507</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>83.330565690994206</v>
       </c>
@@ -4560,8 +4635,17 @@
       <c r="O10">
         <v>73.677732467651296</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q10">
+        <v>87.734484672546301</v>
+      </c>
+      <c r="R10">
+        <v>0.263791751192403</v>
+      </c>
+      <c r="S10">
+        <v>73.007450342178302</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>87.459385395050006</v>
       </c>
@@ -4598,8 +4682,17 @@
       <c r="O11">
         <v>72.953715562820406</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q11">
+        <v>87.900489568710299</v>
+      </c>
+      <c r="R11">
+        <v>0.26024197134928401</v>
+      </c>
+      <c r="S11">
+        <v>69.657107353210407</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>87.826973199844304</v>
       </c>
@@ -4636,8 +4729,17 @@
       <c r="O12">
         <v>77.163248062133704</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q12">
+        <v>85.071265697479205</v>
+      </c>
+      <c r="R12">
+        <v>0.31405787178449801</v>
+      </c>
+      <c r="S12">
+        <v>72.425482749938894</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>87.976378202438298</v>
       </c>
@@ -4674,8 +4776,17 @@
       <c r="O13">
         <v>74.365638732910099</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q13">
+        <v>87.957406044006305</v>
+      </c>
+      <c r="R13">
+        <v>0.265459077894315</v>
+      </c>
+      <c r="S13">
+        <v>75.334001779556203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>87.537646293640094</v>
       </c>
@@ -4712,8 +4823,17 @@
       <c r="O14">
         <v>75.288620233535696</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q14">
+        <v>87.917089462280202</v>
+      </c>
+      <c r="R14">
+        <v>0.26089043518615401</v>
+      </c>
+      <c r="S14">
+        <v>71.083654880523596</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>87.122631072998004</v>
       </c>
@@ -4750,8 +4870,17 @@
       <c r="O15">
         <v>72.426981210708604</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="Q15">
+        <v>87.615907192230196</v>
+      </c>
+      <c r="R15">
+        <v>0.28684454690901301</v>
+      </c>
+      <c r="S15">
+        <v>72.312381505966101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.555032014846802</v>
       </c>
@@ -4788,8 +4917,17 @@
       <c r="O16">
         <v>72.276866912841797</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <v>87.855434417724595</v>
+      </c>
+      <c r="R16">
+        <v>0.26828533962800399</v>
+      </c>
+      <c r="S16">
+        <v>75.232361078262301</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>83.700525760650606</v>
       </c>
@@ -4826,8 +4964,17 @@
       <c r="O17">
         <v>70.518104314804006</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>87.703657150268498</v>
+      </c>
+      <c r="R17">
+        <v>0.27761200636785699</v>
+      </c>
+      <c r="S17">
+        <v>71.242110967636094</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>87.964522838592501</v>
       </c>
@@ -4864,8 +5011,17 @@
       <c r="O18">
         <v>74.608963251113806</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q18">
+        <v>87.276780605316105</v>
+      </c>
+      <c r="R18">
+        <v>0.26761227144483102</v>
+      </c>
+      <c r="S18">
+        <v>70.763823270797701</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>87.774801254272404</v>
       </c>
@@ -4902,8 +5058,17 @@
       <c r="O19">
         <v>71.804437398910494</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q19">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="R19">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="S19">
+        <v>72.717964172363196</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>87.732112407684298</v>
       </c>
@@ -4940,8 +5105,17 @@
       <c r="O20">
         <v>70.653208732604895</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q20">
+        <v>83.283138275146399</v>
+      </c>
+      <c r="R20">
+        <v>0.30064781244692101</v>
+      </c>
+      <c r="S20">
+        <v>73.800097465515094</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>83.211988210678101</v>
       </c>
@@ -4978,8 +5152,17 @@
       <c r="O21">
         <v>74.5605340003967</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q21">
+        <v>87.060970067977905</v>
+      </c>
+      <c r="R21">
+        <v>0.29719339798510602</v>
+      </c>
+      <c r="S21">
+        <v>72.217993497848497</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>88.185071945190401</v>
       </c>
@@ -5016,8 +5199,17 @@
       <c r="O22">
         <v>72.6554660797119</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q22">
+        <v>88.296532630920396</v>
+      </c>
+      <c r="R22">
+        <v>0.25886780820845401</v>
+      </c>
+      <c r="S22">
+        <v>75.353200435638399</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>82.941639423370304</v>
       </c>
@@ -5054,8 +5246,17 @@
       <c r="O23">
         <v>72.875539779663001</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <v>87.914717197418199</v>
+      </c>
+      <c r="R23">
+        <v>0.27213141955012099</v>
+      </c>
+      <c r="S23">
+        <v>71.697496414184499</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>87.746340036392198</v>
       </c>
@@ -5092,8 +5293,17 @@
       <c r="O24">
         <v>71.4219002723693</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q24">
+        <v>86.958998441696096</v>
+      </c>
+      <c r="R24">
+        <v>0.29416847245012201</v>
+      </c>
+      <c r="S24">
+        <v>75.1012024879455</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>82.941639423370304</v>
       </c>
@@ -5130,8 +5340,17 @@
       <c r="O25">
         <v>74.556910276412907</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q25">
+        <v>88.059383630752507</v>
+      </c>
+      <c r="R25">
+        <v>0.27134637639290798</v>
+      </c>
+      <c r="S25">
+        <v>72.344587802886906</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>82.941639423370304</v>
       </c>
@@ -5168,8 +5387,17 @@
       <c r="O26">
         <v>70.297173976898193</v>
       </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q26">
+        <v>88.104444742202702</v>
+      </c>
+      <c r="R26">
+        <v>0.26532468423970001</v>
+      </c>
+      <c r="S26">
+        <v>71.357617855071993</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>82.941639423370304</v>
       </c>
@@ -5206,8 +5434,17 @@
       <c r="O27">
         <v>77.233538150787297</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q27">
+        <v>83.271276950836096</v>
+      </c>
+      <c r="R27">
+        <v>0.30881494839443802</v>
+      </c>
+      <c r="S27">
+        <v>73.223740577697697</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>87.770056724548297</v>
       </c>
@@ -5244,8 +5481,17 @@
       <c r="O28">
         <v>77.932897090911794</v>
       </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q28">
+        <v>87.760573625564504</v>
+      </c>
+      <c r="R28">
+        <v>0.27090088435611598</v>
+      </c>
+      <c r="S28">
+        <v>69.036902189254704</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>86.963737010955796</v>
       </c>
@@ -5282,8 +5528,17 @@
       <c r="O29">
         <v>70.965582609176593</v>
       </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q29">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="R29">
+        <v>0.29699016838172398</v>
+      </c>
+      <c r="S29">
+        <v>73.070634126663194</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>87.5661075115203</v>
       </c>
@@ -5320,8 +5575,17 @@
       <c r="O30">
         <v>75.934179544448796</v>
       </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q30">
+        <v>87.264925241470294</v>
+      </c>
+      <c r="R30">
+        <v>0.284858503280708</v>
+      </c>
+      <c r="S30">
+        <v>72.2075066566467</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>86.911565065383897</v>
       </c>
@@ -5358,8 +5622,17 @@
       <c r="O31">
         <v>70.873831272125202</v>
       </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q31">
+        <v>87.226980924606295</v>
+      </c>
+      <c r="R31">
+        <v>0.29508772968735603</v>
+      </c>
+      <c r="S31">
+        <v>73.820480346679602</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>87.355041503906193</v>
       </c>
@@ -5396,8 +5669,17 @@
       <c r="O32">
         <v>70.536624431610093</v>
       </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q32">
+        <v>87.430930137634206</v>
+      </c>
+      <c r="R32">
+        <v>0.30049246508136601</v>
+      </c>
+      <c r="S32">
+        <v>72.832002878189002</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.367682695388794</v>
       </c>
@@ -5434,8 +5716,17 @@
       <c r="O33">
         <v>70.537974357604895</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q33">
+        <v>87.032514810562105</v>
+      </c>
+      <c r="R33">
+        <v>0.28769832397700501</v>
+      </c>
+      <c r="S33">
+        <v>73.749711275100694</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.713926076888995</v>
       </c>
@@ -5472,8 +5763,17 @@
       <c r="O34">
         <v>74.6077942848205</v>
       </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q34">
+        <v>87.136858701705904</v>
+      </c>
+      <c r="R34">
+        <v>0.291208854473755</v>
+      </c>
+      <c r="S34">
+        <v>70.985456943511906</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>87.606424093246403</v>
       </c>
@@ -5510,8 +5810,17 @@
       <c r="O35">
         <v>71.2465531826019</v>
       </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q35">
+        <v>87.848317623138399</v>
+      </c>
+      <c r="R35">
+        <v>0.26365141086413701</v>
+      </c>
+      <c r="S35">
+        <v>75.029891729354802</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.611948490142794</v>
       </c>
@@ -5548,8 +5857,17 @@
       <c r="O36">
         <v>70.495869398116994</v>
       </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q36">
+        <v>88.607203960418701</v>
+      </c>
+      <c r="R36">
+        <v>0.25171889708067702</v>
+      </c>
+      <c r="S36">
+        <v>75.250156164169297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>87.509191036224294</v>
       </c>
@@ -5586,8 +5904,17 @@
       <c r="O37">
         <v>73.691384077072101</v>
       </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q37">
+        <v>87.162947654724107</v>
+      </c>
+      <c r="R37">
+        <v>0.27219134221932501</v>
+      </c>
+      <c r="S37">
+        <v>73.761211633682194</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>82.941639423370304</v>
       </c>
@@ -5624,8 +5951,17 @@
       <c r="O38">
         <v>72.077340126037598</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q38">
+        <v>87.051486968994098</v>
+      </c>
+      <c r="R38">
+        <v>0.28005267312842902</v>
+      </c>
+      <c r="S38">
+        <v>70.9909183979034</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>87.992978096008301</v>
       </c>
@@ -5662,8 +5998,17 @@
       <c r="O39">
         <v>76.662908792495699</v>
       </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q39">
+        <v>87.630134820938096</v>
+      </c>
+      <c r="R39">
+        <v>0.29075864017798397</v>
+      </c>
+      <c r="S39">
+        <v>73.186587095260606</v>
+      </c>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.402468919754</v>
       </c>
@@ -5700,8 +6045,17 @@
       <c r="O40">
         <v>78.373812913894596</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q40">
+        <v>88.021439313888493</v>
+      </c>
+      <c r="R40">
+        <v>0.25811993370596498</v>
+      </c>
+      <c r="S40">
+        <v>74.147364854812594</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.014322519302297</v>
       </c>
@@ -5738,8 +6092,17 @@
       <c r="O41">
         <v>72.380852460861206</v>
       </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q41">
+        <v>82.939267158508301</v>
+      </c>
+      <c r="R41">
+        <v>0.33297670761921799</v>
+      </c>
+      <c r="S41">
+        <v>72.172680377960205</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>84.355062246322603</v>
       </c>
@@ -5776,8 +6139,17 @@
       <c r="O42">
         <v>72.045834302902193</v>
       </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q42">
+        <v>87.727367877960205</v>
+      </c>
+      <c r="R42">
+        <v>0.26665605488314398</v>
+      </c>
+      <c r="S42">
+        <v>72.596275568008394</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>86.766904592513995</v>
       </c>
@@ -5814,8 +6186,17 @@
       <c r="O43">
         <v>75.1889808177948</v>
       </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q43">
+        <v>88.547915220260606</v>
+      </c>
+      <c r="R43">
+        <v>0.272359962511594</v>
+      </c>
+      <c r="S43">
+        <v>74.676091432571397</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>82.941639423370304</v>
       </c>
@@ -5852,8 +6233,17 @@
       <c r="O44">
         <v>71.436408996582003</v>
       </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q44">
+        <v>87.563735246658297</v>
+      </c>
+      <c r="R44">
+        <v>0.27786745282299602</v>
+      </c>
+      <c r="S44">
+        <v>72.845376014709402</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -5890,8 +6280,17 @@
       <c r="O45">
         <v>74.170302152633596</v>
       </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q45">
+        <v>87.784284353256197</v>
+      </c>
+      <c r="R45">
+        <v>0.28105299032230302</v>
+      </c>
+      <c r="S45">
+        <v>72.744814634323106</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>87.682312726974402</v>
       </c>
@@ -5928,8 +6327,17 @@
       <c r="O46">
         <v>75.208889961242605</v>
       </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q46">
+        <v>84.599334001541095</v>
+      </c>
+      <c r="R46">
+        <v>0.29336210926296502</v>
+      </c>
+      <c r="S46">
+        <v>72.313711166381793</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>86.973226070403996</v>
       </c>
@@ -5966,8 +6374,17 @@
       <c r="O47">
         <v>74.689979314804006</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q47">
+        <v>87.696540355682302</v>
+      </c>
+      <c r="R47">
+        <v>0.26635324594339999</v>
+      </c>
+      <c r="S47">
+        <v>71.462985992431598</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>87.281525135040198</v>
       </c>
@@ -6004,8 +6421,17 @@
       <c r="O48">
         <v>75.620335817336994</v>
       </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q48">
+        <v>86.5155220031738</v>
+      </c>
+      <c r="R48">
+        <v>0.28276195560040801</v>
+      </c>
+      <c r="S48">
+        <v>71.436714410781804</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>87.260180711746202</v>
       </c>
@@ -6042,8 +6468,17 @@
       <c r="O49">
         <v>74.735875129699707</v>
       </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q49">
+        <v>87.554246187209998</v>
+      </c>
+      <c r="R49">
+        <v>0.27109047767019301</v>
+      </c>
+      <c r="S49">
+        <v>71.229358673095703</v>
+      </c>
+    </row>
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>82.941639423370304</v>
       </c>
@@ -6080,8 +6515,17 @@
       <c r="O50">
         <v>72.200090408325195</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q50">
+        <v>83.828586339950505</v>
+      </c>
+      <c r="R50">
+        <v>0.32420824389931802</v>
+      </c>
+      <c r="S50">
+        <v>71.258295536041203</v>
+      </c>
+    </row>
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>87.736856937408405</v>
       </c>
@@ -6118,8 +6562,18 @@
       <c r="O51">
         <v>74.092184543609605</v>
       </c>
+      <c r="Q51">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="R51">
+        <v>0.336088248761089</v>
+      </c>
+      <c r="S51">
+        <v>69.337912321090698</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 200 Packet Run 2D
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78753D53-9BF9-4F02-A6AD-3E3DD3C5D2E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF303BC-8227-42A8-B79D-C78C7DA0CFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="2550" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1110" yWindow="2190" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN 1D" sheetId="1" r:id="rId1"/>
@@ -4187,7 +4187,7 @@
   <dimension ref="A1:AA51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="AA2" sqref="AA2"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4336,6 +4336,15 @@
       <c r="W3">
         <v>74.316713571548405</v>
       </c>
+      <c r="Y3">
+        <v>88.130527734756399</v>
+      </c>
+      <c r="Z3">
+        <v>0.27344635745206602</v>
+      </c>
+      <c r="AA3">
+        <v>67.290010929107595</v>
+      </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -4392,6 +4401,15 @@
       <c r="W4">
         <v>69.506042003631507</v>
       </c>
+      <c r="Y4">
+        <v>88.920247554778996</v>
+      </c>
+      <c r="Z4">
+        <v>0.25774980586164398</v>
+      </c>
+      <c r="AA4">
+        <v>66.396825075149494</v>
+      </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -4448,6 +4466,15 @@
       <c r="W5">
         <v>69.852652549743596</v>
       </c>
+      <c r="Y5">
+        <v>83.821469545364295</v>
+      </c>
+      <c r="Z5">
+        <v>0.297402189457594</v>
+      </c>
+      <c r="AA5">
+        <v>65.558467149734497</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -4504,6 +4531,15 @@
       <c r="W6">
         <v>64.877549886703406</v>
       </c>
+      <c r="Y6">
+        <v>87.620651721954303</v>
+      </c>
+      <c r="Z6">
+        <v>0.28040545287405499</v>
+      </c>
+      <c r="AA6">
+        <v>65.826833248138399</v>
+      </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -4560,6 +4596,15 @@
       <c r="W7">
         <v>65.772783041000295</v>
       </c>
+      <c r="Y7">
+        <v>87.561362981796194</v>
+      </c>
+      <c r="Z7">
+        <v>0.29203820308600498</v>
+      </c>
+      <c r="AA7">
+        <v>65.761678695678697</v>
+      </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -4616,6 +4661,15 @@
       <c r="W8">
         <v>67.877670288085895</v>
       </c>
+      <c r="Y8">
+        <v>83.892619609832707</v>
+      </c>
+      <c r="Z8">
+        <v>0.288058755348577</v>
+      </c>
+      <c r="AA8">
+        <v>65.0974698066711</v>
+      </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -4672,6 +4726,15 @@
       <c r="W9">
         <v>70.144351720809894</v>
       </c>
+      <c r="Y9">
+        <v>88.011950254440293</v>
+      </c>
+      <c r="Z9">
+        <v>0.26516301425847799</v>
+      </c>
+      <c r="AA9">
+        <v>61.287345170974703</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -4728,6 +4791,15 @@
       <c r="W10">
         <v>70.288437843322697</v>
       </c>
+      <c r="Y10">
+        <v>87.803256511688204</v>
+      </c>
+      <c r="Z10">
+        <v>0.27637953875471399</v>
+      </c>
+      <c r="AA10">
+        <v>61.200113534927297</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -4784,6 +4856,15 @@
       <c r="W11">
         <v>67.8787970542907</v>
       </c>
+      <c r="Y11">
+        <v>87.563735246658297</v>
+      </c>
+      <c r="Z11">
+        <v>0.28503508429721502</v>
+      </c>
+      <c r="AA11">
+        <v>66.596321582794104</v>
+      </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -4840,6 +4921,15 @@
       <c r="W12">
         <v>70.629859924316406</v>
       </c>
+      <c r="Y12">
+        <v>87.203264236450195</v>
+      </c>
+      <c r="Z12">
+        <v>0.28297697417776302</v>
+      </c>
+      <c r="AA12">
+        <v>64.106638193130493</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -4896,6 +4986,15 @@
       <c r="W13">
         <v>66.259264707565293</v>
       </c>
+      <c r="Y13">
+        <v>87.947922945022498</v>
+      </c>
+      <c r="Z13">
+        <v>0.26649139156371499</v>
+      </c>
+      <c r="AA13">
+        <v>64.160237550735403</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -4952,6 +5051,15 @@
       <c r="W14">
         <v>68.587527990341101</v>
       </c>
+      <c r="Y14">
+        <v>88.524198532104407</v>
+      </c>
+      <c r="Z14">
+        <v>0.26339664288289399</v>
+      </c>
+      <c r="AA14">
+        <v>61.358152866363497</v>
+      </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -5008,6 +5116,15 @@
       <c r="W15">
         <v>69.465696811675997</v>
       </c>
+      <c r="Y15">
+        <v>83.712381124496403</v>
+      </c>
+      <c r="Z15">
+        <v>0.28441361926408898</v>
+      </c>
+      <c r="AA15">
+        <v>65.032004833221393</v>
+      </c>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -5064,8 +5181,17 @@
       <c r="W16">
         <v>69.229522228240896</v>
       </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y16">
+        <v>83.736097812652503</v>
+      </c>
+      <c r="Z16">
+        <v>0.28139868792735001</v>
+      </c>
+      <c r="AA16">
+        <v>65.463674068450899</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>83.700525760650606</v>
       </c>
@@ -5120,8 +5246,17 @@
       <c r="W17">
         <v>65.322001218795705</v>
       </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y17">
+        <v>87.848317623138399</v>
+      </c>
+      <c r="Z17">
+        <v>0.26422198295238403</v>
+      </c>
+      <c r="AA17">
+        <v>66.049296617507906</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>87.964522838592501</v>
       </c>
@@ -5176,8 +5311,17 @@
       <c r="W18">
         <v>68.409426212310706</v>
       </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y18">
+        <v>83.264166116714406</v>
+      </c>
+      <c r="Z18">
+        <v>0.30746913967835998</v>
+      </c>
+      <c r="AA18">
+        <v>61.688814640045102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>87.774801254272404</v>
       </c>
@@ -5232,8 +5376,17 @@
       <c r="W19">
         <v>69.898846149444495</v>
       </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y19">
+        <v>86.653071641921997</v>
+      </c>
+      <c r="Z19">
+        <v>0.29631816906081898</v>
+      </c>
+      <c r="AA19">
+        <v>65.205819129943805</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>87.732112407684298</v>
       </c>
@@ -5288,8 +5441,17 @@
       <c r="W20">
         <v>69.131679534912095</v>
       </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y20">
+        <v>88.711553812026906</v>
+      </c>
+      <c r="Z20">
+        <v>0.26160770693638902</v>
+      </c>
+      <c r="AA20">
+        <v>66.543475866317706</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>83.211988210678101</v>
       </c>
@@ -5344,8 +5506,17 @@
       <c r="W21">
         <v>70.083317041397095</v>
       </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y21">
+        <v>87.089431285858097</v>
+      </c>
+      <c r="Z21">
+        <v>0.29469060519281698</v>
+      </c>
+      <c r="AA21">
+        <v>67.582562446594196</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>88.185071945190401</v>
       </c>
@@ -5400,8 +5571,17 @@
       <c r="W22">
         <v>69.007638454437199</v>
       </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y22">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="Z22">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="AA22">
+        <v>67.450929641723604</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>82.941639423370304</v>
       </c>
@@ -5456,8 +5636,17 @@
       <c r="W23">
         <v>69.852119445800696</v>
       </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y23">
+        <v>87.440413236617999</v>
+      </c>
+      <c r="Z23">
+        <v>0.26581365415767599</v>
+      </c>
+      <c r="AA23">
+        <v>67.692631244659395</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>87.746340036392198</v>
       </c>
@@ -5512,8 +5701,17 @@
       <c r="W24">
         <v>70.281395912170396</v>
       </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y24">
+        <v>87.053859233856201</v>
+      </c>
+      <c r="Z24">
+        <v>0.327350065479457</v>
+      </c>
+      <c r="AA24">
+        <v>67.456271886825505</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>82.941639423370304</v>
       </c>
@@ -5568,8 +5766,17 @@
       <c r="W25">
         <v>64.9467613697052</v>
       </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y25">
+        <v>88.417482376098604</v>
+      </c>
+      <c r="Z25">
+        <v>0.249481786307755</v>
+      </c>
+      <c r="AA25">
+        <v>64.375463724136296</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>82.941639423370304</v>
       </c>
@@ -5624,8 +5831,17 @@
       <c r="W26">
         <v>68.834173202514606</v>
       </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y26">
+        <v>87.826973199844304</v>
+      </c>
+      <c r="Z26">
+        <v>0.271586461314759</v>
+      </c>
+      <c r="AA26">
+        <v>60.734239101409898</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>82.941639423370304</v>
       </c>
@@ -5680,8 +5896,17 @@
       <c r="W27">
         <v>68.769514560699406</v>
       </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y27">
+        <v>86.980342864990206</v>
+      </c>
+      <c r="Z27">
+        <v>0.29200259537853901</v>
+      </c>
+      <c r="AA27">
+        <v>66.988158702850299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>87.770056724548297</v>
       </c>
@@ -5736,8 +5961,17 @@
       <c r="W28">
         <v>68.027851343154893</v>
       </c>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y28">
+        <v>87.817490100860596</v>
+      </c>
+      <c r="Z28">
+        <v>0.25658139156344401</v>
+      </c>
+      <c r="AA28">
+        <v>61.1500530242919</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>86.963737010955796</v>
       </c>
@@ -5792,8 +6026,17 @@
       <c r="W29">
         <v>71.526809930801306</v>
       </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y29">
+        <v>88.464915752410803</v>
+      </c>
+      <c r="Z29">
+        <v>0.25718509018241598</v>
+      </c>
+      <c r="AA29">
+        <v>60.492553949356001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>87.5661075115203</v>
       </c>
@@ -5848,8 +6091,17 @@
       <c r="W30">
         <v>65.306699991226196</v>
       </c>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y30">
+        <v>87.881517410278306</v>
+      </c>
+      <c r="Z30">
+        <v>0.26282472246713801</v>
+      </c>
+      <c r="AA30">
+        <v>66.510779142379704</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>86.911565065383897</v>
       </c>
@@ -5904,8 +6156,17 @@
       <c r="W31">
         <v>70.745268821716294</v>
       </c>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y31">
+        <v>87.762939929962101</v>
+      </c>
+      <c r="Z31">
+        <v>0.27445424753006098</v>
+      </c>
+      <c r="AA31">
+        <v>66.378743171691895</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>87.355041503906193</v>
       </c>
@@ -5960,8 +6221,17 @@
       <c r="W32">
         <v>65.823185205459595</v>
       </c>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y32">
+        <v>86.747932434082003</v>
+      </c>
+      <c r="Z32">
+        <v>0.29183078213038699</v>
+      </c>
+      <c r="AA32">
+        <v>61.351038455963099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>88.367682695388794</v>
       </c>
@@ -6016,8 +6286,17 @@
       <c r="W33">
         <v>68.772596836090003</v>
       </c>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y33">
+        <v>87.698912620544405</v>
+      </c>
+      <c r="Z33">
+        <v>0.273095712291332</v>
+      </c>
+      <c r="AA33">
+        <v>66.023054361343299</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.713926076888995</v>
       </c>
@@ -6072,8 +6351,17 @@
       <c r="W34">
         <v>68.517350912094102</v>
       </c>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y34">
+        <v>88.0166947841644</v>
+      </c>
+      <c r="Z34">
+        <v>0.25742864137367399</v>
+      </c>
+      <c r="AA34">
+        <v>67.002029418945298</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>87.606424093246403</v>
       </c>
@@ -6128,8 +6416,17 @@
       <c r="W35">
         <v>66.560115575790405</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y35">
+        <v>88.078355789184499</v>
+      </c>
+      <c r="Z35">
+        <v>0.25665540870306502</v>
+      </c>
+      <c r="AA35">
+        <v>61.413606643676701</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.611948490142794</v>
       </c>
@@ -6184,8 +6481,17 @@
       <c r="W36">
         <v>67.782172918319702</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y36">
+        <v>87.722629308700505</v>
+      </c>
+      <c r="Z36">
+        <v>0.25741935373843799</v>
+      </c>
+      <c r="AA36">
+        <v>67.168449163436804</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>87.509191036224294</v>
       </c>
@@ -6240,8 +6546,17 @@
       <c r="W37">
         <v>67.162470102310095</v>
       </c>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y37">
+        <v>83.209615945815997</v>
+      </c>
+      <c r="Z37">
+        <v>0.328430703784232</v>
+      </c>
+      <c r="AA37">
+        <v>66.8585751056671</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>82.941639423370304</v>
       </c>
@@ -6296,8 +6611,17 @@
       <c r="W38">
         <v>69.233812570571899</v>
       </c>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y38">
+        <v>87.698912620544405</v>
+      </c>
+      <c r="Z38">
+        <v>0.27151091939571698</v>
+      </c>
+      <c r="AA38">
+        <v>67.386412620544405</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>87.992978096008301</v>
       </c>
@@ -6352,8 +6676,17 @@
       <c r="W39">
         <v>66.373887062072697</v>
       </c>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y39">
+        <v>87.241208553314195</v>
+      </c>
+      <c r="Z39">
+        <v>0.26767146111504297</v>
+      </c>
+      <c r="AA39">
+        <v>63.078752994537297</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.402468919754</v>
       </c>
@@ -6408,8 +6741,17 @@
       <c r="W40">
         <v>68.996634244918795</v>
       </c>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y40">
+        <v>87.696540355682302</v>
+      </c>
+      <c r="Z40">
+        <v>0.29575851041206302</v>
+      </c>
+      <c r="AA40">
+        <v>66.118104219436603</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.014322519302297</v>
       </c>
@@ -6464,8 +6806,17 @@
       <c r="W41">
         <v>69.872815847396794</v>
       </c>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y41">
+        <v>88.147127628326402</v>
+      </c>
+      <c r="Z41">
+        <v>0.268626176879037</v>
+      </c>
+      <c r="AA41">
+        <v>60.746504306793199</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>84.355062246322603</v>
       </c>
@@ -6520,8 +6871,17 @@
       <c r="W42">
         <v>69.376658678054795</v>
       </c>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y42">
+        <v>83.366137742996202</v>
+      </c>
+      <c r="Z42">
+        <v>0.31244047473066799</v>
+      </c>
+      <c r="AA42">
+        <v>66.8369717597961</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>86.766904592513995</v>
       </c>
@@ -6576,8 +6936,17 @@
       <c r="W43">
         <v>68.154401540756197</v>
       </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y43">
+        <v>84.260201454162598</v>
+      </c>
+      <c r="Z43">
+        <v>0.28698463674673402</v>
+      </c>
+      <c r="AA43">
+        <v>66.3361496925354</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>82.941639423370304</v>
       </c>
@@ -6632,8 +7001,17 @@
       <c r="W44">
         <v>70.136420249938894</v>
       </c>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y44">
+        <v>87.623023986816406</v>
+      </c>
+      <c r="Z44">
+        <v>0.26719601728273101</v>
+      </c>
+      <c r="AA44">
+        <v>61.371240615844698</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -6688,8 +7066,17 @@
       <c r="W45">
         <v>68.698766469955402</v>
       </c>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y45">
+        <v>88.657009601593003</v>
+      </c>
+      <c r="Z45">
+        <v>0.25705344326551899</v>
+      </c>
+      <c r="AA45">
+        <v>64.951596975326495</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>87.682312726974402</v>
       </c>
@@ -6744,8 +7131,17 @@
       <c r="W46">
         <v>69.543472051620398</v>
       </c>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y46">
+        <v>87.577962875366197</v>
+      </c>
+      <c r="Z46">
+        <v>0.276600441735673</v>
+      </c>
+      <c r="AA46">
+        <v>60.868054389953599</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>86.973226070403996</v>
       </c>
@@ -6800,8 +7196,17 @@
       <c r="W47">
         <v>69.951856374740601</v>
       </c>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y47">
+        <v>87.224608659744206</v>
+      </c>
+      <c r="Z47">
+        <v>0.264391790864409</v>
+      </c>
+      <c r="AA47">
+        <v>66.776542425155597</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>87.281525135040198</v>
       </c>
@@ -6856,8 +7261,17 @@
       <c r="W48">
         <v>69.610427856445298</v>
       </c>
-    </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y48">
+        <v>86.629354953765798</v>
+      </c>
+      <c r="Z48">
+        <v>0.30728197478090602</v>
+      </c>
+      <c r="AA48">
+        <v>65.724978685379</v>
+      </c>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>87.260180711746202</v>
       </c>
@@ -6912,8 +7326,17 @@
       <c r="W49">
         <v>66.058926343917804</v>
       </c>
-    </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y49">
+        <v>87.684684991836505</v>
+      </c>
+      <c r="Z49">
+        <v>0.28741314188365003</v>
+      </c>
+      <c r="AA49">
+        <v>66.127233982086096</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>82.941639423370304</v>
       </c>
@@ -6968,8 +7391,17 @@
       <c r="W50">
         <v>70.269962549209595</v>
       </c>
-    </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="Y50">
+        <v>87.649106979370103</v>
+      </c>
+      <c r="Z50">
+        <v>0.30061774726076301</v>
+      </c>
+      <c r="AA50">
+        <v>64.955434799194293</v>
+      </c>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>87.736856937408405</v>
       </c>
@@ -7023,6 +7455,15 @@
       </c>
       <c r="W51">
         <v>64.490930795669499</v>
+      </c>
+      <c r="Y51">
+        <v>88.358193635940495</v>
+      </c>
+      <c r="Z51">
+        <v>0.26374111377715398</v>
+      </c>
+      <c r="AA51">
+        <v>61.443469762802103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 298 Packet run mw !D
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF303BC-8227-42A8-B79D-C78C7DA0CFB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DC46FB-5424-4EF1-B3F0-B407757C804E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1110" yWindow="2190" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CNN 1D" sheetId="1" r:id="rId1"/>
     <sheet name="CNN 2D" sheetId="2" r:id="rId2"/>
+    <sheet name="MW CNN 1D" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="12">
   <si>
     <t>Acc</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>200 Packets</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time</t>
   </si>
 </sst>
 </file>
@@ -4186,7 +4190,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61D26FF1-09F9-44E0-BBA7-4C47B034FF96}">
   <dimension ref="A1:AA51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
@@ -7470,4 +7474,587 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A06EE43-A370-47E6-9A9B-D644A56FBF0A}">
+  <dimension ref="A1:G51"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>89.899682998657198</v>
+      </c>
+      <c r="B3">
+        <v>0.25593475341601801</v>
+      </c>
+      <c r="C3">
+        <v>629.61373281478802</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>89.669644832610999</v>
+      </c>
+      <c r="B4">
+        <v>0.27932078153680101</v>
+      </c>
+      <c r="C4">
+        <v>620.31075048446598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>87.739229202270494</v>
+      </c>
+      <c r="B5">
+        <v>0.27616908617080299</v>
+      </c>
+      <c r="C5">
+        <v>622.61563682556096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>87.928950786590505</v>
+      </c>
+      <c r="B6">
+        <v>0.30643616261680501</v>
+      </c>
+      <c r="C6">
+        <v>620.07716345787003</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>87.656223773956299</v>
+      </c>
+      <c r="B7">
+        <v>0.32576677804585602</v>
+      </c>
+      <c r="C7">
+        <v>623.313329219818</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>89.000874757766695</v>
+      </c>
+      <c r="B8">
+        <v>0.25954075623456002</v>
+      </c>
+      <c r="C8">
+        <v>620.18612217903103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>89.169257879257202</v>
+      </c>
+      <c r="B9">
+        <v>0.25807979315569501</v>
+      </c>
+      <c r="C9">
+        <v>623.250921487808</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>89.216685295104895</v>
+      </c>
+      <c r="B10">
+        <v>0.25581393391264901</v>
+      </c>
+      <c r="C10">
+        <v>622.42791533470097</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>89.356607198715196</v>
+      </c>
+      <c r="B11">
+        <v>0.25247172338670998</v>
+      </c>
+      <c r="C11">
+        <v>621.18253993988003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>88.744753599166799</v>
+      </c>
+      <c r="B12">
+        <v>0.24845205380204</v>
+      </c>
+      <c r="C12">
+        <v>623.61626076698303</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>88.946330547332707</v>
+      </c>
+      <c r="B13">
+        <v>0.27470413344004901</v>
+      </c>
+      <c r="C13">
+        <v>619.62087702751103</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>88.317877054214406</v>
+      </c>
+      <c r="B14">
+        <v>0.29265578793354702</v>
+      </c>
+      <c r="C14">
+        <v>621.20873451232899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>89.446723461151095</v>
+      </c>
+      <c r="B15">
+        <v>0.25481620887200901</v>
+      </c>
+      <c r="C15">
+        <v>622.78855776786804</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>88.227760791778493</v>
+      </c>
+      <c r="B16">
+        <v>0.27021681278103599</v>
+      </c>
+      <c r="C16">
+        <v>620.91040968894902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>89.000874757766695</v>
+      </c>
+      <c r="B17">
+        <v>0.25701161256516702</v>
+      </c>
+      <c r="C17">
+        <v>619.70832848548798</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>89.211940765380803</v>
+      </c>
+      <c r="B18">
+        <v>0.253373333388688</v>
+      </c>
+      <c r="C18">
+        <v>622.00117516517605</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>88.251477479934593</v>
+      </c>
+      <c r="B19">
+        <v>0.27868630412323597</v>
+      </c>
+      <c r="C19">
+        <v>622.52004361152603</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>88.075983524322496</v>
+      </c>
+      <c r="B20">
+        <v>0.30781715617771499</v>
+      </c>
+      <c r="C20">
+        <v>620.82996916770901</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>88.993763923645005</v>
+      </c>
+      <c r="B21">
+        <v>0.25344664179127702</v>
+      </c>
+      <c r="C21">
+        <v>620.46274471282902</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>87.331324815750094</v>
+      </c>
+      <c r="B22">
+        <v>0.30415420046414798</v>
+      </c>
+      <c r="C22">
+        <v>625.07487797737099</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>87.447530031204195</v>
+      </c>
+      <c r="B23">
+        <v>0.30682559471366999</v>
+      </c>
+      <c r="C23">
+        <v>620.61193203925995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>88.287049531936603</v>
+      </c>
+      <c r="B24">
+        <v>0.27912531950338199</v>
+      </c>
+      <c r="C24">
+        <v>621.68988919258095</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>89.098107814788804</v>
+      </c>
+      <c r="B25">
+        <v>0.25731988630920799</v>
+      </c>
+      <c r="C25">
+        <v>620.42281103134098</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>88.135272264480506</v>
+      </c>
+      <c r="B26">
+        <v>0.29874858677112998</v>
+      </c>
+      <c r="C26">
+        <v>625.19871401786804</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>88.334476947784395</v>
+      </c>
+      <c r="B27">
+        <v>0.28577206744850697</v>
+      </c>
+      <c r="C27">
+        <v>621.87540721893299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>89.361351728439303</v>
+      </c>
+      <c r="B28">
+        <v>0.24558426476231299</v>
+      </c>
+      <c r="C28">
+        <v>624.073350429534</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>89.306801557540894</v>
+      </c>
+      <c r="B29">
+        <v>0.25280046165144898</v>
+      </c>
+      <c r="C29">
+        <v>625.62148094177201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>88.315504789352403</v>
+      </c>
+      <c r="B30">
+        <v>0.27090228943310002</v>
+      </c>
+      <c r="C30">
+        <v>622.66134953498795</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>87.895745038986206</v>
+      </c>
+      <c r="B31">
+        <v>0.28100848707252302</v>
+      </c>
+      <c r="C31">
+        <v>622.57876133918705</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>88.747125864028902</v>
+      </c>
+      <c r="B32">
+        <v>0.27410961023838198</v>
+      </c>
+      <c r="C32">
+        <v>622.42392969131402</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>89.370834827423096</v>
+      </c>
+      <c r="B33">
+        <v>0.26262793515588601</v>
+      </c>
+      <c r="C33">
+        <v>622.95025801658596</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>88.737636804580603</v>
+      </c>
+      <c r="B34">
+        <v>0.27065842287150599</v>
+      </c>
+      <c r="C34">
+        <v>621.00262737274102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>88.389027118682804</v>
+      </c>
+      <c r="B35">
+        <v>0.28455346995084202</v>
+      </c>
+      <c r="C35">
+        <v>619.62267351150501</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>88.268077373504596</v>
+      </c>
+      <c r="B36">
+        <v>0.28403646209373001</v>
+      </c>
+      <c r="C36">
+        <v>622.44991159438996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>88.8846755027771</v>
+      </c>
+      <c r="B37">
+        <v>0.259713368020911</v>
+      </c>
+      <c r="C37">
+        <v>625.08124709129299</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>87.741601467132497</v>
+      </c>
+      <c r="B38">
+        <v>0.286458535266501</v>
+      </c>
+      <c r="C38">
+        <v>623.22033381462097</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>89.309173822402897</v>
+      </c>
+      <c r="B39">
+        <v>0.25667114041414002</v>
+      </c>
+      <c r="C39">
+        <v>619.80937767028797</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>87.722629308700505</v>
+      </c>
+      <c r="B40">
+        <v>0.32560889764015499</v>
+      </c>
+      <c r="C40">
+        <v>624.04310846328701</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>88.891786336898804</v>
+      </c>
+      <c r="B41">
+        <v>0.28413221820336199</v>
+      </c>
+      <c r="C41">
+        <v>622.62831640243496</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>88.922619819641099</v>
+      </c>
+      <c r="B42">
+        <v>0.26338667526728399</v>
+      </c>
+      <c r="C42">
+        <v>623.05654406547501</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>88.509970903396606</v>
+      </c>
+      <c r="B43">
+        <v>0.26999710821183998</v>
+      </c>
+      <c r="C43">
+        <v>622.40083050727799</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>89.057791233062702</v>
+      </c>
+      <c r="B44">
+        <v>0.25949050475079799</v>
+      </c>
+      <c r="C44">
+        <v>621.44749498367298</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="B45">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="C45">
+        <v>620.072613477706</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>89.072024822235093</v>
+      </c>
+      <c r="B46">
+        <v>0.258677962333</v>
+      </c>
+      <c r="C46">
+        <v>624.22593569755497</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>88.782697916030799</v>
+      </c>
+      <c r="B47">
+        <v>0.27610162069314398</v>
+      </c>
+      <c r="C47">
+        <v>621.95561194419804</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>88.906013965606604</v>
+      </c>
+      <c r="B48">
+        <v>0.26900770298879201</v>
+      </c>
+      <c r="C48">
+        <v>620.71887111663796</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>88.336849212646399</v>
+      </c>
+      <c r="B49">
+        <v>0.28707863962150998</v>
+      </c>
+      <c r="C49">
+        <v>621.87014770507801</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>88.206416368484497</v>
+      </c>
+      <c r="B50">
+        <v>0.27207447418147801</v>
+      </c>
+      <c r="C50">
+        <v>619.91724228858902</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>88.097327947616506</v>
+      </c>
+      <c r="B51">
+        <v>0.27564597893096798</v>
+      </c>
+      <c r="C51">
+        <v>624.51877474784806</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added 290 Packet run MW 1d
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DC46FB-5424-4EF1-B3F0-B407757C804E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA53E2F-C786-4175-8FE1-4F5971AEC8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="12">
   <si>
     <t>Acc</t>
   </si>
@@ -7478,23 +7478,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A06EE43-A370-47E6-9A9B-D644A56FBF0A}">
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7513,8 +7516,17 @@
       <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.899682998657198</v>
       </c>
@@ -7524,8 +7536,17 @@
       <c r="C3">
         <v>629.61373281478802</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>89.147913455963106</v>
+      </c>
+      <c r="F3">
+        <v>0.26857903370728298</v>
+      </c>
+      <c r="G3">
+        <v>603.068132162094</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>89.669644832610999</v>
       </c>
@@ -7535,8 +7556,17 @@
       <c r="C4">
         <v>620.31075048446598</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>89.150285720825195</v>
+      </c>
+      <c r="F4">
+        <v>0.248842758329333</v>
+      </c>
+      <c r="G4">
+        <v>594.46053647994995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>87.739229202270494</v>
       </c>
@@ -7546,8 +7576,17 @@
       <c r="C5">
         <v>622.61563682556096</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>89.007991552352905</v>
+      </c>
+      <c r="F5">
+        <v>0.25321479901417998</v>
+      </c>
+      <c r="G5">
+        <v>595.02324151992798</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.928950786590505</v>
       </c>
@@ -7557,8 +7596,17 @@
       <c r="C6">
         <v>620.07716345787003</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>89.204829931259098</v>
+      </c>
+      <c r="F6">
+        <v>0.26044764199624498</v>
+      </c>
+      <c r="G6">
+        <v>596.55497908592201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>87.656223773956299</v>
       </c>
@@ -7568,8 +7616,17 @@
       <c r="C7">
         <v>623.313329219818</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>88.097327947616506</v>
+      </c>
+      <c r="F7">
+        <v>0.28145703729974902</v>
+      </c>
+      <c r="G7">
+        <v>598.80659556388798</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>89.000874757766695</v>
       </c>
@@ -7579,8 +7636,17 @@
       <c r="C8">
         <v>620.18612217903103</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>88.820642232894897</v>
+      </c>
+      <c r="F8">
+        <v>0.2569100149945</v>
+      </c>
+      <c r="G8">
+        <v>597.05055975914001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.169257879257202</v>
       </c>
@@ -7590,8 +7656,17 @@
       <c r="C9">
         <v>623.250921487808</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>89.361351728439303</v>
+      </c>
+      <c r="F9">
+        <v>0.24868068436680699</v>
+      </c>
+      <c r="G9">
+        <v>597.54162454605103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.216685295104895</v>
       </c>
@@ -7601,8 +7676,17 @@
       <c r="C10">
         <v>622.42791533470097</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>89.840394258499103</v>
+      </c>
+      <c r="F10">
+        <v>0.254047972597995</v>
+      </c>
+      <c r="G10">
+        <v>594.49819874763398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.356607198715196</v>
       </c>
@@ -7612,8 +7696,17 @@
       <c r="C11">
         <v>621.18253993988003</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>89.126569032668996</v>
+      </c>
+      <c r="F11">
+        <v>0.24492994293838699</v>
+      </c>
+      <c r="G11">
+        <v>626.51882672309796</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>88.744753599166799</v>
       </c>
@@ -7623,8 +7716,17 @@
       <c r="C12">
         <v>623.61626076698303</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>89.093369245529104</v>
+      </c>
+      <c r="F12">
+        <v>0.264490755426184</v>
+      </c>
+      <c r="G12">
+        <v>622.97183203697205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>88.946330547332707</v>
       </c>
@@ -7634,8 +7736,17 @@
       <c r="C13">
         <v>619.62087702751103</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>88.7352645397186</v>
+      </c>
+      <c r="F13">
+        <v>0.26715121349469001</v>
+      </c>
+      <c r="G13">
+        <v>626.605017662048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>88.317877054214406</v>
       </c>
@@ -7645,8 +7756,17 @@
       <c r="C14">
         <v>621.20873451232899</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>88.550287485122595</v>
+      </c>
+      <c r="F14">
+        <v>0.25549109000405601</v>
+      </c>
+      <c r="G14">
+        <v>621.65510725975003</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.446723461151095</v>
       </c>
@@ -7656,8 +7776,17 @@
       <c r="C15">
         <v>622.78855776786804</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>87.855434417724595</v>
+      </c>
+      <c r="F15">
+        <v>0.31578386592705798</v>
+      </c>
+      <c r="G15">
+        <v>625.92930412292401</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.227760791778493</v>
       </c>
@@ -7667,8 +7796,17 @@
       <c r="C16">
         <v>620.91040968894902</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>87.691795825958195</v>
+      </c>
+      <c r="F16">
+        <v>0.29081200122031697</v>
+      </c>
+      <c r="G16">
+        <v>624.45639634132306</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.000874757766695</v>
       </c>
@@ -7678,8 +7816,17 @@
       <c r="C17">
         <v>619.70832848548798</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>89.162141084671006</v>
+      </c>
+      <c r="F17">
+        <v>0.254558706449942</v>
+      </c>
+      <c r="G17">
+        <v>624.07658600807099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.211940765380803</v>
       </c>
@@ -7689,8 +7836,17 @@
       <c r="C18">
         <v>622.00117516517605</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>88.204044103622394</v>
+      </c>
+      <c r="F18">
+        <v>0.28474434469498799</v>
+      </c>
+      <c r="G18">
+        <v>597.86826133728005</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>88.251477479934593</v>
       </c>
@@ -7700,8 +7856,17 @@
       <c r="C19">
         <v>622.52004361152603</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>88.955819606781006</v>
+      </c>
+      <c r="F19">
+        <v>0.27045019738305198</v>
+      </c>
+      <c r="G19">
+        <v>600.72510051727295</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>88.075983524322496</v>
       </c>
@@ -7711,8 +7876,17 @@
       <c r="C20">
         <v>620.82996916770901</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>89.138424396514793</v>
+      </c>
+      <c r="F20">
+        <v>0.26071879735326098</v>
+      </c>
+      <c r="G20">
+        <v>594.50169444084099</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>88.993763923645005</v>
       </c>
@@ -7722,8 +7896,17 @@
       <c r="C21">
         <v>620.46274471282902</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>88.4388267993927</v>
+      </c>
+      <c r="F21">
+        <v>0.272076325806687</v>
+      </c>
+      <c r="G21">
+        <v>597.10161566734303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>87.331324815750094</v>
       </c>
@@ -7733,8 +7916,17 @@
       <c r="C22">
         <v>625.07487797737099</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>88.981902599334703</v>
+      </c>
+      <c r="F22">
+        <v>0.28059903449910301</v>
+      </c>
+      <c r="G22">
+        <v>599.09105467796303</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>87.447530031204195</v>
       </c>
@@ -7744,8 +7936,17 @@
       <c r="C23">
         <v>620.61193203925995</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>89.038819074630695</v>
+      </c>
+      <c r="F23">
+        <v>0.27318828151923003</v>
+      </c>
+      <c r="G23">
+        <v>598.84158515930096</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.287049531936603</v>
       </c>
@@ -7755,8 +7956,17 @@
       <c r="C24">
         <v>621.68988919258095</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>87.966895103454505</v>
+      </c>
+      <c r="F24">
+        <v>0.30326147420745198</v>
+      </c>
+      <c r="G24">
+        <v>595.70589900016705</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>89.098107814788804</v>
       </c>
@@ -7766,8 +7976,17 @@
       <c r="C25">
         <v>620.42281103134098</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>88.158988952636705</v>
+      </c>
+      <c r="F25">
+        <v>0.26622943177910702</v>
+      </c>
+      <c r="G25">
+        <v>597.52832674980095</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>88.135272264480506</v>
       </c>
@@ -7777,8 +7996,17 @@
       <c r="C26">
         <v>625.19871401786804</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>88.754236698150606</v>
+      </c>
+      <c r="F26">
+        <v>0.27335121566751502</v>
+      </c>
+      <c r="G26">
+        <v>597.51077818870499</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.334476947784395</v>
       </c>
@@ -7788,8 +8016,17 @@
       <c r="C27">
         <v>621.87540721893299</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>87.777173519134493</v>
+      </c>
+      <c r="F27">
+        <v>0.29522743620245001</v>
+      </c>
+      <c r="G27">
+        <v>598.20227146148602</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.361351728439303</v>
       </c>
@@ -7799,8 +8036,17 @@
       <c r="C28">
         <v>624.073350429534</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>88.144755363464299</v>
+      </c>
+      <c r="F28">
+        <v>0.28394295179797502</v>
+      </c>
+      <c r="G28">
+        <v>597.24572086334194</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.306801557540894</v>
       </c>
@@ -7810,8 +8056,17 @@
       <c r="C29">
         <v>625.62148094177201</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>88.251477479934593</v>
+      </c>
+      <c r="F29">
+        <v>0.27660272217203602</v>
+      </c>
+      <c r="G29">
+        <v>595.452190160751</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>88.315504789352403</v>
       </c>
@@ -7821,8 +8076,17 @@
       <c r="C30">
         <v>622.66134953498795</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>89.157396554946899</v>
+      </c>
+      <c r="F30">
+        <v>0.28012373466246498</v>
+      </c>
+      <c r="G30">
+        <v>596.81295394897404</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>87.895745038986206</v>
       </c>
@@ -7832,8 +8096,17 @@
       <c r="C31">
         <v>622.57876133918705</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>87.907606363296495</v>
+      </c>
+      <c r="F31">
+        <v>0.261589169804755</v>
+      </c>
+      <c r="G31">
+        <v>592.13518071174599</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.747125864028902</v>
       </c>
@@ -7843,8 +8116,17 @@
       <c r="C32">
         <v>622.42392969131402</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>88.021439313888493</v>
+      </c>
+      <c r="F32">
+        <v>0.28523247776489002</v>
+      </c>
+      <c r="G32">
+        <v>598.74224305152802</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>89.370834827423096</v>
       </c>
@@ -7854,8 +8136,17 @@
       <c r="C33">
         <v>622.95025801658596</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>89.079135656356797</v>
+      </c>
+      <c r="F33">
+        <v>0.26079855601980401</v>
+      </c>
+      <c r="G33">
+        <v>597.650529146194</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -7865,8 +8156,17 @@
       <c r="C34">
         <v>621.00262737274102</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>89.911544322967501</v>
+      </c>
+      <c r="F34">
+        <v>0.25300722584263702</v>
+      </c>
+      <c r="G34">
+        <v>598.34940481185902</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.389027118682804</v>
       </c>
@@ -7876,8 +8176,17 @@
       <c r="C35">
         <v>619.62267351150501</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>88.917875289916907</v>
+      </c>
+      <c r="F35">
+        <v>0.259902310250682</v>
+      </c>
+      <c r="G35">
+        <v>596.34551358222905</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.268077373504596</v>
       </c>
@@ -7887,8 +8196,17 @@
       <c r="C36">
         <v>622.44991159438996</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>89.007991552352905</v>
+      </c>
+      <c r="F36">
+        <v>0.27669326043972498</v>
+      </c>
+      <c r="G36">
+        <v>597.82621169090203</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.8846755027771</v>
       </c>
@@ -7898,8 +8216,17 @@
       <c r="C37">
         <v>625.08124709129299</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>89.404034614562903</v>
+      </c>
+      <c r="F37">
+        <v>0.25748578514735398</v>
+      </c>
+      <c r="G37">
+        <v>597.85539650916996</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>87.741601467132497</v>
       </c>
@@ -7909,8 +8236,17 @@
       <c r="C38">
         <v>623.22033381462097</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>89.022219181060706</v>
+      </c>
+      <c r="F38">
+        <v>0.24398595633627301</v>
+      </c>
+      <c r="G38">
+        <v>596.35876345634404</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.309173822402897</v>
       </c>
@@ -7920,8 +8256,17 @@
       <c r="C39">
         <v>619.80937767028797</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>87.784284353256197</v>
+      </c>
+      <c r="F39">
+        <v>0.29019046121226699</v>
+      </c>
+      <c r="G39">
+        <v>595.74957299232403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.722629308700505</v>
       </c>
@@ -7931,8 +8276,17 @@
       <c r="C40">
         <v>624.04310846328701</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>89.053052663803101</v>
+      </c>
+      <c r="F40">
+        <v>0.26330253773477702</v>
+      </c>
+      <c r="G40">
+        <v>598.54657983779896</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.891786336898804</v>
       </c>
@@ -7942,8 +8296,17 @@
       <c r="C41">
         <v>622.62831640243496</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>88.749498128890906</v>
+      </c>
+      <c r="F41">
+        <v>0.25400611398098</v>
+      </c>
+      <c r="G41">
+        <v>599.62389469146694</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>88.922619819641099</v>
       </c>
@@ -7953,8 +8316,17 @@
       <c r="C42">
         <v>623.05654406547501</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>89.316290616989093</v>
+      </c>
+      <c r="F42">
+        <v>0.24883833904820499</v>
+      </c>
+      <c r="G42">
+        <v>600.51636362075806</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>88.509970903396606</v>
       </c>
@@ -7964,8 +8336,17 @@
       <c r="C43">
         <v>622.40083050727799</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>88.279932737350407</v>
+      </c>
+      <c r="F43">
+        <v>0.286496894217867</v>
+      </c>
+      <c r="G43">
+        <v>595.27686357498101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.057791233062702</v>
       </c>
@@ -7975,8 +8356,17 @@
       <c r="C44">
         <v>621.44749498367298</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>88.972419500350895</v>
+      </c>
+      <c r="F44">
+        <v>0.27657860226737102</v>
+      </c>
+      <c r="G44">
+        <v>596.48798751830998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -7986,8 +8376,17 @@
       <c r="C45">
         <v>620.072613477706</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>88.009577989578204</v>
+      </c>
+      <c r="F45">
+        <v>0.275368125577443</v>
+      </c>
+      <c r="G45">
+        <v>599.66729974746704</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>89.072024822235093</v>
       </c>
@@ -7997,8 +8396,17 @@
       <c r="C46">
         <v>624.22593569755497</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>89.076763391494694</v>
+      </c>
+      <c r="F46">
+        <v>0.256679909101515</v>
+      </c>
+      <c r="G46">
+        <v>598.844078540802</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>88.782697916030799</v>
       </c>
@@ -8008,8 +8416,17 @@
       <c r="C47">
         <v>621.95561194419804</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>89.057791233062702</v>
+      </c>
+      <c r="F47">
+        <v>0.25425598798473997</v>
+      </c>
+      <c r="G47">
+        <v>597.57954907417297</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>88.906013965606604</v>
       </c>
@@ -8019,8 +8436,17 @@
       <c r="C48">
         <v>620.71887111663796</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>88.313138484954806</v>
+      </c>
+      <c r="F48">
+        <v>0.28561226159894598</v>
+      </c>
+      <c r="G48">
+        <v>600.35681700706402</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.336849212646399</v>
       </c>
@@ -8030,8 +8456,17 @@
       <c r="C49">
         <v>621.87014770507801</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>88.052266836166297</v>
+      </c>
+      <c r="F49">
+        <v>0.26715121061036701</v>
+      </c>
+      <c r="G49">
+        <v>599.00766682624806</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>88.206416368484497</v>
       </c>
@@ -8041,8 +8476,17 @@
       <c r="C50">
         <v>619.91724228858902</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>89.088624715804997</v>
+      </c>
+      <c r="F50">
+        <v>0.26098381193810899</v>
+      </c>
+      <c r="G50">
+        <v>597.94709277153004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>88.097327947616506</v>
       </c>
@@ -8051,6 +8495,15 @@
       </c>
       <c r="C51">
         <v>624.51877474784806</v>
+      </c>
+      <c r="E51">
+        <v>89.169257879257202</v>
+      </c>
+      <c r="F51">
+        <v>0.25830146733526599</v>
+      </c>
+      <c r="G51">
+        <v>598.093134641647</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 270 packet run MW 1D
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECA53E2F-C786-4175-8FE1-4F5971AEC8AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA865735-4964-475F-A9D0-43763CECDC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="12">
   <si>
     <t>Acc</t>
   </si>
@@ -7478,15 +7478,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A06EE43-A370-47E6-9A9B-D644A56FBF0A}">
-  <dimension ref="A1:K51"/>
+  <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+      <selection activeCell="S16" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -7496,8 +7496,11 @@
       <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7525,8 +7528,17 @@
       <c r="K2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.899682998657198</v>
       </c>
@@ -7545,8 +7557,17 @@
       <c r="G3">
         <v>603.068132162094</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3">
+        <v>88.526570796966496</v>
+      </c>
+      <c r="J3">
+        <v>0.27364717987528597</v>
+      </c>
+      <c r="K3">
+        <v>571.54140663146904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>89.669644832610999</v>
       </c>
@@ -7565,8 +7586,17 @@
       <c r="G4">
         <v>594.46053647994995</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I4">
+        <v>89.508384466171194</v>
+      </c>
+      <c r="J4">
+        <v>0.26449414726576298</v>
+      </c>
+      <c r="K4">
+        <v>563.20081591606095</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>87.739229202270494</v>
       </c>
@@ -7585,8 +7615,17 @@
       <c r="G5">
         <v>595.02324151992798</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I5">
+        <v>88.806414604186998</v>
+      </c>
+      <c r="J5">
+        <v>0.25839889372028602</v>
+      </c>
+      <c r="K5">
+        <v>570.53296017646699</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.928950786590505</v>
       </c>
@@ -7605,8 +7644,17 @@
       <c r="G6">
         <v>596.55497908592201</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I6">
+        <v>89.207202196121202</v>
+      </c>
+      <c r="J6">
+        <v>0.26261496832917403</v>
+      </c>
+      <c r="K6">
+        <v>567.04648327827397</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>87.656223773956299</v>
       </c>
@@ -7625,8 +7673,17 @@
       <c r="G7">
         <v>598.80659556388798</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I7">
+        <v>89.029335975646902</v>
+      </c>
+      <c r="J7">
+        <v>0.248651185612245</v>
+      </c>
+      <c r="K7">
+        <v>567.60861730575505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>89.000874757766695</v>
       </c>
@@ -7645,8 +7702,17 @@
       <c r="G8">
         <v>597.05055975914001</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>88.704437017440796</v>
+      </c>
+      <c r="J8">
+        <v>0.26690111964305602</v>
+      </c>
+      <c r="K8">
+        <v>567.39737844467095</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.169257879257202</v>
       </c>
@@ -7665,8 +7731,17 @@
       <c r="G9">
         <v>597.54162454605103</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I9">
+        <v>88.981902599334703</v>
+      </c>
+      <c r="J9">
+        <v>0.24983153020603099</v>
+      </c>
+      <c r="K9">
+        <v>569.47559022903397</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.216685295104895</v>
       </c>
@@ -7685,8 +7760,17 @@
       <c r="G10">
         <v>594.49819874763398</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I10">
+        <v>89.453840255737305</v>
+      </c>
+      <c r="J10">
+        <v>0.25886353362694098</v>
+      </c>
+      <c r="K10">
+        <v>567.98920059204102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.356607198715196</v>
       </c>
@@ -7705,8 +7789,17 @@
       <c r="G11">
         <v>626.51882672309796</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I11">
+        <v>89.5131289958953</v>
+      </c>
+      <c r="J11">
+        <v>0.27139978508277002</v>
+      </c>
+      <c r="K11">
+        <v>566.18249654769897</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>88.744753599166799</v>
       </c>
@@ -7725,8 +7818,17 @@
       <c r="G12">
         <v>622.97183203697205</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I12">
+        <v>89.226174354553194</v>
+      </c>
+      <c r="J12">
+        <v>0.25948665560720902</v>
+      </c>
+      <c r="K12">
+        <v>568.16771006584099</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>88.946330547332707</v>
       </c>
@@ -7745,8 +7847,17 @@
       <c r="G13">
         <v>626.605017662048</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>88.661748170852604</v>
+      </c>
+      <c r="J13">
+        <v>0.26117336892303</v>
+      </c>
+      <c r="K13">
+        <v>566.52932882308903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>88.317877054214406</v>
       </c>
@@ -7765,8 +7876,17 @@
       <c r="G14">
         <v>621.65510725975003</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>88.910758495330796</v>
+      </c>
+      <c r="J14">
+        <v>0.26289581964776798</v>
+      </c>
+      <c r="K14">
+        <v>567.09138488769497</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.446723461151095</v>
       </c>
@@ -7785,8 +7905,17 @@
       <c r="G15">
         <v>625.92930412292401</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I15">
+        <v>88.161361217498694</v>
+      </c>
+      <c r="J15">
+        <v>0.28794452782073499</v>
+      </c>
+      <c r="K15">
+        <v>568.954289674758</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.227760791778493</v>
       </c>
@@ -7805,8 +7934,17 @@
       <c r="G16">
         <v>624.45639634132306</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16">
+        <v>89.024591445922795</v>
+      </c>
+      <c r="J16">
+        <v>0.27293423157291502</v>
+      </c>
+      <c r="K16">
+        <v>564.79920411109902</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.000874757766695</v>
       </c>
@@ -7825,8 +7963,17 @@
       <c r="G17">
         <v>624.07658600807099</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17">
+        <v>89.811939001083303</v>
+      </c>
+      <c r="J17">
+        <v>0.25717963969796198</v>
+      </c>
+      <c r="K17">
+        <v>570.29118657112099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.211940765380803</v>
       </c>
@@ -7845,8 +7992,17 @@
       <c r="G18">
         <v>597.86826133728005</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18">
+        <v>88.801670074462805</v>
+      </c>
+      <c r="J18">
+        <v>0.28394434498728299</v>
+      </c>
+      <c r="K18">
+        <v>564.91241025924603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>88.251477479934593</v>
       </c>
@@ -7865,8 +8021,17 @@
       <c r="G19">
         <v>600.72510051727295</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19">
+        <v>88.294166326522799</v>
+      </c>
+      <c r="J19">
+        <v>0.28930436779771002</v>
+      </c>
+      <c r="K19">
+        <v>565.87722325325001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>88.075983524322496</v>
       </c>
@@ -7885,8 +8050,17 @@
       <c r="G20">
         <v>594.50169444084099</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20">
+        <v>89.088624715804997</v>
+      </c>
+      <c r="J20">
+        <v>0.26881124585344601</v>
+      </c>
+      <c r="K20">
+        <v>568.35680985450699</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>88.993763923645005</v>
       </c>
@@ -7905,8 +8079,17 @@
       <c r="G21">
         <v>597.10161566734303</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21">
+        <v>88.391393423080402</v>
+      </c>
+      <c r="J21">
+        <v>0.291519165259574</v>
+      </c>
+      <c r="K21">
+        <v>569.515851259231</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>87.331324815750094</v>
       </c>
@@ -7925,8 +8108,17 @@
       <c r="G22">
         <v>599.09105467796303</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22">
+        <v>87.938433885574298</v>
+      </c>
+      <c r="J22">
+        <v>0.28873213954559801</v>
+      </c>
+      <c r="K22">
+        <v>569.02983236312798</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>87.447530031204195</v>
       </c>
@@ -7945,8 +8137,17 @@
       <c r="G23">
         <v>598.84158515930096</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23">
+        <v>88.763725757598806</v>
+      </c>
+      <c r="J23">
+        <v>0.26834346629382499</v>
+      </c>
+      <c r="K23">
+        <v>566.78986501693703</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.287049531936603</v>
       </c>
@@ -7965,8 +8166,17 @@
       <c r="G24">
         <v>595.70589900016705</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24">
+        <v>88.009577989578204</v>
+      </c>
+      <c r="J24">
+        <v>0.274134513162546</v>
+      </c>
+      <c r="K24">
+        <v>568.81757926940895</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>89.098107814788804</v>
       </c>
@@ -7985,8 +8195,17 @@
       <c r="G25">
         <v>597.52832674980095</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25">
+        <v>89.155024290084796</v>
+      </c>
+      <c r="J25">
+        <v>0.259638950536135</v>
+      </c>
+      <c r="K25">
+        <v>568.20859313011101</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>88.135272264480506</v>
       </c>
@@ -8005,8 +8224,17 @@
       <c r="G26">
         <v>597.51077818870499</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26">
+        <v>88.894158601760793</v>
+      </c>
+      <c r="J26">
+        <v>0.265488644609297</v>
+      </c>
+      <c r="K26">
+        <v>569.044016361236</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.334476947784395</v>
       </c>
@@ -8025,8 +8253,17 @@
       <c r="G27">
         <v>598.20227146148602</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27">
+        <v>89.444351196289006</v>
+      </c>
+      <c r="J27">
+        <v>0.24944659968504601</v>
+      </c>
+      <c r="K27">
+        <v>567.303020238876</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.361351728439303</v>
       </c>
@@ -8045,8 +8282,17 @@
       <c r="G28">
         <v>597.24572086334194</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28">
+        <v>88.704437017440796</v>
+      </c>
+      <c r="J28">
+        <v>0.26888305771927401</v>
+      </c>
+      <c r="K28">
+        <v>564.03714585304203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.306801557540894</v>
       </c>
@@ -8065,8 +8311,17 @@
       <c r="G29">
         <v>595.452190160751</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29">
+        <v>87.675195932388306</v>
+      </c>
+      <c r="J29">
+        <v>0.27972395518576798</v>
+      </c>
+      <c r="K29">
+        <v>570.32110118865899</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>88.315504789352403</v>
       </c>
@@ -8085,8 +8340,17 @@
       <c r="G30">
         <v>596.81295394897404</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>90.011143684387207</v>
+      </c>
+      <c r="J30">
+        <v>0.23787439667117899</v>
+      </c>
+      <c r="K30">
+        <v>565.27814984321503</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>87.895745038986206</v>
       </c>
@@ -8105,8 +8369,17 @@
       <c r="G31">
         <v>592.13518071174599</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>88.730525970458899</v>
+      </c>
+      <c r="J31">
+        <v>0.27651749239611101</v>
+      </c>
+      <c r="K31">
+        <v>569.52728033065796</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.747125864028902</v>
       </c>
@@ -8125,8 +8398,17 @@
       <c r="G32">
         <v>598.74224305152802</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="J32">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="K32">
+        <v>567.20298838615395</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>89.370834827423096</v>
       </c>
@@ -8145,8 +8427,17 @@
       <c r="G33">
         <v>597.650529146194</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33">
+        <v>88.590604066848698</v>
+      </c>
+      <c r="J33">
+        <v>0.25385649970335</v>
+      </c>
+      <c r="K33">
+        <v>568.78105330467201</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -8165,8 +8456,17 @@
       <c r="G34">
         <v>598.34940481185902</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34">
+        <v>89.109969139099107</v>
+      </c>
+      <c r="J34">
+        <v>0.26093641278191998</v>
+      </c>
+      <c r="K34">
+        <v>564.85970544814995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.389027118682804</v>
       </c>
@@ -8185,8 +8485,17 @@
       <c r="G35">
         <v>596.34551358222905</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35">
+        <v>88.502860069274902</v>
+      </c>
+      <c r="J35">
+        <v>0.279851582453916</v>
+      </c>
+      <c r="K35">
+        <v>565.68032455444302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.268077373504596</v>
       </c>
@@ -8205,8 +8514,17 @@
       <c r="G36">
         <v>597.82621169090203</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>87.888634204864502</v>
+      </c>
+      <c r="J36">
+        <v>0.276040247304353</v>
+      </c>
+      <c r="K36">
+        <v>564.46240520477295</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.8846755027771</v>
       </c>
@@ -8225,8 +8543,17 @@
       <c r="G37">
         <v>597.85539650916996</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37">
+        <v>88.939219713211003</v>
+      </c>
+      <c r="J37">
+        <v>0.26452549647477203</v>
+      </c>
+      <c r="K37">
+        <v>566.59601569175697</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>87.741601467132497</v>
       </c>
@@ -8245,8 +8572,17 @@
       <c r="G38">
         <v>596.35876345634404</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38">
+        <v>89.9874329566955</v>
+      </c>
+      <c r="J38">
+        <v>0.25380408502098301</v>
+      </c>
+      <c r="K38">
+        <v>568.67201066017105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.309173822402897</v>
       </c>
@@ -8265,8 +8601,17 @@
       <c r="G39">
         <v>595.74957299232403</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39">
+        <v>89.280718564987097</v>
+      </c>
+      <c r="J39">
+        <v>0.25534665625980801</v>
+      </c>
+      <c r="K39">
+        <v>568.89972043037403</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.722629308700505</v>
       </c>
@@ -8285,8 +8630,17 @@
       <c r="G40">
         <v>598.54657983779896</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40">
+        <v>87.962150573730398</v>
+      </c>
+      <c r="J40">
+        <v>0.28369151539454701</v>
+      </c>
+      <c r="K40">
+        <v>566.00424218177795</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.891786336898804</v>
       </c>
@@ -8305,8 +8659,17 @@
       <c r="G41">
         <v>599.62389469146694</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>89.088624715804997</v>
+      </c>
+      <c r="J41">
+        <v>0.25009892779530601</v>
+      </c>
+      <c r="K41">
+        <v>568.02661538124005</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>88.922619819641099</v>
       </c>
@@ -8325,8 +8688,17 @@
       <c r="G42">
         <v>600.51636362075806</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <v>89.079135656356797</v>
+      </c>
+      <c r="J42">
+        <v>0.26349528033048503</v>
+      </c>
+      <c r="K42">
+        <v>565.79061031341496</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>88.509970903396606</v>
       </c>
@@ -8345,8 +8717,17 @@
       <c r="G43">
         <v>595.27686357498101</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <v>88.080728054046602</v>
+      </c>
+      <c r="J43">
+        <v>0.28729819680042201</v>
+      </c>
+      <c r="K43">
+        <v>570.74440741539001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.057791233062702</v>
       </c>
@@ -8365,8 +8746,17 @@
       <c r="G44">
         <v>596.48798751830998</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <v>88.474398851394596</v>
+      </c>
+      <c r="J44">
+        <v>0.27594648872458599</v>
+      </c>
+      <c r="K44">
+        <v>566.73435997962895</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -8385,8 +8775,17 @@
       <c r="G45">
         <v>599.66729974746704</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45">
+        <v>89.107596874237004</v>
+      </c>
+      <c r="J45">
+        <v>0.25494215230629202</v>
+      </c>
+      <c r="K45">
+        <v>567.932703971862</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>89.072024822235093</v>
       </c>
@@ -8405,8 +8804,17 @@
       <c r="G46">
         <v>598.844078540802</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <v>89.164513349532996</v>
+      </c>
+      <c r="J46">
+        <v>0.26137452160043101</v>
+      </c>
+      <c r="K46">
+        <v>570.83284282684303</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>88.782697916030799</v>
       </c>
@@ -8425,8 +8833,17 @@
       <c r="G47">
         <v>597.57954907417297</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47">
+        <v>89.254629611968994</v>
+      </c>
+      <c r="J47">
+        <v>0.25538730008993299</v>
+      </c>
+      <c r="K47">
+        <v>565.16936302185002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>88.906013965606604</v>
       </c>
@@ -8445,8 +8862,17 @@
       <c r="G48">
         <v>600.35681700706402</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48">
+        <v>88.991391658782902</v>
+      </c>
+      <c r="J48">
+        <v>0.29412961411902799</v>
+      </c>
+      <c r="K48">
+        <v>569.66812443733204</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.336849212646399</v>
       </c>
@@ -8465,8 +8891,17 @@
       <c r="G49">
         <v>599.00766682624806</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49">
+        <v>89.041191339492798</v>
+      </c>
+      <c r="J49">
+        <v>0.26776675705595399</v>
+      </c>
+      <c r="K49">
+        <v>567.20592927932705</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>88.206416368484497</v>
       </c>
@@ -8485,8 +8920,17 @@
       <c r="G50">
         <v>597.94709277153004</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50">
+        <v>89.155024290084796</v>
+      </c>
+      <c r="J50">
+        <v>0.249937309914257</v>
+      </c>
+      <c r="K50">
+        <v>567.783757925033</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>88.097327947616506</v>
       </c>
@@ -8504,6 +8948,15 @@
       </c>
       <c r="G51">
         <v>598.093134641647</v>
+      </c>
+      <c r="I51">
+        <v>88.611948490142794</v>
+      </c>
+      <c r="J51">
+        <v>0.28223201247204599</v>
+      </c>
+      <c r="K51">
+        <v>570.62241840362503</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 250 packet run MW 1D
</commit_message>
<xml_diff>
--- a/50TrialsVaryPackets.csv.xlsx
+++ b/50TrialsVaryPackets.csv.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\AP-Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA865735-4964-475F-A9D0-43763CECDC5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE71D59C-8C66-40EA-AE64-D27E4A4964B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="12">
   <si>
     <t>Acc</t>
   </si>
@@ -7478,15 +7478,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A06EE43-A370-47E6-9A9B-D644A56FBF0A}">
-  <dimension ref="A1:O51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="T12" sqref="T12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
@@ -7499,8 +7499,11 @@
       <c r="N1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -7537,8 +7540,17 @@
       <c r="O2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="Q2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>89.899682998657198</v>
       </c>
@@ -7566,8 +7578,17 @@
       <c r="K3">
         <v>571.54140663146904</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>88.483887910842896</v>
+      </c>
+      <c r="N3">
+        <v>0.281325041714515</v>
+      </c>
+      <c r="O3">
+        <v>551.36055135726895</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>89.669644832610999</v>
       </c>
@@ -7595,8 +7616,17 @@
       <c r="K4">
         <v>563.20081591606095</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>88.996136188506995</v>
+      </c>
+      <c r="N4">
+        <v>0.252420932368148</v>
+      </c>
+      <c r="O4">
+        <v>544.04951500892605</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>87.739229202270494</v>
       </c>
@@ -7624,8 +7654,17 @@
       <c r="K5">
         <v>570.53296017646699</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>88.417482376098604</v>
+      </c>
+      <c r="N5">
+        <v>0.306426730454052</v>
+      </c>
+      <c r="O5">
+        <v>542.28713583946205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>87.928950786590505</v>
       </c>
@@ -7653,8 +7692,17 @@
       <c r="K6">
         <v>567.04648327827397</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>89.041191339492798</v>
+      </c>
+      <c r="N6">
+        <v>0.26398389835938002</v>
+      </c>
+      <c r="O6">
+        <v>546.41168141364994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>87.656223773956299</v>
       </c>
@@ -7682,8 +7730,17 @@
       <c r="K7">
         <v>567.60861730575505</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>88.889414072036701</v>
+      </c>
+      <c r="N7">
+        <v>0.28471131582523101</v>
+      </c>
+      <c r="O7">
+        <v>541.61022663116398</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>89.000874757766695</v>
       </c>
@@ -7711,8 +7768,17 @@
       <c r="K8">
         <v>567.39737844467095</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>88.851469755172701</v>
+      </c>
+      <c r="N8">
+        <v>0.27909826622030498</v>
+      </c>
+      <c r="O8">
+        <v>542.92116403579701</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>89.169257879257202</v>
       </c>
@@ -7740,8 +7806,17 @@
       <c r="K9">
         <v>569.47559022903397</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>88.986647129058795</v>
+      </c>
+      <c r="N9">
+        <v>0.26166537757056002</v>
+      </c>
+      <c r="O9">
+        <v>545.85422968864395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>89.216685295104895</v>
       </c>
@@ -7769,8 +7844,17 @@
       <c r="K10">
         <v>567.98920059204102</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>88.355821371078406</v>
+      </c>
+      <c r="N10">
+        <v>0.284870725911266</v>
+      </c>
+      <c r="O10">
+        <v>547.05730724334705</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>89.356607198715196</v>
       </c>
@@ -7798,8 +7882,17 @@
       <c r="K11">
         <v>566.18249654769897</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>88.597720861434894</v>
+      </c>
+      <c r="N11">
+        <v>0.28846056012302701</v>
+      </c>
+      <c r="O11">
+        <v>544.99331116676296</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>88.744753599166799</v>
       </c>
@@ -7827,8 +7920,17 @@
       <c r="K12">
         <v>568.16771006584099</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>88.6830925941467</v>
+      </c>
+      <c r="N12">
+        <v>0.26560601756776298</v>
+      </c>
+      <c r="O12">
+        <v>546.16639089584305</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>88.946330547332707</v>
       </c>
@@ -7856,8 +7958,17 @@
       <c r="K13">
         <v>566.52932882308903</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>87.36452460289</v>
+      </c>
+      <c r="N13">
+        <v>0.359610378499442</v>
+      </c>
+      <c r="O13">
+        <v>546.45408487319901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>88.317877054214406</v>
       </c>
@@ -7885,8 +7996,17 @@
       <c r="K14">
         <v>567.09138488769497</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14">
+        <v>88.901275396347003</v>
+      </c>
+      <c r="N14">
+        <v>0.26030729608185499</v>
+      </c>
+      <c r="O14">
+        <v>546.16273212432804</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>89.446723461151095</v>
       </c>
@@ -7914,8 +8034,17 @@
       <c r="K15">
         <v>568.954289674758</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15">
+        <v>88.614320755004798</v>
+      </c>
+      <c r="N15">
+        <v>0.28436701727602598</v>
+      </c>
+      <c r="O15">
+        <v>546.87314581870999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>88.227760791778493</v>
       </c>
@@ -7943,8 +8072,17 @@
       <c r="K16">
         <v>564.79920411109902</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>89.036452770233097</v>
+      </c>
+      <c r="N16">
+        <v>0.27837585723352398</v>
+      </c>
+      <c r="O16">
+        <v>547.32949757575898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>89.000874757766695</v>
       </c>
@@ -7972,8 +8110,17 @@
       <c r="K17">
         <v>570.29118657112099</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>88.939219713211003</v>
+      </c>
+      <c r="N17">
+        <v>0.26104552296434202</v>
+      </c>
+      <c r="O17">
+        <v>545.30119872093201</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>89.211940765380803</v>
       </c>
@@ -8001,8 +8148,17 @@
       <c r="K18">
         <v>564.91241025924603</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>88.711553812026906</v>
+      </c>
+      <c r="N18">
+        <v>0.26672030669906699</v>
+      </c>
+      <c r="O18">
+        <v>545.76163697242703</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>88.251477479934593</v>
       </c>
@@ -8030,8 +8186,17 @@
       <c r="K19">
         <v>565.87722325325001</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>88.640403747558594</v>
+      </c>
+      <c r="N19">
+        <v>0.25990669919340398</v>
+      </c>
+      <c r="O19">
+        <v>545.28115653991699</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>88.075983524322496</v>
       </c>
@@ -8059,8 +8224,17 @@
       <c r="K20">
         <v>568.35680985450699</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>89.010363817214895</v>
+      </c>
+      <c r="N20">
+        <v>0.27289671628287598</v>
+      </c>
+      <c r="O20">
+        <v>545.80812358856201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>88.993763923645005</v>
       </c>
@@ -8088,8 +8262,17 @@
       <c r="K21">
         <v>569.515851259231</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>88.585859537124605</v>
+      </c>
+      <c r="N21">
+        <v>0.29010992726569801</v>
+      </c>
+      <c r="O21">
+        <v>547.65209531784001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>87.331324815750094</v>
       </c>
@@ -8117,8 +8300,17 @@
       <c r="K22">
         <v>569.02983236312798</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>88.204044103622394</v>
+      </c>
+      <c r="N22">
+        <v>0.30982169429669798</v>
+      </c>
+      <c r="O22">
+        <v>545.26629543304398</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>87.447530031204195</v>
       </c>
@@ -8146,8 +8338,17 @@
       <c r="K23">
         <v>566.78986501693703</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>87.639623880386296</v>
+      </c>
+      <c r="N23">
+        <v>0.264758731574678</v>
+      </c>
+      <c r="O23">
+        <v>544.52358675002995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>88.287049531936603</v>
       </c>
@@ -8175,8 +8376,17 @@
       <c r="K24">
         <v>568.81757926940895</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>90.044349431991506</v>
+      </c>
+      <c r="N24">
+        <v>0.24955440453571301</v>
+      </c>
+      <c r="O24">
+        <v>546.63705778121903</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>89.098107814788804</v>
       </c>
@@ -8204,8 +8414,17 @@
       <c r="K25">
         <v>568.20859313011101</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>89.543956518173204</v>
+      </c>
+      <c r="N25">
+        <v>0.25332823623609002</v>
+      </c>
+      <c r="O25">
+        <v>546.20874142646699</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>88.135272264480506</v>
       </c>
@@ -8233,8 +8452,17 @@
       <c r="K26">
         <v>569.044016361236</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>88.834869861602698</v>
+      </c>
+      <c r="N26">
+        <v>0.26073585859903697</v>
+      </c>
+      <c r="O26">
+        <v>547.71153569221497</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>88.334476947784395</v>
       </c>
@@ -8262,8 +8490,17 @@
       <c r="K27">
         <v>567.303020238876</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N27">
+        <v>2.6234215325207999</v>
+      </c>
+      <c r="O27">
+        <v>545.36057758331299</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>89.361351728439303</v>
       </c>
@@ -8291,8 +8528,17 @@
       <c r="K28">
         <v>564.03714585304203</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>82.941639423370304</v>
+      </c>
+      <c r="N28">
+        <v>2.62342143300845</v>
+      </c>
+      <c r="O28">
+        <v>543.04964137077297</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>89.306801557540894</v>
       </c>
@@ -8320,8 +8566,17 @@
       <c r="K29">
         <v>570.32110118865899</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>88.777953386306706</v>
+      </c>
+      <c r="N29">
+        <v>0.27444691853879799</v>
+      </c>
+      <c r="O29">
+        <v>544.50223922729401</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>88.315504789352403</v>
       </c>
@@ -8349,8 +8604,17 @@
       <c r="K30">
         <v>565.27814984321503</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>88.808786869049001</v>
+      </c>
+      <c r="N30">
+        <v>0.28404082121221902</v>
+      </c>
+      <c r="O30">
+        <v>547.74136209487904</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>87.895745038986206</v>
       </c>
@@ -8378,8 +8642,17 @@
       <c r="K31">
         <v>569.52728033065796</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M31">
+        <v>88.626176118850694</v>
+      </c>
+      <c r="N31">
+        <v>0.26247188221237999</v>
+      </c>
+      <c r="O31">
+        <v>543.99815678596497</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>88.747125864028902</v>
       </c>
@@ -8407,8 +8680,17 @@
       <c r="K32">
         <v>567.20298838615395</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>89.100480079650794</v>
+      </c>
+      <c r="N32">
+        <v>0.259553523475755</v>
+      </c>
+      <c r="O32">
+        <v>547.98098540306</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>89.370834827423096</v>
       </c>
@@ -8436,8 +8718,17 @@
       <c r="K33">
         <v>568.78105330467201</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M33">
+        <v>88.846731185913001</v>
+      </c>
+      <c r="N33">
+        <v>0.26531235577315598</v>
+      </c>
+      <c r="O33">
+        <v>544.29760575294495</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>88.737636804580603</v>
       </c>
@@ -8465,8 +8756,17 @@
       <c r="K34">
         <v>564.85970544814995</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M34">
+        <v>88.633292913436804</v>
+      </c>
+      <c r="N34">
+        <v>0.27672774358729701</v>
+      </c>
+      <c r="O34">
+        <v>544.23738980293194</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>88.389027118682804</v>
       </c>
@@ -8494,8 +8794,17 @@
       <c r="K35">
         <v>565.68032455444302</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M35">
+        <v>89.067280292510901</v>
+      </c>
+      <c r="N35">
+        <v>0.248404741251362</v>
+      </c>
+      <c r="O35">
+        <v>543.86246681213299</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>88.268077373504596</v>
       </c>
@@ -8523,8 +8832,17 @@
       <c r="K36">
         <v>564.46240520477295</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M36">
+        <v>89.031708240509005</v>
+      </c>
+      <c r="N36">
+        <v>0.26492855713896202</v>
+      </c>
+      <c r="O36">
+        <v>544.77868914604096</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>88.8846755027771</v>
       </c>
@@ -8552,8 +8870,17 @@
       <c r="K37">
         <v>566.59601569175697</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M37">
+        <v>88.830125331878605</v>
+      </c>
+      <c r="N37">
+        <v>0.25159506870326198</v>
+      </c>
+      <c r="O37">
+        <v>547.13121771812405</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>87.741601467132497</v>
       </c>
@@ -8581,8 +8908,17 @@
       <c r="K38">
         <v>568.67201066017105</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>87.608796358108506</v>
+      </c>
+      <c r="N38">
+        <v>0.29609051382293999</v>
+      </c>
+      <c r="O38">
+        <v>547.16282296180702</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>89.309173822402897</v>
       </c>
@@ -8610,8 +8946,17 @@
       <c r="K39">
         <v>568.89972043037403</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M39">
+        <v>87.947922945022498</v>
+      </c>
+      <c r="N39">
+        <v>0.28873343550453801</v>
+      </c>
+      <c r="O39">
+        <v>549.94790124893098</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>87.722629308700505</v>
       </c>
@@ -8639,8 +8984,17 @@
       <c r="K40">
         <v>566.00424218177795</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>88.426971435546804</v>
+      </c>
+      <c r="N40">
+        <v>0.27449781699912401</v>
+      </c>
+      <c r="O40">
+        <v>545.10195541381802</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>88.891786336898804</v>
       </c>
@@ -8668,8 +9022,17 @@
       <c r="K41">
         <v>568.02661538124005</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M41">
+        <v>89.043563604354802</v>
+      </c>
+      <c r="N41">
+        <v>0.268049381352639</v>
+      </c>
+      <c r="O41">
+        <v>547.15556144714299</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>88.922619819641099</v>
       </c>
@@ -8697,8 +9060,17 @@
       <c r="K42">
         <v>565.79061031341496</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M42">
+        <v>88.846731185913001</v>
+      </c>
+      <c r="N42">
+        <v>0.25549514489000302</v>
+      </c>
+      <c r="O42">
+        <v>552.29076719284001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>88.509970903396606</v>
       </c>
@@ -8726,8 +9098,17 @@
       <c r="K43">
         <v>570.74440741539001</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M43">
+        <v>88.962930440902696</v>
+      </c>
+      <c r="N43">
+        <v>0.26159132634100402</v>
+      </c>
+      <c r="O43">
+        <v>547.493482589721</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>89.057791233062702</v>
       </c>
@@ -8755,8 +9136,17 @@
       <c r="K44">
         <v>566.73435997962895</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>88.661748170852604</v>
+      </c>
+      <c r="N44">
+        <v>0.28134602580025903</v>
+      </c>
+      <c r="O44">
+        <v>546.67198348045304</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>82.941639423370304</v>
       </c>
@@ -8784,8 +9174,17 @@
       <c r="K45">
         <v>567.932703971862</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M45">
+        <v>88.936847448348999</v>
+      </c>
+      <c r="N45">
+        <v>0.24437450679058301</v>
+      </c>
+      <c r="O45">
+        <v>542.47305011749199</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>89.072024822235093</v>
       </c>
@@ -8813,8 +9212,17 @@
       <c r="K46">
         <v>570.83284282684303</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>89.088624715804997</v>
+      </c>
+      <c r="N46">
+        <v>0.25561373741417698</v>
+      </c>
+      <c r="O46">
+        <v>547.44016408920197</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>88.782697916030799</v>
       </c>
@@ -8842,8 +9250,17 @@
       <c r="K47">
         <v>565.16936302185002</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M47">
+        <v>89.000874757766695</v>
+      </c>
+      <c r="N47">
+        <v>0.26804574518342</v>
+      </c>
+      <c r="O47">
+        <v>544.81893038749695</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>88.906013965606604</v>
       </c>
@@ -8871,8 +9288,17 @@
       <c r="K48">
         <v>569.66812443733204</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M48">
+        <v>88.901275396347003</v>
+      </c>
+      <c r="N48">
+        <v>0.25049732122971802</v>
+      </c>
+      <c r="O48">
+        <v>546.60061383247296</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>88.336849212646399</v>
       </c>
@@ -8900,8 +9326,17 @@
       <c r="K49">
         <v>567.20592927932705</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>88.974791765212998</v>
+      </c>
+      <c r="N49">
+        <v>0.26366006618967502</v>
+      </c>
+      <c r="O49">
+        <v>546.98892784118596</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>88.206416368484497</v>
       </c>
@@ -8929,8 +9364,17 @@
       <c r="K50">
         <v>567.783757925033</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M50">
+        <v>88.657009601593003</v>
+      </c>
+      <c r="N50">
+        <v>0.27222664157325699</v>
+      </c>
+      <c r="O50">
+        <v>543.56502509117104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>88.097327947616506</v>
       </c>
@@ -8957,6 +9401,15 @@
       </c>
       <c r="K51">
         <v>570.62241840362503</v>
+      </c>
+      <c r="M51">
+        <v>89.638817310333195</v>
+      </c>
+      <c r="N51">
+        <v>0.25382578302136999</v>
+      </c>
+      <c r="O51">
+        <v>546.291284561157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>